<commit_message>
CIERRRE 27 NOV 2021
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 11  NOVIEMBRE 2021/BALANCE    ZAVALETA   NOVIEMBRE    2021.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 11  NOVIEMBRE 2021/BALANCE    ZAVALETA   NOVIEMBRE    2021.xlsx
@@ -146,7 +146,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="112">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -465,6 +465,24 @@
   <si>
     <t>PEREJIL-CEBOLLA-PIMIENTO-</t>
   </si>
+  <si>
+    <t>JAMON-LONGANIZA-LACTEOS</t>
+  </si>
+  <si>
+    <t>POLLO--MAIZ-PAN</t>
+  </si>
+  <si>
+    <t>POLLO--LONGANIZA</t>
+  </si>
+  <si>
+    <t>NOMINA # 46</t>
+  </si>
+  <si>
+    <t>POLLO--LACTEOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                      </t>
+  </si>
 </sst>
 </file>
 
@@ -478,7 +496,7 @@
     <numFmt numFmtId="167" formatCode="[$$-80A]#,##0.00;\-[$$-80A]#,##0.00"/>
     <numFmt numFmtId="168" formatCode="[$-C0A]d\-mmm\-yyyy;@"/>
   </numFmts>
-  <fonts count="48" x14ac:knownFonts="1">
+  <fonts count="49" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -859,8 +877,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -927,6 +952,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="61">
     <border>
@@ -1687,7 +1718,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="291">
+  <cellXfs count="290">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -2147,6 +2178,102 @@
     <xf numFmtId="44" fontId="2" fillId="0" borderId="56" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="60" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="47" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="39" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="44" fillId="0" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="47" fillId="0" borderId="50" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="6" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="6" borderId="51" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="6" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="50" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2180,84 +2307,18 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="6" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="6" borderId="51" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="6" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="50" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="43" fillId="6" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="43" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="43" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="43" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2267,40 +2328,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="39" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="43" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="44" fillId="0" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="43" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="20" fillId="12" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="41" fillId="0" borderId="50" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="50" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="46" fillId="0" borderId="50" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="50" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="47" fillId="0" borderId="50" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="2" fillId="12" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -3473,23 +3507,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="235"/>
-      <c r="C1" s="237" t="s">
+      <c r="B1" s="269"/>
+      <c r="C1" s="271" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="238"/>
-      <c r="E1" s="238"/>
-      <c r="F1" s="238"/>
-      <c r="G1" s="238"/>
-      <c r="H1" s="238"/>
-      <c r="I1" s="238"/>
-      <c r="J1" s="238"/>
-      <c r="K1" s="238"/>
-      <c r="L1" s="238"/>
-      <c r="M1" s="238"/>
+      <c r="D1" s="272"/>
+      <c r="E1" s="272"/>
+      <c r="F1" s="272"/>
+      <c r="G1" s="272"/>
+      <c r="H1" s="272"/>
+      <c r="I1" s="272"/>
+      <c r="J1" s="272"/>
+      <c r="K1" s="272"/>
+      <c r="L1" s="272"/>
+      <c r="M1" s="272"/>
     </row>
     <row r="2" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="236"/>
+      <c r="B2" s="270"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -3499,17 +3533,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:19" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="239" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="240"/>
+      <c r="B3" s="273" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="274"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="241" t="s">
+      <c r="H3" s="275" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="241"/>
+      <c r="I3" s="275"/>
       <c r="K3" s="178"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
@@ -3523,14 +3557,14 @@
         <v>0</v>
       </c>
       <c r="D4" s="18"/>
-      <c r="E4" s="242" t="s">
+      <c r="E4" s="276" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="243"/>
-      <c r="H4" s="244" t="s">
+      <c r="F4" s="277"/>
+      <c r="H4" s="278" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="245"/>
+      <c r="I4" s="279"/>
       <c r="J4" s="19"/>
       <c r="K4" s="179"/>
       <c r="L4" s="20"/>
@@ -3540,10 +3574,10 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="251" t="s">
+      <c r="P4" s="250" t="s">
         <v>6</v>
       </c>
-      <c r="Q4" s="252"/>
+      <c r="Q4" s="251"/>
     </row>
     <row r="5" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
@@ -4984,11 +5018,11 @@
       <c r="J39" s="60"/>
       <c r="K39" s="190"/>
       <c r="L39" s="61"/>
-      <c r="M39" s="253">
+      <c r="M39" s="252">
         <f>SUM(M5:M38)</f>
         <v>247061</v>
       </c>
-      <c r="N39" s="255">
+      <c r="N39" s="254">
         <f>SUM(N5:N38)</f>
         <v>172863</v>
       </c>
@@ -5014,8 +5048,8 @@
       <c r="J40" s="60"/>
       <c r="K40" s="41"/>
       <c r="L40" s="61"/>
-      <c r="M40" s="254"/>
-      <c r="N40" s="256"/>
+      <c r="M40" s="253"/>
+      <c r="N40" s="255"/>
       <c r="P40" s="34"/>
       <c r="Q40" s="9"/>
     </row>
@@ -5230,29 +5264,29 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="257" t="s">
+      <c r="H52" s="256" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="258"/>
+      <c r="I52" s="257"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="259">
+      <c r="K52" s="258">
         <f>I50+L50</f>
         <v>53873.49</v>
       </c>
-      <c r="L52" s="260"/>
-      <c r="M52" s="261">
+      <c r="L52" s="259"/>
+      <c r="M52" s="260">
         <f>N39+M39</f>
         <v>419924</v>
       </c>
-      <c r="N52" s="262"/>
+      <c r="N52" s="261"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D53" s="263" t="s">
+      <c r="D53" s="262" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="263"/>
+      <c r="E53" s="262"/>
       <c r="F53" s="101">
         <f>F50-K52-C50</f>
         <v>471038.61</v>
@@ -5263,22 +5297,22 @@
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="263" t="s">
+      <c r="D54" s="262" t="s">
         <v>101</v>
       </c>
-      <c r="E54" s="263"/>
+      <c r="E54" s="262"/>
       <c r="F54" s="96">
         <v>-549976.4</v>
       </c>
-      <c r="I54" s="264" t="s">
+      <c r="I54" s="263" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="265"/>
-      <c r="K54" s="266">
+      <c r="J54" s="264"/>
+      <c r="K54" s="265">
         <f>F56+F57+F58</f>
         <v>-24577.400000000023</v>
       </c>
-      <c r="L54" s="267"/>
+      <c r="L54" s="266"/>
       <c r="P54" s="34"/>
       <c r="Q54" s="9"/>
     </row>
@@ -5311,11 +5345,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="268">
+      <c r="K56" s="267">
         <f>-C4</f>
         <v>0</v>
       </c>
-      <c r="L56" s="269"/>
+      <c r="L56" s="268"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -5332,22 +5366,22 @@
       <c r="C58" s="112">
         <v>44507</v>
       </c>
-      <c r="D58" s="246" t="s">
+      <c r="D58" s="245" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="247"/>
+      <c r="E58" s="246"/>
       <c r="F58" s="113">
         <v>567389.35</v>
       </c>
-      <c r="I58" s="248" t="s">
+      <c r="I58" s="247" t="s">
         <v>103</v>
       </c>
-      <c r="J58" s="249"/>
-      <c r="K58" s="250">
+      <c r="J58" s="248"/>
+      <c r="K58" s="249">
         <f>K54+K56</f>
         <v>-24577.400000000023</v>
       </c>
-      <c r="L58" s="250"/>
+      <c r="L58" s="249"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -5491,6 +5525,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="I58:J58"/>
     <mergeCell ref="K58:L58"/>
@@ -5505,12 +5545,6 @@
     <mergeCell ref="I54:J54"/>
     <mergeCell ref="K54:L54"/>
     <mergeCell ref="K56:L56"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.15748031496062992" top="0.35433070866141736" bottom="0.31496062992125984" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="75" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -6835,7 +6869,7 @@
       <c r="A41" s="140">
         <v>44507</v>
       </c>
-      <c r="B41" s="270" t="s">
+      <c r="B41" s="280" t="s">
         <v>98</v>
       </c>
       <c r="C41" s="204">
@@ -6867,7 +6901,7 @@
       <c r="A42" s="140" t="s">
         <v>99</v>
       </c>
-      <c r="B42" s="271"/>
+      <c r="B42" s="281"/>
       <c r="C42" s="143">
         <v>0</v>
       </c>
@@ -8454,11 +8488,11 @@
   </sheetPr>
   <dimension ref="A1:S80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.42578125" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" style="97" customWidth="1"/>
@@ -8475,28 +8509,28 @@
     <col min="14" max="14" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.140625" customWidth="1"/>
     <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.140625" style="2" customWidth="1"/>
+    <col min="17" max="17" width="18.140625" style="287" customWidth="1"/>
     <col min="18" max="18" width="15.28515625" style="176" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="235"/>
-      <c r="C1" s="237" t="s">
+      <c r="B1" s="269"/>
+      <c r="C1" s="271" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="238"/>
-      <c r="E1" s="238"/>
-      <c r="F1" s="238"/>
-      <c r="G1" s="238"/>
-      <c r="H1" s="238"/>
-      <c r="I1" s="238"/>
-      <c r="J1" s="238"/>
-      <c r="K1" s="238"/>
-      <c r="L1" s="238"/>
-      <c r="M1" s="238"/>
+      <c r="D1" s="272"/>
+      <c r="E1" s="272"/>
+      <c r="F1" s="272"/>
+      <c r="G1" s="272"/>
+      <c r="H1" s="272"/>
+      <c r="I1" s="272"/>
+      <c r="J1" s="272"/>
+      <c r="K1" s="272"/>
+      <c r="L1" s="272"/>
+      <c r="M1" s="272"/>
     </row>
     <row r="2" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="236"/>
+      <c r="B2" s="270"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -8506,17 +8540,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:19" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="239" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="240"/>
+      <c r="B3" s="273" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="274"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="241" t="s">
+      <c r="H3" s="275" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="241"/>
+      <c r="I3" s="275"/>
       <c r="K3" s="178"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
@@ -8532,14 +8566,14 @@
       <c r="D4" s="18">
         <v>44507</v>
       </c>
-      <c r="E4" s="242" t="s">
+      <c r="E4" s="276" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="243"/>
-      <c r="H4" s="244" t="s">
+      <c r="F4" s="277"/>
+      <c r="H4" s="278" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="245"/>
+      <c r="I4" s="279"/>
       <c r="J4" s="19"/>
       <c r="K4" s="179"/>
       <c r="L4" s="20"/>
@@ -8549,10 +8583,10 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="251" t="s">
+      <c r="P4" s="250" t="s">
         <v>6</v>
       </c>
-      <c r="Q4" s="252"/>
+      <c r="Q4" s="251"/>
     </row>
     <row r="5" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
@@ -8638,29 +8672,35 @@
         <f>N6+M6+L6+I6+C6</f>
         <v>11269</v>
       </c>
-      <c r="Q6" s="290">
+      <c r="Q6" s="244">
         <f>P6-F6</f>
         <v>-26378</v>
       </c>
       <c r="R6" s="38"/>
       <c r="S6" s="147"/>
     </row>
-    <row r="7" spans="1:19" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="23"/>
       <c r="B7" s="24">
         <v>44510</v>
       </c>
-      <c r="C7" s="25"/>
+      <c r="C7" s="25">
+        <v>0</v>
+      </c>
       <c r="D7" s="40"/>
       <c r="E7" s="27">
         <v>44510</v>
       </c>
-      <c r="F7" s="28"/>
+      <c r="F7" s="28">
+        <v>34995</v>
+      </c>
       <c r="G7" s="2"/>
       <c r="H7" s="36">
         <v>44510</v>
       </c>
-      <c r="I7" s="30"/>
+      <c r="I7" s="30">
+        <v>64</v>
+      </c>
       <c r="J7" s="37"/>
       <c r="K7" s="38"/>
       <c r="L7" s="39"/>
@@ -8668,16 +8708,16 @@
         <v>0</v>
       </c>
       <c r="N7" s="33">
-        <v>0</v>
-      </c>
-      <c r="O7" s="285"/>
+        <v>4538</v>
+      </c>
+      <c r="O7" s="243"/>
       <c r="P7" s="69">
-        <f t="shared" ref="P6:P32" si="0">N7+M7+L7+I7+C7</f>
-        <v>0</v>
-      </c>
-      <c r="Q7" s="287">
-        <f t="shared" ref="Q6:Q38" si="1">P7-F7</f>
-        <v>0</v>
+        <f t="shared" ref="P7:P32" si="0">N7+M7+L7+I7+C7</f>
+        <v>4602</v>
+      </c>
+      <c r="Q7" s="244">
+        <f t="shared" ref="Q7:Q38" si="1">P7-F7</f>
+        <v>-30393</v>
       </c>
       <c r="R7" s="38"/>
       <c r="S7" s="147"/>
@@ -8687,34 +8727,48 @@
       <c r="B8" s="24">
         <v>44511</v>
       </c>
-      <c r="C8" s="25"/>
-      <c r="D8" s="42"/>
+      <c r="C8" s="25">
+        <v>10911</v>
+      </c>
+      <c r="D8" s="42" t="s">
+        <v>106</v>
+      </c>
       <c r="E8" s="27">
         <v>44511</v>
       </c>
-      <c r="F8" s="28"/>
+      <c r="F8" s="28">
+        <v>42232</v>
+      </c>
       <c r="G8" s="2"/>
       <c r="H8" s="36">
         <v>44511</v>
       </c>
-      <c r="I8" s="30"/>
-      <c r="J8" s="43"/>
-      <c r="K8" s="38"/>
-      <c r="L8" s="39"/>
+      <c r="I8" s="30">
+        <v>37</v>
+      </c>
+      <c r="J8" s="43">
+        <v>44511</v>
+      </c>
+      <c r="K8" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="L8" s="39">
+        <v>1665</v>
+      </c>
       <c r="M8" s="32">
         <v>0</v>
       </c>
       <c r="N8" s="33">
-        <v>0</v>
+        <v>9420</v>
       </c>
       <c r="O8" s="2"/>
       <c r="P8" s="69">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q8" s="288">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>22033</v>
+      </c>
+      <c r="Q8" s="244">
+        <f t="shared" si="1"/>
+        <v>-20199</v>
       </c>
       <c r="R8" s="38"/>
       <c r="S8" s="147"/>
@@ -8724,33 +8778,48 @@
       <c r="B9" s="24">
         <v>44512</v>
       </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="42"/>
+      <c r="C9" s="25">
+        <v>3408</v>
+      </c>
+      <c r="D9" s="42" t="s">
+        <v>107</v>
+      </c>
       <c r="E9" s="27">
         <v>44512</v>
       </c>
-      <c r="F9" s="28"/>
+      <c r="F9" s="28">
+        <v>53684</v>
+      </c>
       <c r="G9" s="2"/>
       <c r="H9" s="36">
         <v>44512</v>
       </c>
-      <c r="I9" s="30"/>
-      <c r="J9" s="37"/>
-      <c r="K9" s="284"/>
-      <c r="L9" s="39"/>
+      <c r="I9" s="30">
+        <v>72</v>
+      </c>
+      <c r="J9" s="37">
+        <v>44512</v>
+      </c>
+      <c r="K9" s="242" t="s">
+        <v>34</v>
+      </c>
+      <c r="L9" s="39">
+        <v>2280</v>
+      </c>
       <c r="M9" s="32">
         <v>0</v>
       </c>
       <c r="N9" s="33">
-        <v>0</v>
+        <v>12246</v>
       </c>
       <c r="O9" s="2"/>
       <c r="P9" s="69">
         <f>N9+M9+L9+I9+C9</f>
-        <v>0</v>
-      </c>
-      <c r="Q9" s="289" t="s">
-        <v>58</v>
+        <v>18006</v>
+      </c>
+      <c r="Q9" s="244">
+        <f t="shared" si="1"/>
+        <v>-35678</v>
       </c>
       <c r="R9" s="38"/>
       <c r="S9" s="147"/>
@@ -8760,34 +8829,48 @@
       <c r="B10" s="24">
         <v>44513</v>
       </c>
-      <c r="C10" s="25"/>
-      <c r="D10" s="40"/>
+      <c r="C10" s="25">
+        <v>6328</v>
+      </c>
+      <c r="D10" s="40" t="s">
+        <v>108</v>
+      </c>
       <c r="E10" s="27">
         <v>44513</v>
       </c>
-      <c r="F10" s="28"/>
+      <c r="F10" s="28">
+        <v>71293</v>
+      </c>
       <c r="G10" s="2"/>
       <c r="H10" s="36">
         <v>44513</v>
       </c>
-      <c r="I10" s="30"/>
-      <c r="J10" s="37"/>
-      <c r="K10" s="180"/>
-      <c r="L10" s="45"/>
+      <c r="I10" s="30">
+        <v>60</v>
+      </c>
+      <c r="J10" s="37">
+        <v>44513</v>
+      </c>
+      <c r="K10" s="288" t="s">
+        <v>109</v>
+      </c>
+      <c r="L10" s="289">
+        <v>13100</v>
+      </c>
       <c r="M10" s="32">
         <v>0</v>
       </c>
       <c r="N10" s="33">
-        <v>0</v>
+        <v>20880</v>
       </c>
       <c r="O10" s="2"/>
       <c r="P10" s="69">
         <f t="shared" ref="P10:P14" si="2">N10+M10+L10+I10+C10</f>
-        <v>0</v>
-      </c>
-      <c r="Q10" s="288">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>40368</v>
+      </c>
+      <c r="Q10" s="244">
+        <f t="shared" si="1"/>
+        <v>-30925</v>
       </c>
       <c r="R10" s="38"/>
       <c r="S10" s="147"/>
@@ -8797,17 +8880,23 @@
       <c r="B11" s="24">
         <v>44514</v>
       </c>
-      <c r="C11" s="25"/>
+      <c r="C11" s="25">
+        <v>0</v>
+      </c>
       <c r="D11" s="35"/>
       <c r="E11" s="27">
         <v>44514</v>
       </c>
-      <c r="F11" s="28"/>
+      <c r="F11" s="28">
+        <v>48859</v>
+      </c>
       <c r="G11" s="2"/>
       <c r="H11" s="36">
         <v>44514</v>
       </c>
-      <c r="I11" s="30"/>
+      <c r="I11" s="30">
+        <v>1875</v>
+      </c>
       <c r="J11" s="43"/>
       <c r="K11" s="181"/>
       <c r="L11" s="39"/>
@@ -8815,16 +8904,16 @@
         <v>0</v>
       </c>
       <c r="N11" s="33">
-        <v>0</v>
+        <v>11746</v>
       </c>
       <c r="O11" s="2"/>
       <c r="P11" s="69">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Q11" s="222">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>13621</v>
+      </c>
+      <c r="Q11" s="244">
+        <f t="shared" si="1"/>
+        <v>-35238</v>
       </c>
       <c r="R11" s="38"/>
       <c r="S11" s="147"/>
@@ -8834,39 +8923,49 @@
       <c r="B12" s="24">
         <v>44515</v>
       </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="35"/>
+      <c r="C12" s="25">
+        <v>1310</v>
+      </c>
+      <c r="D12" s="35" t="s">
+        <v>110</v>
+      </c>
       <c r="E12" s="27">
         <v>44515</v>
       </c>
-      <c r="F12" s="28"/>
+      <c r="F12" s="28">
+        <v>50041</v>
+      </c>
       <c r="G12" s="2"/>
       <c r="H12" s="36">
         <v>44515</v>
       </c>
-      <c r="I12" s="30"/>
+      <c r="I12" s="30">
+        <v>2054</v>
+      </c>
       <c r="J12" s="37"/>
-      <c r="K12" s="182"/>
+      <c r="K12" s="182" t="s">
+        <v>111</v>
+      </c>
       <c r="L12" s="39"/>
       <c r="M12" s="32">
         <v>0</v>
       </c>
       <c r="N12" s="33">
-        <v>0</v>
+        <v>16831</v>
       </c>
       <c r="O12" s="2"/>
       <c r="P12" s="69">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Q12" s="222">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>20195</v>
+      </c>
+      <c r="Q12" s="244">
+        <f t="shared" si="1"/>
+        <v>-29846</v>
       </c>
       <c r="R12" s="38"/>
       <c r="S12" s="147"/>
     </row>
-    <row r="13" spans="1:19" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="23"/>
       <c r="B13" s="24">
         <v>44516</v>
@@ -8896,7 +8995,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q13" s="287">
+      <c r="Q13" s="244">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -8933,14 +9032,14 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q14" s="289">
+      <c r="Q14" s="244">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R14" s="38"/>
       <c r="S14" s="147"/>
     </row>
-    <row r="15" spans="1:19" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="23"/>
       <c r="B15" s="24">
         <v>44518</v>
@@ -8969,7 +9068,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q15" s="286">
+      <c r="Q15" s="244">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -9005,7 +9104,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q16" s="222">
+      <c r="Q16" s="244">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -9041,7 +9140,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q17" s="222">
+      <c r="Q17" s="244">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -9077,7 +9176,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q18" s="288">
+      <c r="Q18" s="244">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -9113,7 +9212,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q19" s="288">
+      <c r="Q19" s="244">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -9149,7 +9248,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q20" s="222">
+      <c r="Q20" s="244">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -9185,7 +9284,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q21" s="222">
+      <c r="Q21" s="244">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -9221,7 +9320,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q22" s="288">
+      <c r="Q22" s="244">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -9257,7 +9356,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q23" s="288">
+      <c r="Q23" s="244">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -9293,7 +9392,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q24" s="288">
+      <c r="Q24" s="244">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -9329,7 +9428,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q25" s="233">
+      <c r="Q25" s="244">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -9364,7 +9463,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q26" s="9">
+      <c r="Q26" s="244">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -9399,7 +9498,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q27" s="9">
+      <c r="Q27" s="244">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -9434,7 +9533,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q28" s="9">
+      <c r="Q28" s="244">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -9469,7 +9568,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q29" s="9">
+      <c r="Q29" s="244">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -9504,7 +9603,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q30" s="9">
+      <c r="Q30" s="244">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -9539,7 +9638,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q31" s="9">
+      <c r="Q31" s="244">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -9574,7 +9673,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q32" s="9">
+      <c r="Q32" s="244">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -9602,7 +9701,7 @@
       <c r="P33" s="34">
         <v>0</v>
       </c>
-      <c r="Q33" s="9">
+      <c r="Q33" s="244">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -9636,7 +9735,7 @@
       <c r="P34" s="34">
         <v>0</v>
       </c>
-      <c r="Q34" s="9">
+      <c r="Q34" s="244">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -9670,7 +9769,7 @@
       <c r="P35" s="34">
         <v>0</v>
       </c>
-      <c r="Q35" s="9">
+      <c r="Q35" s="244">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -9700,7 +9799,7 @@
       <c r="P36" s="34">
         <v>0</v>
       </c>
-      <c r="Q36" s="9">
+      <c r="Q36" s="244">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -9730,7 +9829,7 @@
       <c r="P37" s="34">
         <v>0</v>
       </c>
-      <c r="Q37" s="9">
+      <c r="Q37" s="244">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -9759,7 +9858,7 @@
       <c r="P38" s="151">
         <v>0</v>
       </c>
-      <c r="Q38" s="151">
+      <c r="Q38" s="244">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -9777,21 +9876,21 @@
       <c r="J39" s="60"/>
       <c r="K39" s="190"/>
       <c r="L39" s="61"/>
-      <c r="M39" s="253">
+      <c r="M39" s="252">
         <f>SUM(M5:M38)</f>
         <v>0</v>
       </c>
-      <c r="N39" s="255">
+      <c r="N39" s="254">
         <f>SUM(N5:N38)</f>
-        <v>26123</v>
+        <v>101784</v>
       </c>
       <c r="P39" s="34">
         <f>SUM(P5:P38)</f>
-        <v>39032</v>
+        <v>157857</v>
       </c>
       <c r="Q39" s="234">
         <f>SUM(Q5:Q38)</f>
-        <v>-54314</v>
+        <v>-236593</v>
       </c>
     </row>
     <row r="40" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -9807,10 +9906,10 @@
       <c r="J40" s="60"/>
       <c r="K40" s="41"/>
       <c r="L40" s="61"/>
-      <c r="M40" s="254"/>
-      <c r="N40" s="256"/>
+      <c r="M40" s="253"/>
+      <c r="N40" s="255"/>
       <c r="P40" s="34"/>
-      <c r="Q40" s="9"/>
+      <c r="Q40" s="13"/>
     </row>
     <row r="41" spans="1:18" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="23"/>
@@ -9828,7 +9927,7 @@
       <c r="M41" s="78"/>
       <c r="N41" s="79"/>
       <c r="P41" s="34"/>
-      <c r="Q41" s="9"/>
+      <c r="Q41" s="13"/>
     </row>
     <row r="42" spans="1:18" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="23"/>
@@ -9846,7 +9945,7 @@
       <c r="M42" s="78"/>
       <c r="N42" s="79"/>
       <c r="P42" s="34"/>
-      <c r="Q42" s="9"/>
+      <c r="Q42" s="13"/>
     </row>
     <row r="43" spans="1:18" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="23"/>
@@ -9864,7 +9963,7 @@
       <c r="M43" s="78"/>
       <c r="N43" s="79"/>
       <c r="P43" s="34"/>
-      <c r="Q43" s="9"/>
+      <c r="Q43" s="13"/>
     </row>
     <row r="44" spans="1:18" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="23"/>
@@ -9882,7 +9981,7 @@
       <c r="M44" s="78"/>
       <c r="N44" s="79"/>
       <c r="P44" s="34"/>
-      <c r="Q44" s="9"/>
+      <c r="Q44" s="13"/>
     </row>
     <row r="45" spans="1:18" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="23"/>
@@ -9900,7 +9999,7 @@
       <c r="M45" s="78"/>
       <c r="N45" s="79"/>
       <c r="P45" s="34"/>
-      <c r="Q45" s="9"/>
+      <c r="Q45" s="13"/>
     </row>
     <row r="46" spans="1:18" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="23"/>
@@ -9918,7 +10017,7 @@
       <c r="M46" s="78"/>
       <c r="N46" s="79"/>
       <c r="P46" s="34"/>
-      <c r="Q46" s="9"/>
+      <c r="Q46" s="13"/>
     </row>
     <row r="47" spans="1:18" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="23"/>
@@ -9936,7 +10035,7 @@
       <c r="M47" s="78"/>
       <c r="N47" s="79"/>
       <c r="P47" s="34"/>
-      <c r="Q47" s="9"/>
+      <c r="Q47" s="13"/>
     </row>
     <row r="48" spans="1:18" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="23"/>
@@ -9954,9 +10053,9 @@
       <c r="M48" s="78"/>
       <c r="N48" s="79"/>
       <c r="P48" s="34"/>
-      <c r="Q48" s="9"/>
-    </row>
-    <row r="49" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q48" s="13"/>
+    </row>
+    <row r="49" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="23"/>
       <c r="B49" s="80"/>
       <c r="C49" s="25">
@@ -9973,7 +10072,7 @@
       <c r="M49" s="85"/>
       <c r="N49" s="33"/>
       <c r="P49" s="34"/>
-      <c r="Q49" s="9"/>
+      <c r="Q49" s="13"/>
     </row>
     <row r="50" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B50" s="86" t="s">
@@ -9981,7 +10080,7 @@
       </c>
       <c r="C50" s="87">
         <f>SUM(C5:C49)</f>
-        <v>12221</v>
+        <v>34178</v>
       </c>
       <c r="D50" s="88"/>
       <c r="E50" s="89" t="s">
@@ -9989,7 +10088,7 @@
       </c>
       <c r="F50" s="90">
         <f>SUM(F5:F49)</f>
-        <v>93346</v>
+        <v>394450</v>
       </c>
       <c r="G50" s="88"/>
       <c r="H50" s="91" t="s">
@@ -9997,7 +10096,7 @@
       </c>
       <c r="I50" s="92">
         <f>SUM(I5:I49)</f>
-        <v>688</v>
+        <v>4850</v>
       </c>
       <c r="J50" s="93"/>
       <c r="K50" s="94" t="s">
@@ -10005,75 +10104,75 @@
       </c>
       <c r="L50" s="95">
         <f>SUM(L5:L49)</f>
-        <v>0</v>
+        <v>17045</v>
       </c>
       <c r="M50" s="96"/>
       <c r="N50" s="96"/>
       <c r="P50" s="34"/>
-      <c r="Q50" s="9"/>
-    </row>
-    <row r="51" spans="1:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q50" s="13"/>
+    </row>
+    <row r="51" spans="1:17" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C51" s="3" t="s">
         <v>7</v>
       </c>
       <c r="P51" s="34"/>
-      <c r="Q51" s="9"/>
+      <c r="Q51" s="13"/>
     </row>
     <row r="52" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="257" t="s">
+      <c r="H52" s="256" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="258"/>
+      <c r="I52" s="257"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="259">
+      <c r="K52" s="258">
         <f>I50+L50</f>
-        <v>688</v>
-      </c>
-      <c r="L52" s="260"/>
-      <c r="M52" s="261">
+        <v>21895</v>
+      </c>
+      <c r="L52" s="259"/>
+      <c r="M52" s="260">
         <f>N39+M39</f>
-        <v>26123</v>
-      </c>
-      <c r="N52" s="262"/>
+        <v>101784</v>
+      </c>
+      <c r="N52" s="261"/>
       <c r="P52" s="34"/>
-      <c r="Q52" s="9"/>
-    </row>
-    <row r="53" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D53" s="263" t="s">
+      <c r="Q52" s="13"/>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D53" s="262" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="263"/>
+      <c r="E53" s="262"/>
       <c r="F53" s="101">
         <f>F50-K52-C50</f>
-        <v>80437</v>
+        <v>338377</v>
       </c>
       <c r="I53" s="102"/>
       <c r="J53" s="103"/>
       <c r="P53" s="34"/>
-      <c r="Q53" s="9"/>
+      <c r="Q53" s="13"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="263" t="s">
+      <c r="D54" s="262" t="s">
         <v>101</v>
       </c>
-      <c r="E54" s="263"/>
+      <c r="E54" s="262"/>
       <c r="F54" s="96">
         <v>-549976.4</v>
       </c>
-      <c r="I54" s="264" t="s">
+      <c r="I54" s="263" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="265"/>
-      <c r="K54" s="266">
+      <c r="J54" s="264"/>
+      <c r="K54" s="265">
         <f>F56+F57+F58</f>
-        <v>-469539.4</v>
-      </c>
-      <c r="L54" s="267"/>
+        <v>-211599.40000000002</v>
+      </c>
+      <c r="L54" s="266"/>
       <c r="P54" s="34"/>
-      <c r="Q54" s="9"/>
+      <c r="Q54" s="13"/>
     </row>
     <row r="55" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D55" s="203" t="s">
@@ -10097,18 +10196,18 @@
       </c>
       <c r="F56" s="96">
         <f>SUM(F53:F55)</f>
-        <v>-469539.4</v>
+        <v>-211599.40000000002</v>
       </c>
       <c r="H56" s="23"/>
       <c r="I56" s="108" t="s">
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="268">
+      <c r="K56" s="267">
         <f>-C4</f>
         <v>-567389.35</v>
       </c>
-      <c r="L56" s="269"/>
+      <c r="L56" s="268"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -10123,22 +10222,22 @@
     </row>
     <row r="58" spans="1:17" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C58" s="112"/>
-      <c r="D58" s="246" t="s">
+      <c r="D58" s="245" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="247"/>
+      <c r="E58" s="246"/>
       <c r="F58" s="113">
         <v>0</v>
       </c>
-      <c r="I58" s="248" t="s">
+      <c r="I58" s="247" t="s">
         <v>103</v>
       </c>
-      <c r="J58" s="249"/>
-      <c r="K58" s="250">
+      <c r="J58" s="248"/>
+      <c r="K58" s="249">
         <f>K54+K56</f>
-        <v>-1036928.75</v>
-      </c>
-      <c r="L58" s="250"/>
+        <v>-778988.75</v>
+      </c>
+      <c r="L58" s="249"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -10165,14 +10264,14 @@
       <c r="M61" s="124"/>
       <c r="N61" s="98"/>
     </row>
-    <row r="62" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B62" s="121"/>
       <c r="C62" s="125"/>
       <c r="E62" s="34"/>
       <c r="M62" s="124"/>
       <c r="N62" s="98"/>
     </row>
-    <row r="63" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B63" s="121"/>
       <c r="C63" s="125"/>
       <c r="E63" s="34"/>
@@ -10180,13 +10279,13 @@
       <c r="L63" s="127"/>
       <c r="M63" s="1"/>
     </row>
-    <row r="64" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B64" s="121"/>
       <c r="C64" s="125"/>
       <c r="E64" s="34"/>
       <c r="M64" s="1"/>
     </row>
-    <row r="65" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B65" s="121"/>
       <c r="C65" s="125"/>
       <c r="D65" s="128"/>
@@ -10282,11 +10381,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="I54:J54"/>
-    <mergeCell ref="K54:L54"/>
-    <mergeCell ref="K56:L56"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="I58:J58"/>
     <mergeCell ref="K58:L58"/>
@@ -10296,16 +10396,16 @@
     <mergeCell ref="H52:I52"/>
     <mergeCell ref="K52:L52"/>
     <mergeCell ref="M52:N52"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="I54:J54"/>
+    <mergeCell ref="K54:L54"/>
+    <mergeCell ref="K56:L56"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -10407,9 +10507,9 @@
         <f>C3-E3</f>
         <v>0</v>
       </c>
-      <c r="I3" s="280"/>
-      <c r="J3" s="281"/>
-      <c r="K3" s="282"/>
+      <c r="I3" s="238"/>
+      <c r="J3" s="239"/>
+      <c r="K3" s="240"/>
       <c r="L3" s="136"/>
       <c r="M3" s="69"/>
       <c r="N3" s="196">
@@ -10428,9 +10528,9 @@
         <v>0</v>
       </c>
       <c r="G4" s="138"/>
-      <c r="I4" s="280"/>
-      <c r="J4" s="281"/>
-      <c r="K4" s="282"/>
+      <c r="I4" s="238"/>
+      <c r="J4" s="239"/>
+      <c r="K4" s="240"/>
       <c r="L4" s="136"/>
       <c r="M4" s="69"/>
       <c r="N4" s="137">
@@ -10448,9 +10548,9 @@
         <f t="shared" ref="F5:F68" si="0">F4+C5-E5</f>
         <v>0</v>
       </c>
-      <c r="I5" s="280"/>
-      <c r="J5" s="281"/>
-      <c r="K5" s="282"/>
+      <c r="I5" s="238"/>
+      <c r="J5" s="239"/>
+      <c r="K5" s="240"/>
       <c r="L5" s="136"/>
       <c r="M5" s="69"/>
       <c r="N5" s="137">
@@ -10468,9 +10568,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I6" s="280"/>
-      <c r="J6" s="281"/>
-      <c r="K6" s="282"/>
+      <c r="I6" s="238"/>
+      <c r="J6" s="239"/>
+      <c r="K6" s="240"/>
       <c r="L6" s="136"/>
       <c r="M6" s="69"/>
       <c r="N6" s="137">
@@ -10488,9 +10588,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I7" s="280"/>
-      <c r="J7" s="281"/>
-      <c r="K7" s="282"/>
+      <c r="I7" s="238"/>
+      <c r="J7" s="239"/>
+      <c r="K7" s="240"/>
       <c r="L7" s="136"/>
       <c r="M7" s="69"/>
       <c r="N7" s="137">
@@ -10508,9 +10608,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I8" s="280"/>
-      <c r="J8" s="281"/>
-      <c r="K8" s="282"/>
+      <c r="I8" s="238"/>
+      <c r="J8" s="239"/>
+      <c r="K8" s="240"/>
       <c r="L8" s="136"/>
       <c r="M8" s="69"/>
       <c r="N8" s="137">
@@ -10528,9 +10628,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I9" s="280"/>
-      <c r="J9" s="281"/>
-      <c r="K9" s="282"/>
+      <c r="I9" s="238"/>
+      <c r="J9" s="239"/>
+      <c r="K9" s="240"/>
       <c r="L9" s="136"/>
       <c r="M9" s="69"/>
       <c r="N9" s="137">
@@ -10549,9 +10649,9 @@
         <v>0</v>
       </c>
       <c r="G10" s="138"/>
-      <c r="I10" s="280"/>
-      <c r="J10" s="281"/>
-      <c r="K10" s="282"/>
+      <c r="I10" s="238"/>
+      <c r="J10" s="239"/>
+      <c r="K10" s="240"/>
       <c r="L10" s="136"/>
       <c r="M10" s="69"/>
       <c r="N10" s="137">
@@ -10569,9 +10669,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I11" s="280"/>
-      <c r="J11" s="281"/>
-      <c r="K11" s="282"/>
+      <c r="I11" s="238"/>
+      <c r="J11" s="239"/>
+      <c r="K11" s="240"/>
       <c r="L11" s="140"/>
       <c r="M11" s="69"/>
       <c r="N11" s="137">
@@ -10589,9 +10689,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I12" s="280"/>
-      <c r="J12" s="281"/>
-      <c r="K12" s="282"/>
+      <c r="I12" s="238"/>
+      <c r="J12" s="239"/>
+      <c r="K12" s="240"/>
       <c r="L12" s="140"/>
       <c r="M12" s="69"/>
       <c r="N12" s="137">
@@ -10601,17 +10701,17 @@
     </row>
     <row r="13" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="140"/>
-      <c r="B13" s="275"/>
-      <c r="C13" s="276"/>
+      <c r="B13" s="235"/>
+      <c r="C13" s="236"/>
       <c r="D13" s="140"/>
       <c r="E13" s="69"/>
       <c r="F13" s="137">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I13" s="280"/>
-      <c r="J13" s="281"/>
-      <c r="K13" s="282"/>
+      <c r="I13" s="238"/>
+      <c r="J13" s="239"/>
+      <c r="K13" s="240"/>
       <c r="L13" s="140"/>
       <c r="M13" s="69"/>
       <c r="N13" s="137">
@@ -10629,9 +10729,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I14" s="280"/>
-      <c r="J14" s="281"/>
-      <c r="K14" s="282"/>
+      <c r="I14" s="238"/>
+      <c r="J14" s="239"/>
+      <c r="K14" s="240"/>
       <c r="L14" s="140"/>
       <c r="M14" s="69"/>
       <c r="N14" s="137">
@@ -10649,9 +10749,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I15" s="280"/>
-      <c r="J15" s="281"/>
-      <c r="K15" s="282"/>
+      <c r="I15" s="238"/>
+      <c r="J15" s="239"/>
+      <c r="K15" s="240"/>
       <c r="L15" s="140"/>
       <c r="M15" s="69"/>
       <c r="N15" s="137">
@@ -10669,9 +10769,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I16" s="280"/>
-      <c r="J16" s="281"/>
-      <c r="K16" s="282"/>
+      <c r="I16" s="238"/>
+      <c r="J16" s="239"/>
+      <c r="K16" s="240"/>
       <c r="L16" s="140"/>
       <c r="M16" s="69"/>
       <c r="N16" s="137">
@@ -10689,9 +10789,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I17" s="280"/>
-      <c r="J17" s="281"/>
-      <c r="K17" s="282"/>
+      <c r="I17" s="238"/>
+      <c r="J17" s="239"/>
+      <c r="K17" s="240"/>
       <c r="L17" s="140"/>
       <c r="M17" s="69"/>
       <c r="N17" s="137">
@@ -10709,9 +10809,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I18" s="280"/>
-      <c r="J18" s="281"/>
-      <c r="K18" s="282"/>
+      <c r="I18" s="238"/>
+      <c r="J18" s="239"/>
+      <c r="K18" s="240"/>
       <c r="L18" s="140"/>
       <c r="M18" s="69"/>
       <c r="N18" s="137">
@@ -10729,9 +10829,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I19" s="280"/>
-      <c r="J19" s="281"/>
-      <c r="K19" s="282"/>
+      <c r="I19" s="238"/>
+      <c r="J19" s="239"/>
+      <c r="K19" s="240"/>
       <c r="L19" s="140"/>
       <c r="M19" s="69"/>
       <c r="N19" s="137">
@@ -10749,9 +10849,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I20" s="280"/>
-      <c r="J20" s="281"/>
-      <c r="K20" s="282"/>
+      <c r="I20" s="238"/>
+      <c r="J20" s="239"/>
+      <c r="K20" s="240"/>
       <c r="L20" s="140"/>
       <c r="M20" s="69"/>
       <c r="N20" s="137">
@@ -10769,9 +10869,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I21" s="280"/>
-      <c r="J21" s="281"/>
-      <c r="K21" s="282"/>
+      <c r="I21" s="238"/>
+      <c r="J21" s="239"/>
+      <c r="K21" s="240"/>
       <c r="L21" s="140"/>
       <c r="M21" s="69"/>
       <c r="N21" s="137">
@@ -10790,9 +10890,9 @@
         <v>0</v>
       </c>
       <c r="G22" s="138"/>
-      <c r="I22" s="280"/>
-      <c r="J22" s="281"/>
-      <c r="K22" s="282"/>
+      <c r="I22" s="238"/>
+      <c r="J22" s="239"/>
+      <c r="K22" s="240"/>
       <c r="L22" s="140"/>
       <c r="M22" s="69"/>
       <c r="N22" s="137">
@@ -10810,9 +10910,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I23" s="280"/>
-      <c r="J23" s="281"/>
-      <c r="K23" s="282"/>
+      <c r="I23" s="238"/>
+      <c r="J23" s="239"/>
+      <c r="K23" s="240"/>
       <c r="L23" s="140"/>
       <c r="M23" s="69"/>
       <c r="N23" s="137">
@@ -10830,9 +10930,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I24" s="280"/>
-      <c r="J24" s="281"/>
-      <c r="K24" s="282"/>
+      <c r="I24" s="238"/>
+      <c r="J24" s="239"/>
+      <c r="K24" s="240"/>
       <c r="L24" s="140"/>
       <c r="M24" s="69"/>
       <c r="N24" s="137">
@@ -10850,9 +10950,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I25" s="280"/>
-      <c r="J25" s="281"/>
-      <c r="K25" s="282"/>
+      <c r="I25" s="238"/>
+      <c r="J25" s="239"/>
+      <c r="K25" s="240"/>
       <c r="L25" s="140"/>
       <c r="M25" s="69"/>
       <c r="N25" s="137">
@@ -10870,9 +10970,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I26" s="280"/>
-      <c r="J26" s="281"/>
-      <c r="K26" s="282"/>
+      <c r="I26" s="238"/>
+      <c r="J26" s="239"/>
+      <c r="K26" s="240"/>
       <c r="L26" s="140"/>
       <c r="M26" s="69"/>
       <c r="N26" s="137">
@@ -10890,9 +10990,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I27" s="280"/>
-      <c r="J27" s="281"/>
-      <c r="K27" s="282"/>
+      <c r="I27" s="238"/>
+      <c r="J27" s="239"/>
+      <c r="K27" s="240"/>
       <c r="L27" s="140"/>
       <c r="M27" s="69"/>
       <c r="N27" s="137">
@@ -10910,9 +11010,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I28" s="280"/>
-      <c r="J28" s="281"/>
-      <c r="K28" s="282"/>
+      <c r="I28" s="238"/>
+      <c r="J28" s="239"/>
+      <c r="K28" s="240"/>
       <c r="L28" s="140"/>
       <c r="M28" s="69"/>
       <c r="N28" s="137">
@@ -10930,9 +11030,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I29" s="280"/>
-      <c r="J29" s="281"/>
-      <c r="K29" s="282"/>
+      <c r="I29" s="238"/>
+      <c r="J29" s="239"/>
+      <c r="K29" s="240"/>
       <c r="L29" s="140"/>
       <c r="M29" s="69"/>
       <c r="N29" s="137">
@@ -10951,9 +11051,9 @@
         <v>0</v>
       </c>
       <c r="G30" s="138"/>
-      <c r="I30" s="280"/>
-      <c r="J30" s="281"/>
-      <c r="K30" s="282"/>
+      <c r="I30" s="238"/>
+      <c r="J30" s="239"/>
+      <c r="K30" s="240"/>
       <c r="L30" s="140"/>
       <c r="M30" s="69"/>
       <c r="N30" s="137">
@@ -10971,9 +11071,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I31" s="280"/>
-      <c r="J31" s="281"/>
-      <c r="K31" s="282"/>
+      <c r="I31" s="238"/>
+      <c r="J31" s="239"/>
+      <c r="K31" s="240"/>
       <c r="L31" s="140"/>
       <c r="M31" s="69"/>
       <c r="N31" s="137">
@@ -10991,9 +11091,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I32" s="280"/>
-      <c r="J32" s="281"/>
-      <c r="K32" s="282"/>
+      <c r="I32" s="238"/>
+      <c r="J32" s="239"/>
+      <c r="K32" s="240"/>
       <c r="L32" s="140"/>
       <c r="M32" s="69"/>
       <c r="N32" s="137">
@@ -11011,9 +11111,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I33" s="280"/>
-      <c r="J33" s="281"/>
-      <c r="K33" s="282"/>
+      <c r="I33" s="238"/>
+      <c r="J33" s="239"/>
+      <c r="K33" s="240"/>
       <c r="L33" s="140"/>
       <c r="M33" s="69"/>
       <c r="N33" s="137">
@@ -11031,9 +11131,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I34" s="280"/>
-      <c r="J34" s="281"/>
-      <c r="K34" s="282"/>
+      <c r="I34" s="238"/>
+      <c r="J34" s="239"/>
+      <c r="K34" s="240"/>
       <c r="L34" s="140"/>
       <c r="M34" s="69"/>
       <c r="N34" s="137">
@@ -11051,9 +11151,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I35" s="280"/>
-      <c r="J35" s="281"/>
-      <c r="K35" s="282"/>
+      <c r="I35" s="238"/>
+      <c r="J35" s="239"/>
+      <c r="K35" s="240"/>
       <c r="L35" s="140"/>
       <c r="M35" s="69"/>
       <c r="N35" s="137">
@@ -11071,9 +11171,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I36" s="280"/>
-      <c r="J36" s="281"/>
-      <c r="K36" s="282"/>
+      <c r="I36" s="238"/>
+      <c r="J36" s="239"/>
+      <c r="K36" s="240"/>
       <c r="L36" s="140"/>
       <c r="M36" s="69"/>
       <c r="N36" s="137">
@@ -11091,9 +11191,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I37" s="280"/>
-      <c r="J37" s="281"/>
-      <c r="K37" s="282"/>
+      <c r="I37" s="238"/>
+      <c r="J37" s="239"/>
+      <c r="K37" s="240"/>
       <c r="L37" s="140"/>
       <c r="M37" s="69"/>
       <c r="N37" s="137">
@@ -11111,9 +11211,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I38" s="280"/>
-      <c r="J38" s="281"/>
-      <c r="K38" s="282"/>
+      <c r="I38" s="238"/>
+      <c r="J38" s="239"/>
+      <c r="K38" s="240"/>
       <c r="L38" s="140"/>
       <c r="M38" s="69"/>
       <c r="N38" s="137">
@@ -11131,9 +11231,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I39" s="280"/>
-      <c r="J39" s="281"/>
-      <c r="K39" s="282"/>
+      <c r="I39" s="238"/>
+      <c r="J39" s="239"/>
+      <c r="K39" s="240"/>
       <c r="L39" s="140"/>
       <c r="M39" s="69"/>
       <c r="N39" s="137">
@@ -11151,9 +11251,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I40" s="280"/>
-      <c r="J40" s="281"/>
-      <c r="K40" s="282"/>
+      <c r="I40" s="238"/>
+      <c r="J40" s="239"/>
+      <c r="K40" s="240"/>
       <c r="L40" s="140"/>
       <c r="M40" s="69"/>
       <c r="N40" s="137">
@@ -11163,17 +11263,17 @@
     </row>
     <row r="41" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="140"/>
-      <c r="B41" s="277"/>
-      <c r="C41" s="278"/>
+      <c r="B41" s="282"/>
+      <c r="C41" s="237"/>
       <c r="D41" s="140"/>
       <c r="E41" s="69"/>
       <c r="F41" s="137">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I41" s="280"/>
-      <c r="J41" s="281"/>
-      <c r="K41" s="282"/>
+      <c r="I41" s="238"/>
+      <c r="J41" s="239"/>
+      <c r="K41" s="240"/>
       <c r="L41" s="140"/>
       <c r="M41" s="69"/>
       <c r="N41" s="137">
@@ -11183,7 +11283,7 @@
     </row>
     <row r="42" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="140"/>
-      <c r="B42" s="279"/>
+      <c r="B42" s="283"/>
       <c r="C42" s="69"/>
       <c r="D42" s="140"/>
       <c r="E42" s="69"/>
@@ -11191,9 +11291,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I42" s="280"/>
-      <c r="J42" s="281"/>
-      <c r="K42" s="282"/>
+      <c r="I42" s="238"/>
+      <c r="J42" s="239"/>
+      <c r="K42" s="240"/>
       <c r="L42" s="140"/>
       <c r="M42" s="69"/>
       <c r="N42" s="137">
@@ -11211,9 +11311,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I43" s="280"/>
-      <c r="J43" s="281"/>
-      <c r="K43" s="282"/>
+      <c r="I43" s="238"/>
+      <c r="J43" s="239"/>
+      <c r="K43" s="240"/>
       <c r="L43" s="140"/>
       <c r="M43" s="69"/>
       <c r="N43" s="137">
@@ -11231,9 +11331,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I44" s="280"/>
-      <c r="J44" s="281"/>
-      <c r="K44" s="283"/>
+      <c r="I44" s="238"/>
+      <c r="J44" s="239"/>
+      <c r="K44" s="241"/>
       <c r="L44" s="140"/>
       <c r="M44" s="69"/>
       <c r="N44" s="137">
@@ -11251,9 +11351,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I45" s="280"/>
-      <c r="J45" s="281"/>
-      <c r="K45" s="282"/>
+      <c r="I45" s="238"/>
+      <c r="J45" s="239"/>
+      <c r="K45" s="240"/>
       <c r="L45" s="140"/>
       <c r="M45" s="69"/>
       <c r="N45" s="137">
@@ -11271,9 +11371,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I46" s="280"/>
-      <c r="J46" s="281"/>
-      <c r="K46" s="282"/>
+      <c r="I46" s="238"/>
+      <c r="J46" s="239"/>
+      <c r="K46" s="240"/>
       <c r="L46" s="140"/>
       <c r="M46" s="69"/>
       <c r="N46" s="137">
@@ -11291,9 +11391,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I47" s="280"/>
-      <c r="J47" s="281"/>
-      <c r="K47" s="282"/>
+      <c r="I47" s="238"/>
+      <c r="J47" s="239"/>
+      <c r="K47" s="240"/>
       <c r="L47" s="140"/>
       <c r="M47" s="69"/>
       <c r="N47" s="137">
@@ -11311,9 +11411,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I48" s="280"/>
-      <c r="J48" s="281"/>
-      <c r="K48" s="282"/>
+      <c r="I48" s="238"/>
+      <c r="J48" s="239"/>
+      <c r="K48" s="240"/>
       <c r="L48" s="140"/>
       <c r="M48" s="69"/>
       <c r="N48" s="137">
@@ -11331,9 +11431,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I49" s="280"/>
-      <c r="J49" s="281"/>
-      <c r="K49" s="282"/>
+      <c r="I49" s="238"/>
+      <c r="J49" s="239"/>
+      <c r="K49" s="240"/>
       <c r="L49" s="140"/>
       <c r="M49" s="69"/>
       <c r="N49" s="137">
@@ -11351,9 +11451,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I50" s="280"/>
-      <c r="J50" s="281"/>
-      <c r="K50" s="282"/>
+      <c r="I50" s="238"/>
+      <c r="J50" s="239"/>
+      <c r="K50" s="240"/>
       <c r="L50" s="140"/>
       <c r="M50" s="69"/>
       <c r="N50" s="137">
@@ -11371,9 +11471,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I51" s="280"/>
-      <c r="J51" s="281"/>
-      <c r="K51" s="282"/>
+      <c r="I51" s="238"/>
+      <c r="J51" s="239"/>
+      <c r="K51" s="240"/>
       <c r="L51" s="140"/>
       <c r="M51" s="69"/>
       <c r="N51" s="137">
@@ -11391,9 +11491,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I52" s="280"/>
-      <c r="J52" s="281"/>
-      <c r="K52" s="282"/>
+      <c r="I52" s="238"/>
+      <c r="J52" s="239"/>
+      <c r="K52" s="240"/>
       <c r="L52" s="140"/>
       <c r="M52" s="69"/>
       <c r="N52" s="137">
@@ -11411,9 +11511,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I53" s="280"/>
-      <c r="J53" s="281"/>
-      <c r="K53" s="282"/>
+      <c r="I53" s="238"/>
+      <c r="J53" s="239"/>
+      <c r="K53" s="240"/>
       <c r="L53" s="140"/>
       <c r="M53" s="69"/>
       <c r="N53" s="137">
@@ -11431,9 +11531,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I54" s="280"/>
-      <c r="J54" s="281"/>
-      <c r="K54" s="282"/>
+      <c r="I54" s="238"/>
+      <c r="J54" s="239"/>
+      <c r="K54" s="240"/>
       <c r="L54" s="140"/>
       <c r="M54" s="69"/>
       <c r="N54" s="137">
@@ -11451,9 +11551,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I55" s="280"/>
-      <c r="J55" s="281"/>
-      <c r="K55" s="282"/>
+      <c r="I55" s="238"/>
+      <c r="J55" s="239"/>
+      <c r="K55" s="240"/>
       <c r="L55" s="140"/>
       <c r="M55" s="69"/>
       <c r="N55" s="137">
@@ -11471,9 +11571,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I56" s="280"/>
-      <c r="J56" s="281"/>
-      <c r="K56" s="282"/>
+      <c r="I56" s="238"/>
+      <c r="J56" s="239"/>
+      <c r="K56" s="240"/>
       <c r="L56" s="140"/>
       <c r="M56" s="69"/>
       <c r="N56" s="137">
@@ -11491,9 +11591,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I57" s="280"/>
-      <c r="J57" s="281"/>
-      <c r="K57" s="282"/>
+      <c r="I57" s="238"/>
+      <c r="J57" s="239"/>
+      <c r="K57" s="240"/>
       <c r="L57" s="140"/>
       <c r="M57" s="69"/>
       <c r="N57" s="137">
@@ -11511,9 +11611,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I58" s="280"/>
-      <c r="J58" s="281"/>
-      <c r="K58" s="282"/>
+      <c r="I58" s="238"/>
+      <c r="J58" s="239"/>
+      <c r="K58" s="240"/>
       <c r="L58" s="140"/>
       <c r="M58" s="69"/>
       <c r="N58" s="137">
@@ -11531,9 +11631,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I59" s="280"/>
-      <c r="J59" s="281"/>
-      <c r="K59" s="283"/>
+      <c r="I59" s="238"/>
+      <c r="J59" s="239"/>
+      <c r="K59" s="241"/>
       <c r="L59" s="140"/>
       <c r="M59" s="69"/>
       <c r="N59" s="137">
@@ -12707,12 +12807,12 @@
     <row r="42" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="43" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="155"/>
-      <c r="B43" s="272" t="s">
+      <c r="B43" s="284" t="s">
         <v>25</v>
       </c>
-      <c r="C43" s="273"/>
-      <c r="D43" s="273"/>
-      <c r="E43" s="274"/>
+      <c r="C43" s="285"/>
+      <c r="D43" s="285"/>
+      <c r="E43" s="286"/>
       <c r="F43" s="1"/>
     </row>
     <row r="44" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
CIERRE 29 NOV 21
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 11  NOVIEMBRE 2021/BALANCE    ZAVALETA   NOVIEMBRE    2021.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 11  NOVIEMBRE 2021/BALANCE    ZAVALETA   NOVIEMBRE    2021.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14325" windowHeight="10620" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14325" windowHeight="10620" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="OCTUBRE      2 0 2 1     " sheetId="1" r:id="rId1"/>
@@ -146,7 +146,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="119">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -482,6 +482,27 @@
   </si>
   <si>
     <t xml:space="preserve">                                      </t>
+  </si>
+  <si>
+    <t>POLLO-</t>
+  </si>
+  <si>
+    <t>tarejta cobro duplicado $ 685.00</t>
+  </si>
+  <si>
+    <t>POLLO--ENCHILADA</t>
+  </si>
+  <si>
+    <t>POLLO-LACTEOS-LONGANIZA</t>
+  </si>
+  <si>
+    <t>POLLO-QUESOS NLP</t>
+  </si>
+  <si>
+    <t>JAMONES-LONGANIZA-QUESOS-POLLO-CHISTORRA</t>
+  </si>
+  <si>
+    <t>NOMINA # 47</t>
   </si>
 </sst>
 </file>
@@ -885,7 +906,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -958,6 +979,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="61">
     <border>
@@ -1718,7 +1745,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="290">
+  <cellXfs count="296">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -2202,138 +2229,154 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="47" fillId="0" borderId="50" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="6" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="6" borderId="51" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="6" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="50" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="43" fillId="6" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="43" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="43" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="43" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="20" fillId="12" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="2" fillId="12" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="6" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="44" fontId="19" fillId="13" borderId="50" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="6" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="6" borderId="51" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="6" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="50" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="43" fillId="6" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="43" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="43" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="43" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2344,8 +2387,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF0000FF"/>
       <color rgb="FF99CCFF"/>
-      <color rgb="FF0000FF"/>
       <color rgb="FF800000"/>
       <color rgb="FF6600FF"/>
     </mruColors>
@@ -3507,23 +3550,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="269"/>
-      <c r="C1" s="271" t="s">
+      <c r="B1" s="254"/>
+      <c r="C1" s="256" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="272"/>
-      <c r="E1" s="272"/>
-      <c r="F1" s="272"/>
-      <c r="G1" s="272"/>
-      <c r="H1" s="272"/>
-      <c r="I1" s="272"/>
-      <c r="J1" s="272"/>
-      <c r="K1" s="272"/>
-      <c r="L1" s="272"/>
-      <c r="M1" s="272"/>
+      <c r="D1" s="257"/>
+      <c r="E1" s="257"/>
+      <c r="F1" s="257"/>
+      <c r="G1" s="257"/>
+      <c r="H1" s="257"/>
+      <c r="I1" s="257"/>
+      <c r="J1" s="257"/>
+      <c r="K1" s="257"/>
+      <c r="L1" s="257"/>
+      <c r="M1" s="257"/>
     </row>
     <row r="2" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="270"/>
+      <c r="B2" s="255"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -3533,17 +3576,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:19" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="273" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="274"/>
+      <c r="B3" s="258" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="259"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="275" t="s">
+      <c r="H3" s="260" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="275"/>
+      <c r="I3" s="260"/>
       <c r="K3" s="178"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
@@ -3557,14 +3600,14 @@
         <v>0</v>
       </c>
       <c r="D4" s="18"/>
-      <c r="E4" s="276" t="s">
+      <c r="E4" s="261" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="277"/>
-      <c r="H4" s="278" t="s">
+      <c r="F4" s="262"/>
+      <c r="H4" s="263" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="279"/>
+      <c r="I4" s="264"/>
       <c r="J4" s="19"/>
       <c r="K4" s="179"/>
       <c r="L4" s="20"/>
@@ -3574,10 +3617,10 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="250" t="s">
+      <c r="P4" s="270" t="s">
         <v>6</v>
       </c>
-      <c r="Q4" s="251"/>
+      <c r="Q4" s="271"/>
     </row>
     <row r="5" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
@@ -5018,11 +5061,11 @@
       <c r="J39" s="60"/>
       <c r="K39" s="190"/>
       <c r="L39" s="61"/>
-      <c r="M39" s="252">
+      <c r="M39" s="272">
         <f>SUM(M5:M38)</f>
         <v>247061</v>
       </c>
-      <c r="N39" s="254">
+      <c r="N39" s="274">
         <f>SUM(N5:N38)</f>
         <v>172863</v>
       </c>
@@ -5048,8 +5091,8 @@
       <c r="J40" s="60"/>
       <c r="K40" s="41"/>
       <c r="L40" s="61"/>
-      <c r="M40" s="253"/>
-      <c r="N40" s="255"/>
+      <c r="M40" s="273"/>
+      <c r="N40" s="275"/>
       <c r="P40" s="34"/>
       <c r="Q40" s="9"/>
     </row>
@@ -5264,29 +5307,29 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="256" t="s">
+      <c r="H52" s="276" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="257"/>
+      <c r="I52" s="277"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="258">
+      <c r="K52" s="278">
         <f>I50+L50</f>
         <v>53873.49</v>
       </c>
-      <c r="L52" s="259"/>
-      <c r="M52" s="260">
+      <c r="L52" s="279"/>
+      <c r="M52" s="280">
         <f>N39+M39</f>
         <v>419924</v>
       </c>
-      <c r="N52" s="261"/>
+      <c r="N52" s="281"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D53" s="262" t="s">
+      <c r="D53" s="282" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="262"/>
+      <c r="E53" s="282"/>
       <c r="F53" s="101">
         <f>F50-K52-C50</f>
         <v>471038.61</v>
@@ -5297,22 +5340,22 @@
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="262" t="s">
+      <c r="D54" s="282" t="s">
         <v>101</v>
       </c>
-      <c r="E54" s="262"/>
+      <c r="E54" s="282"/>
       <c r="F54" s="96">
         <v>-549976.4</v>
       </c>
-      <c r="I54" s="263" t="s">
+      <c r="I54" s="283" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="264"/>
-      <c r="K54" s="265">
+      <c r="J54" s="284"/>
+      <c r="K54" s="285">
         <f>F56+F57+F58</f>
         <v>-24577.400000000023</v>
       </c>
-      <c r="L54" s="266"/>
+      <c r="L54" s="286"/>
       <c r="P54" s="34"/>
       <c r="Q54" s="9"/>
     </row>
@@ -5345,11 +5388,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="267">
+      <c r="K56" s="287">
         <f>-C4</f>
         <v>0</v>
       </c>
-      <c r="L56" s="268"/>
+      <c r="L56" s="288"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -5366,22 +5409,22 @@
       <c r="C58" s="112">
         <v>44507</v>
       </c>
-      <c r="D58" s="245" t="s">
+      <c r="D58" s="265" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="246"/>
+      <c r="E58" s="266"/>
       <c r="F58" s="113">
         <v>567389.35</v>
       </c>
-      <c r="I58" s="247" t="s">
+      <c r="I58" s="267" t="s">
         <v>103</v>
       </c>
-      <c r="J58" s="248"/>
-      <c r="K58" s="249">
+      <c r="J58" s="268"/>
+      <c r="K58" s="269">
         <f>K54+K56</f>
         <v>-24577.400000000023</v>
       </c>
-      <c r="L58" s="249"/>
+      <c r="L58" s="269"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -5525,12 +5568,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="I58:J58"/>
     <mergeCell ref="K58:L58"/>
@@ -5545,6 +5582,12 @@
     <mergeCell ref="I54:J54"/>
     <mergeCell ref="K54:L54"/>
     <mergeCell ref="K56:L56"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.15748031496062992" top="0.35433070866141736" bottom="0.31496062992125984" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="75" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -6869,7 +6912,7 @@
       <c r="A41" s="140">
         <v>44507</v>
       </c>
-      <c r="B41" s="280" t="s">
+      <c r="B41" s="289" t="s">
         <v>98</v>
       </c>
       <c r="C41" s="204">
@@ -6901,7 +6944,7 @@
       <c r="A42" s="140" t="s">
         <v>99</v>
       </c>
-      <c r="B42" s="281"/>
+      <c r="B42" s="290"/>
       <c r="C42" s="143">
         <v>0</v>
       </c>
@@ -8486,10 +8529,10 @@
   <sheetPr>
     <tabColor rgb="FF002060"/>
   </sheetPr>
-  <dimension ref="A1:S80"/>
+  <dimension ref="A1:U80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+    <sheetView tabSelected="1" topLeftCell="G9" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -8509,28 +8552,28 @@
     <col min="14" max="14" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.140625" customWidth="1"/>
     <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.140625" style="287" customWidth="1"/>
-    <col min="18" max="18" width="15.28515625" style="176" customWidth="1"/>
+    <col min="17" max="17" width="18.140625" style="245" customWidth="1"/>
+    <col min="18" max="18" width="15.28515625" style="248" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="269"/>
-      <c r="C1" s="271" t="s">
+    <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B1" s="254"/>
+      <c r="C1" s="256" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="272"/>
-      <c r="E1" s="272"/>
-      <c r="F1" s="272"/>
-      <c r="G1" s="272"/>
-      <c r="H1" s="272"/>
-      <c r="I1" s="272"/>
-      <c r="J1" s="272"/>
-      <c r="K1" s="272"/>
-      <c r="L1" s="272"/>
-      <c r="M1" s="272"/>
-    </row>
-    <row r="2" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="270"/>
+      <c r="D1" s="257"/>
+      <c r="E1" s="257"/>
+      <c r="F1" s="257"/>
+      <c r="G1" s="257"/>
+      <c r="H1" s="257"/>
+      <c r="I1" s="257"/>
+      <c r="J1" s="257"/>
+      <c r="K1" s="257"/>
+      <c r="L1" s="257"/>
+      <c r="M1" s="257"/>
+    </row>
+    <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="255"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -8539,23 +8582,23 @@
       <c r="M2" s="6"/>
       <c r="N2" s="9"/>
     </row>
-    <row r="3" spans="1:19" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="273" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="274"/>
+    <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="258" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="259"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="275" t="s">
+      <c r="H3" s="260" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="275"/>
+      <c r="I3" s="260"/>
       <c r="K3" s="178"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
     </row>
-    <row r="4" spans="1:19" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
         <v>1</v>
       </c>
@@ -8566,14 +8609,14 @@
       <c r="D4" s="18">
         <v>44507</v>
       </c>
-      <c r="E4" s="276" t="s">
+      <c r="E4" s="261" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="277"/>
-      <c r="H4" s="278" t="s">
+      <c r="F4" s="262"/>
+      <c r="H4" s="263" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="279"/>
+      <c r="I4" s="264"/>
       <c r="J4" s="19"/>
       <c r="K4" s="179"/>
       <c r="L4" s="20"/>
@@ -8583,12 +8626,12 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="250" t="s">
+      <c r="P4" s="270" t="s">
         <v>6</v>
       </c>
-      <c r="Q4" s="251"/>
-    </row>
-    <row r="5" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q4" s="271"/>
+    </row>
+    <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
         <v>7</v>
       </c>
@@ -8632,9 +8675,12 @@
         <f>P5-F5</f>
         <v>-27936</v>
       </c>
-      <c r="R5" s="31"/>
-    </row>
-    <row r="6" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R5" s="250">
+        <f>20000+7936</f>
+        <v>27936</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="23"/>
       <c r="B6" s="24">
         <v>44509</v>
@@ -8676,10 +8722,13 @@
         <f>P6-F6</f>
         <v>-26378</v>
       </c>
-      <c r="R6" s="38"/>
+      <c r="R6" s="251">
+        <f>22000+4378</f>
+        <v>26378</v>
+      </c>
       <c r="S6" s="147"/>
     </row>
-    <row r="7" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="23"/>
       <c r="B7" s="24">
         <v>44510</v>
@@ -8719,10 +8768,13 @@
         <f t="shared" ref="Q7:Q38" si="1">P7-F7</f>
         <v>-30393</v>
       </c>
-      <c r="R7" s="38"/>
+      <c r="R7" s="251">
+        <f>26000+4393</f>
+        <v>30393</v>
+      </c>
       <c r="S7" s="147"/>
     </row>
-    <row r="8" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="23"/>
       <c r="B8" s="24">
         <v>44511</v>
@@ -8770,10 +8822,13 @@
         <f t="shared" si="1"/>
         <v>-20199</v>
       </c>
-      <c r="R8" s="38"/>
+      <c r="R8" s="251">
+        <f>20065+133</f>
+        <v>20198</v>
+      </c>
       <c r="S8" s="147"/>
     </row>
-    <row r="9" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="23"/>
       <c r="B9" s="24">
         <v>44512</v>
@@ -8821,10 +8876,13 @@
         <f t="shared" si="1"/>
         <v>-35678</v>
       </c>
-      <c r="R9" s="38"/>
+      <c r="R9" s="251">
+        <f>35678</f>
+        <v>35678</v>
+      </c>
       <c r="S9" s="147"/>
     </row>
-    <row r="10" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="23"/>
       <c r="B10" s="24">
         <v>44513</v>
@@ -8851,10 +8909,10 @@
       <c r="J10" s="37">
         <v>44513</v>
       </c>
-      <c r="K10" s="288" t="s">
+      <c r="K10" s="246" t="s">
         <v>109</v>
       </c>
-      <c r="L10" s="289">
+      <c r="L10" s="247">
         <v>13100</v>
       </c>
       <c r="M10" s="32">
@@ -8872,10 +8930,13 @@
         <f t="shared" si="1"/>
         <v>-30925</v>
       </c>
-      <c r="R10" s="38"/>
+      <c r="R10" s="251">
+        <f>30925</f>
+        <v>30925</v>
+      </c>
       <c r="S10" s="147"/>
     </row>
-    <row r="11" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="23"/>
       <c r="B11" s="24">
         <v>44514</v>
@@ -8915,10 +8976,13 @@
         <f t="shared" si="1"/>
         <v>-35238</v>
       </c>
-      <c r="R11" s="38"/>
+      <c r="R11" s="251">
+        <f>35238</f>
+        <v>35238</v>
+      </c>
       <c r="S11" s="147"/>
     </row>
-    <row r="12" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="23"/>
       <c r="B12" s="24">
         <v>44515</v>
@@ -8962,25 +9026,36 @@
         <f t="shared" si="1"/>
         <v>-29846</v>
       </c>
-      <c r="R12" s="38"/>
+      <c r="R12" s="251">
+        <f>29000+846</f>
+        <v>29846</v>
+      </c>
       <c r="S12" s="147"/>
     </row>
-    <row r="13" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="23"/>
       <c r="B13" s="24">
         <v>44516</v>
       </c>
-      <c r="C13" s="25"/>
-      <c r="D13" s="42"/>
+      <c r="C13" s="25">
+        <v>1739.36</v>
+      </c>
+      <c r="D13" s="42" t="s">
+        <v>112</v>
+      </c>
       <c r="E13" s="27">
         <v>44516</v>
       </c>
-      <c r="F13" s="28"/>
+      <c r="F13" s="28">
+        <v>65408</v>
+      </c>
       <c r="G13" s="2"/>
       <c r="H13" s="36">
         <v>44516</v>
       </c>
-      <c r="I13" s="30"/>
+      <c r="I13" s="30">
+        <v>1037</v>
+      </c>
       <c r="J13" s="37"/>
       <c r="K13" s="38"/>
       <c r="L13" s="39"/>
@@ -8988,36 +9063,51 @@
         <v>0</v>
       </c>
       <c r="N13" s="33">
-        <v>0</v>
+        <v>21106</v>
       </c>
       <c r="O13" s="2"/>
       <c r="P13" s="69">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>23882.36</v>
       </c>
       <c r="Q13" s="244">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R13" s="38"/>
-      <c r="S13" s="147"/>
-    </row>
-    <row r="14" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+        <v>-41525.64</v>
+      </c>
+      <c r="R13" s="251">
+        <f>41050+1147</f>
+        <v>42197</v>
+      </c>
+      <c r="S13" s="253" t="s">
+        <v>113</v>
+      </c>
+      <c r="T13" s="252"/>
+      <c r="U13" s="252"/>
+    </row>
+    <row r="14" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="23"/>
       <c r="B14" s="24">
         <v>44517</v>
       </c>
-      <c r="C14" s="25"/>
-      <c r="D14" s="40"/>
+      <c r="C14" s="25">
+        <v>6557.5</v>
+      </c>
+      <c r="D14" s="40" t="s">
+        <v>114</v>
+      </c>
       <c r="E14" s="27">
         <v>44517</v>
       </c>
-      <c r="F14" s="28"/>
+      <c r="F14" s="28">
+        <v>53925</v>
+      </c>
       <c r="G14" s="2"/>
       <c r="H14" s="36">
         <v>44517</v>
       </c>
-      <c r="I14" s="30"/>
+      <c r="I14" s="30">
+        <v>36</v>
+      </c>
       <c r="J14" s="37"/>
       <c r="K14" s="38"/>
       <c r="L14" s="39"/>
@@ -9025,36 +9115,46 @@
         <v>0</v>
       </c>
       <c r="N14" s="33">
-        <v>0</v>
+        <v>19362</v>
       </c>
       <c r="O14" s="2"/>
       <c r="P14" s="69">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>25955.5</v>
       </c>
       <c r="Q14" s="244">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R14" s="38"/>
+        <v>-27969.5</v>
+      </c>
+      <c r="R14" s="251">
+        <v>27970</v>
+      </c>
       <c r="S14" s="147"/>
     </row>
-    <row r="15" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="23"/>
       <c r="B15" s="24">
         <v>44518</v>
       </c>
-      <c r="C15" s="25"/>
-      <c r="D15" s="40"/>
+      <c r="C15" s="25">
+        <v>5383</v>
+      </c>
+      <c r="D15" s="40" t="s">
+        <v>115</v>
+      </c>
       <c r="E15" s="27">
         <v>44518</v>
       </c>
-      <c r="F15" s="28"/>
+      <c r="F15" s="28">
+        <v>47322</v>
+      </c>
       <c r="G15" s="2"/>
       <c r="H15" s="36">
         <v>44518</v>
       </c>
-      <c r="I15" s="30"/>
+      <c r="I15" s="30">
+        <v>369</v>
+      </c>
       <c r="J15" s="37"/>
       <c r="K15" s="38"/>
       <c r="L15" s="39"/>
@@ -9062,35 +9162,45 @@
         <v>0</v>
       </c>
       <c r="N15" s="33">
-        <v>0</v>
+        <v>8790</v>
       </c>
       <c r="P15" s="69">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>14542</v>
       </c>
       <c r="Q15" s="244">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R15" s="38"/>
+        <v>-32780</v>
+      </c>
+      <c r="R15" s="251">
+        <v>32780</v>
+      </c>
       <c r="S15" s="147"/>
     </row>
-    <row r="16" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="23"/>
       <c r="B16" s="24">
         <v>44519</v>
       </c>
-      <c r="C16" s="25"/>
-      <c r="D16" s="35"/>
+      <c r="C16" s="25">
+        <v>6078</v>
+      </c>
+      <c r="D16" s="35" t="s">
+        <v>116</v>
+      </c>
       <c r="E16" s="27">
         <v>44519</v>
       </c>
-      <c r="F16" s="28"/>
+      <c r="F16" s="28">
+        <v>58831</v>
+      </c>
       <c r="G16" s="2"/>
       <c r="H16" s="36">
         <v>44519</v>
       </c>
-      <c r="I16" s="30"/>
+      <c r="I16" s="30">
+        <v>82</v>
+      </c>
       <c r="J16" s="37"/>
       <c r="K16" s="182"/>
       <c r="L16" s="9"/>
@@ -9098,17 +9208,19 @@
         <v>0</v>
       </c>
       <c r="N16" s="33">
-        <v>0</v>
+        <v>15295</v>
       </c>
       <c r="P16" s="69">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>21455</v>
       </c>
       <c r="Q16" s="244">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R16" s="38"/>
+        <v>-37376</v>
+      </c>
+      <c r="R16" s="251">
+        <v>37376</v>
+      </c>
       <c r="S16" s="147"/>
     </row>
     <row r="17" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -9116,35 +9228,53 @@
       <c r="B17" s="24">
         <v>44520</v>
       </c>
-      <c r="C17" s="25"/>
-      <c r="D17" s="42"/>
+      <c r="C17" s="25">
+        <v>16886.12</v>
+      </c>
+      <c r="D17" s="42" t="s">
+        <v>117</v>
+      </c>
       <c r="E17" s="27">
         <v>44520</v>
       </c>
-      <c r="F17" s="28"/>
+      <c r="F17" s="28">
+        <v>59425</v>
+      </c>
       <c r="G17" s="2"/>
       <c r="H17" s="36">
         <v>44520</v>
       </c>
-      <c r="I17" s="30"/>
-      <c r="J17" s="37"/>
-      <c r="K17" s="38"/>
-      <c r="L17" s="45"/>
+      <c r="I17" s="30">
+        <v>0</v>
+      </c>
+      <c r="J17" s="37">
+        <v>44520</v>
+      </c>
+      <c r="K17" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="L17" s="45">
+        <f>12537.27+1285.71</f>
+        <v>13822.98</v>
+      </c>
       <c r="M17" s="32">
         <v>0</v>
       </c>
       <c r="N17" s="33">
-        <v>0</v>
+        <v>18910</v>
       </c>
       <c r="P17" s="69">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>49619.1</v>
       </c>
       <c r="Q17" s="244">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R17" s="38"/>
+        <v>-9805.9000000000015</v>
+      </c>
+      <c r="R17" s="251">
+        <f>9805.9+12537.27+1285.71</f>
+        <v>23628.879999999997</v>
+      </c>
       <c r="S17" s="147"/>
     </row>
     <row r="18" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -9152,17 +9282,23 @@
       <c r="B18" s="24">
         <v>44521</v>
       </c>
-      <c r="C18" s="25"/>
+      <c r="C18" s="25">
+        <v>0</v>
+      </c>
       <c r="D18" s="35"/>
       <c r="E18" s="27">
         <v>44521</v>
       </c>
-      <c r="F18" s="28"/>
+      <c r="F18" s="28">
+        <v>45176</v>
+      </c>
       <c r="G18" s="2"/>
       <c r="H18" s="36">
         <v>44521</v>
       </c>
-      <c r="I18" s="30"/>
+      <c r="I18" s="30">
+        <v>1515</v>
+      </c>
       <c r="J18" s="37"/>
       <c r="K18" s="183"/>
       <c r="L18" s="39"/>
@@ -9170,17 +9306,19 @@
         <v>0</v>
       </c>
       <c r="N18" s="33">
-        <v>0</v>
+        <v>21981</v>
       </c>
       <c r="P18" s="69">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23496</v>
       </c>
       <c r="Q18" s="244">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R18" s="38"/>
+        <v>-21680</v>
+      </c>
+      <c r="R18" s="251">
+        <v>21680</v>
+      </c>
       <c r="S18" s="147"/>
     </row>
     <row r="19" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -9188,17 +9326,25 @@
       <c r="B19" s="24">
         <v>44522</v>
       </c>
-      <c r="C19" s="25"/>
-      <c r="D19" s="35"/>
+      <c r="C19" s="25">
+        <v>2692</v>
+      </c>
+      <c r="D19" s="35" t="s">
+        <v>110</v>
+      </c>
       <c r="E19" s="27">
         <v>44522</v>
       </c>
-      <c r="F19" s="28"/>
+      <c r="F19" s="28">
+        <v>52088</v>
+      </c>
       <c r="G19" s="2"/>
       <c r="H19" s="36">
         <v>44522</v>
       </c>
-      <c r="I19" s="30"/>
+      <c r="I19" s="30">
+        <v>0</v>
+      </c>
       <c r="J19" s="37"/>
       <c r="K19" s="46"/>
       <c r="L19" s="47"/>
@@ -9206,17 +9352,19 @@
         <v>0</v>
       </c>
       <c r="N19" s="33">
-        <v>0</v>
+        <v>23026</v>
       </c>
       <c r="P19" s="69">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>25718</v>
       </c>
       <c r="Q19" s="244">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R19" s="38"/>
+        <v>-26370</v>
+      </c>
+      <c r="R19" s="251">
+        <v>26370</v>
+      </c>
       <c r="S19" s="147"/>
     </row>
     <row r="20" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -9224,17 +9372,25 @@
       <c r="B20" s="24">
         <v>44523</v>
       </c>
-      <c r="C20" s="25"/>
-      <c r="D20" s="35"/>
+      <c r="C20" s="25">
+        <v>6094.61</v>
+      </c>
+      <c r="D20" s="35" t="s">
+        <v>108</v>
+      </c>
       <c r="E20" s="27">
         <v>44523</v>
       </c>
-      <c r="F20" s="28"/>
+      <c r="F20" s="28">
+        <v>38542</v>
+      </c>
       <c r="G20" s="2"/>
       <c r="H20" s="36">
         <v>44523</v>
       </c>
-      <c r="I20" s="30"/>
+      <c r="I20" s="30">
+        <v>3668.56</v>
+      </c>
       <c r="J20" s="37"/>
       <c r="K20" s="184"/>
       <c r="L20" s="45"/>
@@ -9242,17 +9398,19 @@
         <v>0</v>
       </c>
       <c r="N20" s="33">
-        <v>0</v>
+        <v>12383</v>
       </c>
       <c r="P20" s="69">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>22146.17</v>
       </c>
       <c r="Q20" s="244">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R20" s="38"/>
+        <v>-16395.830000000002</v>
+      </c>
+      <c r="R20" s="251">
+        <v>16395.830000000002</v>
+      </c>
       <c r="S20" s="147"/>
     </row>
     <row r="21" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -9288,7 +9446,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R21" s="38"/>
+      <c r="R21" s="251"/>
       <c r="S21" s="147"/>
     </row>
     <row r="22" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -9324,7 +9482,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R22" s="38"/>
+      <c r="R22" s="251"/>
       <c r="S22" s="147"/>
     </row>
     <row r="23" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -9360,7 +9518,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R23" s="38"/>
+      <c r="R23" s="251"/>
       <c r="S23" s="147"/>
     </row>
     <row r="24" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -9396,7 +9554,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R24" s="38"/>
+      <c r="R24" s="251"/>
       <c r="S24" s="147"/>
     </row>
     <row r="25" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -9432,7 +9590,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R25" s="31"/>
+      <c r="R25" s="251"/>
     </row>
     <row r="26" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="23"/>
@@ -9467,7 +9625,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R26" s="31"/>
+      <c r="R26" s="251"/>
     </row>
     <row r="27" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="23"/>
@@ -9502,7 +9660,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R27" s="31"/>
+      <c r="R27" s="251"/>
     </row>
     <row r="28" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="23"/>
@@ -9537,7 +9695,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R28" s="31"/>
+      <c r="R28" s="251"/>
     </row>
     <row r="29" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="23"/>
@@ -9572,7 +9730,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R29" s="31"/>
+      <c r="R29" s="251"/>
     </row>
     <row r="30" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="23"/>
@@ -9607,7 +9765,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R30" s="31"/>
+      <c r="R30" s="251"/>
     </row>
     <row r="31" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="23"/>
@@ -9642,7 +9800,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R31" s="31"/>
+      <c r="R31" s="251"/>
     </row>
     <row r="32" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="23"/>
@@ -9677,7 +9835,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R32" s="31"/>
+      <c r="R32" s="249"/>
     </row>
     <row r="33" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="23"/>
@@ -9705,7 +9863,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R33" s="31"/>
+      <c r="R33" s="249"/>
     </row>
     <row r="34" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="23"/>
@@ -9739,7 +9897,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R34" s="31"/>
+      <c r="R34" s="249"/>
     </row>
     <row r="35" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="23"/>
@@ -9773,7 +9931,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R35" s="31"/>
+      <c r="R35" s="249"/>
     </row>
     <row r="36" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="23"/>
@@ -9803,7 +9961,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R36" s="31"/>
+      <c r="R36" s="249"/>
     </row>
     <row r="37" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="23"/>
@@ -9876,21 +10034,21 @@
       <c r="J39" s="60"/>
       <c r="K39" s="190"/>
       <c r="L39" s="61"/>
-      <c r="M39" s="252">
+      <c r="M39" s="272">
         <f>SUM(M5:M38)</f>
         <v>0</v>
       </c>
-      <c r="N39" s="254">
+      <c r="N39" s="274">
         <f>SUM(N5:N38)</f>
-        <v>101784</v>
+        <v>242637</v>
       </c>
       <c r="P39" s="34">
         <f>SUM(P5:P38)</f>
-        <v>157857</v>
+        <v>364671.12999999995</v>
       </c>
       <c r="Q39" s="234">
         <f>SUM(Q5:Q38)</f>
-        <v>-236593</v>
+        <v>-450495.87000000005</v>
       </c>
     </row>
     <row r="40" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -9906,8 +10064,8 @@
       <c r="J40" s="60"/>
       <c r="K40" s="41"/>
       <c r="L40" s="61"/>
-      <c r="M40" s="253"/>
-      <c r="N40" s="255"/>
+      <c r="M40" s="273"/>
+      <c r="N40" s="275"/>
       <c r="P40" s="34"/>
       <c r="Q40" s="13"/>
     </row>
@@ -10080,7 +10238,7 @@
       </c>
       <c r="C50" s="87">
         <f>SUM(C5:C49)</f>
-        <v>34178</v>
+        <v>79608.59</v>
       </c>
       <c r="D50" s="88"/>
       <c r="E50" s="89" t="s">
@@ -10088,7 +10246,7 @@
       </c>
       <c r="F50" s="90">
         <f>SUM(F5:F49)</f>
-        <v>394450</v>
+        <v>815167</v>
       </c>
       <c r="G50" s="88"/>
       <c r="H50" s="91" t="s">
@@ -10096,7 +10254,7 @@
       </c>
       <c r="I50" s="92">
         <f>SUM(I5:I49)</f>
-        <v>4850</v>
+        <v>11557.56</v>
       </c>
       <c r="J50" s="93"/>
       <c r="K50" s="94" t="s">
@@ -10104,7 +10262,7 @@
       </c>
       <c r="L50" s="95">
         <f>SUM(L5:L49)</f>
-        <v>17045</v>
+        <v>30867.98</v>
       </c>
       <c r="M50" s="96"/>
       <c r="N50" s="96"/>
@@ -10122,32 +10280,32 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="256" t="s">
+      <c r="H52" s="276" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="257"/>
+      <c r="I52" s="277"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="258">
+      <c r="K52" s="278">
         <f>I50+L50</f>
-        <v>21895</v>
-      </c>
-      <c r="L52" s="259"/>
-      <c r="M52" s="260">
+        <v>42425.54</v>
+      </c>
+      <c r="L52" s="279"/>
+      <c r="M52" s="280">
         <f>N39+M39</f>
-        <v>101784</v>
-      </c>
-      <c r="N52" s="261"/>
+        <v>242637</v>
+      </c>
+      <c r="N52" s="281"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D53" s="262" t="s">
+      <c r="D53" s="282" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="262"/>
+      <c r="E53" s="282"/>
       <c r="F53" s="101">
         <f>F50-K52-C50</f>
-        <v>338377</v>
+        <v>693132.87</v>
       </c>
       <c r="I53" s="102"/>
       <c r="J53" s="103"/>
@@ -10155,22 +10313,22 @@
       <c r="Q53" s="13"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="262" t="s">
+      <c r="D54" s="282" t="s">
         <v>101</v>
       </c>
-      <c r="E54" s="262"/>
+      <c r="E54" s="282"/>
       <c r="F54" s="96">
         <v>-549976.4</v>
       </c>
-      <c r="I54" s="263" t="s">
+      <c r="I54" s="283" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="264"/>
-      <c r="K54" s="265">
+      <c r="J54" s="284"/>
+      <c r="K54" s="285">
         <f>F56+F57+F58</f>
-        <v>-211599.40000000002</v>
-      </c>
-      <c r="L54" s="266"/>
+        <v>143156.46999999997</v>
+      </c>
+      <c r="L54" s="286"/>
       <c r="P54" s="34"/>
       <c r="Q54" s="13"/>
     </row>
@@ -10196,18 +10354,18 @@
       </c>
       <c r="F56" s="96">
         <f>SUM(F53:F55)</f>
-        <v>-211599.40000000002</v>
+        <v>143156.46999999997</v>
       </c>
       <c r="H56" s="23"/>
       <c r="I56" s="108" t="s">
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="267">
+      <c r="K56" s="287">
         <f>-C4</f>
         <v>-567389.35</v>
       </c>
-      <c r="L56" s="268"/>
+      <c r="L56" s="288"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -10222,22 +10380,22 @@
     </row>
     <row r="58" spans="1:17" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C58" s="112"/>
-      <c r="D58" s="245" t="s">
+      <c r="D58" s="265" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="246"/>
+      <c r="E58" s="266"/>
       <c r="F58" s="113">
         <v>0</v>
       </c>
-      <c r="I58" s="247" t="s">
+      <c r="I58" s="267" t="s">
         <v>103</v>
       </c>
-      <c r="J58" s="248"/>
-      <c r="K58" s="249">
+      <c r="J58" s="268"/>
+      <c r="K58" s="269">
         <f>K54+K56</f>
-        <v>-778988.75</v>
-      </c>
-      <c r="L58" s="249"/>
+        <v>-424232.88</v>
+      </c>
+      <c r="L58" s="269"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -10381,12 +10539,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="I58:J58"/>
     <mergeCell ref="K58:L58"/>
@@ -10401,6 +10553,12 @@
     <mergeCell ref="I54:J54"/>
     <mergeCell ref="K54:L54"/>
     <mergeCell ref="K56:L56"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -11263,7 +11421,7 @@
     </row>
     <row r="41" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="140"/>
-      <c r="B41" s="282"/>
+      <c r="B41" s="291"/>
       <c r="C41" s="237"/>
       <c r="D41" s="140"/>
       <c r="E41" s="69"/>
@@ -11283,7 +11441,7 @@
     </row>
     <row r="42" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="140"/>
-      <c r="B42" s="283"/>
+      <c r="B42" s="292"/>
       <c r="C42" s="69"/>
       <c r="D42" s="140"/>
       <c r="E42" s="69"/>
@@ -12807,12 +12965,12 @@
     <row r="42" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="43" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="155"/>
-      <c r="B43" s="284" t="s">
+      <c r="B43" s="293" t="s">
         <v>25</v>
       </c>
-      <c r="C43" s="285"/>
-      <c r="D43" s="285"/>
-      <c r="E43" s="286"/>
+      <c r="C43" s="294"/>
+      <c r="D43" s="294"/>
+      <c r="E43" s="295"/>
       <c r="F43" s="1"/>
     </row>
     <row r="44" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
CIERRE 3 DE DIC 2021
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 11  NOVIEMBRE 2021/BALANCE    ZAVALETA   NOVIEMBRE    2021.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 11  NOVIEMBRE 2021/BALANCE    ZAVALETA   NOVIEMBRE    2021.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ROUSS\Documents\GitHub\TRABAJO\01 DOCUEMENTOS\CENTRAL  ARCHIVO  2 0 2 1\CENTRAL # 11  NOVIEMBRE 2021\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rouss\Documents\GitHub\TRABAJO\01 DOCUEMENTOS\CENTRAL  ARCHIVO  2 0 2 1\CENTRAL # 11  NOVIEMBRE 2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF211F4B-8E43-44F5-A26B-F051CCD60190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14325" windowHeight="10620" activeTab="2"/>
+    <workbookView xWindow="4035" yWindow="0" windowWidth="16335" windowHeight="11070" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OCTUBRE      2 0 2 1     " sheetId="1" r:id="rId1"/>
@@ -20,22 +21,29 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId6"/>
     <sheet name="C AN C E L A C I O N E S      " sheetId="5" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>ROUSS</author>
   </authors>
   <commentList>
-    <comment ref="J23" authorId="0" shapeId="0">
+    <comment ref="J23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -59,7 +67,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J25" authorId="0" shapeId="0">
+    <comment ref="J25" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -88,12 +96,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>ROUSS</author>
   </authors>
   <commentList>
-    <comment ref="J23" authorId="0" shapeId="0">
+    <comment ref="J23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -117,7 +125,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J25" authorId="0" shapeId="0">
+    <comment ref="J25" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
@@ -146,7 +154,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="123">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -504,11 +512,23 @@
   <si>
     <t>NOMINA # 47</t>
   </si>
+  <si>
+    <t>POLLO</t>
+  </si>
+  <si>
+    <t>JAMON-CREMA-LENGUA-LACTEOS-POLLO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POLLO-QUESOS  </t>
+  </si>
+  <si>
+    <t>NOMINA # 48</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="6">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="[$-C0A]dd\-mmm\-yy;@"/>
@@ -2252,6 +2272,78 @@
     <xf numFmtId="44" fontId="19" fillId="13" borderId="50" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="6" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="6" borderId="51" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="6" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="50" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2283,78 +2375,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="6" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="6" borderId="51" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="6" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="50" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="43" fillId="6" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2424,7 +2444,7 @@
         <xdr:cNvPr id="2" name="2 Conector recto de flecha">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0F00-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2477,7 +2497,7 @@
         <xdr:cNvPr id="3" name="1 Conector recto de flecha">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0F00-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2530,7 +2550,7 @@
         <xdr:cNvPr id="4" name="2 Conector recto de flecha">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0F00-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2583,7 +2603,7 @@
         <xdr:cNvPr id="5" name="Conector recto de flecha 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0F00-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2636,7 +2656,7 @@
         <xdr:cNvPr id="6" name="Abrir llave 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0F00-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2692,7 +2712,7 @@
         <xdr:cNvPr id="7" name="Rectángulo 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0F00-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2792,7 +2812,7 @@
         <xdr:cNvPr id="8" name="Conector recto de flecha 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0F00-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2850,7 +2870,7 @@
         <xdr:cNvPr id="2" name="2 Conector recto de flecha">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0F00-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2903,7 +2923,7 @@
         <xdr:cNvPr id="3" name="1 Conector recto de flecha">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0F00-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2956,7 +2976,7 @@
         <xdr:cNvPr id="4" name="2 Conector recto de flecha">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0F00-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3009,7 +3029,7 @@
         <xdr:cNvPr id="5" name="Conector recto de flecha 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0F00-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3062,7 +3082,7 @@
         <xdr:cNvPr id="6" name="Abrir llave 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0F00-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3118,7 +3138,7 @@
         <xdr:cNvPr id="7" name="Rectángulo 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0F00-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3218,7 +3238,7 @@
         <xdr:cNvPr id="8" name="Conector recto de flecha 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0F00-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3518,7 +3538,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF800000"/>
   </sheetPr>
@@ -3550,23 +3570,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="254"/>
-      <c r="C1" s="256" t="s">
+      <c r="B1" s="278"/>
+      <c r="C1" s="280" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="257"/>
-      <c r="E1" s="257"/>
-      <c r="F1" s="257"/>
-      <c r="G1" s="257"/>
-      <c r="H1" s="257"/>
-      <c r="I1" s="257"/>
-      <c r="J1" s="257"/>
-      <c r="K1" s="257"/>
-      <c r="L1" s="257"/>
-      <c r="M1" s="257"/>
+      <c r="D1" s="281"/>
+      <c r="E1" s="281"/>
+      <c r="F1" s="281"/>
+      <c r="G1" s="281"/>
+      <c r="H1" s="281"/>
+      <c r="I1" s="281"/>
+      <c r="J1" s="281"/>
+      <c r="K1" s="281"/>
+      <c r="L1" s="281"/>
+      <c r="M1" s="281"/>
     </row>
     <row r="2" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="255"/>
+      <c r="B2" s="279"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -3576,17 +3596,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:19" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="258" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="259"/>
+      <c r="B3" s="282" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="283"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="260" t="s">
+      <c r="H3" s="284" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="260"/>
+      <c r="I3" s="284"/>
       <c r="K3" s="178"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
@@ -3600,14 +3620,14 @@
         <v>0</v>
       </c>
       <c r="D4" s="18"/>
-      <c r="E4" s="261" t="s">
+      <c r="E4" s="285" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="262"/>
-      <c r="H4" s="263" t="s">
+      <c r="F4" s="286"/>
+      <c r="H4" s="287" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="264"/>
+      <c r="I4" s="288"/>
       <c r="J4" s="19"/>
       <c r="K4" s="179"/>
       <c r="L4" s="20"/>
@@ -3617,10 +3637,10 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="270" t="s">
+      <c r="P4" s="259" t="s">
         <v>6</v>
       </c>
-      <c r="Q4" s="271"/>
+      <c r="Q4" s="260"/>
     </row>
     <row r="5" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
@@ -5061,11 +5081,11 @@
       <c r="J39" s="60"/>
       <c r="K39" s="190"/>
       <c r="L39" s="61"/>
-      <c r="M39" s="272">
+      <c r="M39" s="261">
         <f>SUM(M5:M38)</f>
         <v>247061</v>
       </c>
-      <c r="N39" s="274">
+      <c r="N39" s="263">
         <f>SUM(N5:N38)</f>
         <v>172863</v>
       </c>
@@ -5091,8 +5111,8 @@
       <c r="J40" s="60"/>
       <c r="K40" s="41"/>
       <c r="L40" s="61"/>
-      <c r="M40" s="273"/>
-      <c r="N40" s="275"/>
+      <c r="M40" s="262"/>
+      <c r="N40" s="264"/>
       <c r="P40" s="34"/>
       <c r="Q40" s="9"/>
     </row>
@@ -5307,29 +5327,29 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="276" t="s">
+      <c r="H52" s="265" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="277"/>
+      <c r="I52" s="266"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="278">
+      <c r="K52" s="267">
         <f>I50+L50</f>
         <v>53873.49</v>
       </c>
-      <c r="L52" s="279"/>
-      <c r="M52" s="280">
+      <c r="L52" s="268"/>
+      <c r="M52" s="269">
         <f>N39+M39</f>
         <v>419924</v>
       </c>
-      <c r="N52" s="281"/>
+      <c r="N52" s="270"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D53" s="282" t="s">
+      <c r="D53" s="271" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="282"/>
+      <c r="E53" s="271"/>
       <c r="F53" s="101">
         <f>F50-K52-C50</f>
         <v>471038.61</v>
@@ -5340,22 +5360,22 @@
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="282" t="s">
+      <c r="D54" s="271" t="s">
         <v>101</v>
       </c>
-      <c r="E54" s="282"/>
+      <c r="E54" s="271"/>
       <c r="F54" s="96">
         <v>-549976.4</v>
       </c>
-      <c r="I54" s="283" t="s">
+      <c r="I54" s="272" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="284"/>
-      <c r="K54" s="285">
+      <c r="J54" s="273"/>
+      <c r="K54" s="274">
         <f>F56+F57+F58</f>
         <v>-24577.400000000023</v>
       </c>
-      <c r="L54" s="286"/>
+      <c r="L54" s="275"/>
       <c r="P54" s="34"/>
       <c r="Q54" s="9"/>
     </row>
@@ -5388,11 +5408,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="287">
+      <c r="K56" s="276">
         <f>-C4</f>
         <v>0</v>
       </c>
-      <c r="L56" s="288"/>
+      <c r="L56" s="277"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -5409,22 +5429,22 @@
       <c r="C58" s="112">
         <v>44507</v>
       </c>
-      <c r="D58" s="265" t="s">
+      <c r="D58" s="254" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="266"/>
+      <c r="E58" s="255"/>
       <c r="F58" s="113">
         <v>567389.35</v>
       </c>
-      <c r="I58" s="267" t="s">
+      <c r="I58" s="256" t="s">
         <v>103</v>
       </c>
-      <c r="J58" s="268"/>
-      <c r="K58" s="269">
+      <c r="J58" s="257"/>
+      <c r="K58" s="258">
         <f>K54+K56</f>
         <v>-24577.400000000023</v>
       </c>
-      <c r="L58" s="269"/>
+      <c r="L58" s="258"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -5568,6 +5588,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="I58:J58"/>
     <mergeCell ref="K58:L58"/>
@@ -5582,12 +5608,6 @@
     <mergeCell ref="I54:J54"/>
     <mergeCell ref="K54:L54"/>
     <mergeCell ref="K56:L56"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.15748031496062992" top="0.35433070866141736" bottom="0.31496062992125984" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="75" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -5597,7 +5617,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FF800000"/>
   </sheetPr>
@@ -8525,14 +8545,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FF002060"/>
   </sheetPr>
   <dimension ref="A1:U80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G9" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView tabSelected="1" topLeftCell="I10" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -8557,23 +8577,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="254"/>
-      <c r="C1" s="256" t="s">
+      <c r="B1" s="278"/>
+      <c r="C1" s="280" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="257"/>
-      <c r="E1" s="257"/>
-      <c r="F1" s="257"/>
-      <c r="G1" s="257"/>
-      <c r="H1" s="257"/>
-      <c r="I1" s="257"/>
-      <c r="J1" s="257"/>
-      <c r="K1" s="257"/>
-      <c r="L1" s="257"/>
-      <c r="M1" s="257"/>
+      <c r="D1" s="281"/>
+      <c r="E1" s="281"/>
+      <c r="F1" s="281"/>
+      <c r="G1" s="281"/>
+      <c r="H1" s="281"/>
+      <c r="I1" s="281"/>
+      <c r="J1" s="281"/>
+      <c r="K1" s="281"/>
+      <c r="L1" s="281"/>
+      <c r="M1" s="281"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="255"/>
+      <c r="B2" s="279"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -8583,17 +8603,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="258" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="259"/>
+      <c r="B3" s="282" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="283"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="260" t="s">
+      <c r="H3" s="284" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="260"/>
+      <c r="I3" s="284"/>
       <c r="K3" s="178"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
@@ -8609,14 +8629,14 @@
       <c r="D4" s="18">
         <v>44507</v>
       </c>
-      <c r="E4" s="261" t="s">
+      <c r="E4" s="285" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="262"/>
-      <c r="H4" s="263" t="s">
+      <c r="F4" s="286"/>
+      <c r="H4" s="287" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="264"/>
+      <c r="I4" s="288"/>
       <c r="J4" s="19"/>
       <c r="K4" s="179"/>
       <c r="L4" s="20"/>
@@ -8626,10 +8646,10 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="270" t="s">
+      <c r="P4" s="259" t="s">
         <v>6</v>
       </c>
-      <c r="Q4" s="271"/>
+      <c r="Q4" s="260"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
@@ -9418,17 +9438,25 @@
       <c r="B21" s="24">
         <v>44524</v>
       </c>
-      <c r="C21" s="25"/>
-      <c r="D21" s="35"/>
+      <c r="C21" s="25">
+        <v>2763.18</v>
+      </c>
+      <c r="D21" s="35" t="s">
+        <v>119</v>
+      </c>
       <c r="E21" s="27">
         <v>44524</v>
       </c>
-      <c r="F21" s="28"/>
+      <c r="F21" s="28">
+        <v>34933</v>
+      </c>
       <c r="G21" s="2"/>
       <c r="H21" s="36">
         <v>44524</v>
       </c>
-      <c r="I21" s="30"/>
+      <c r="I21" s="30">
+        <v>3972</v>
+      </c>
       <c r="J21" s="37"/>
       <c r="K21" s="48"/>
       <c r="L21" s="45"/>
@@ -9436,17 +9464,19 @@
         <v>0</v>
       </c>
       <c r="N21" s="33">
-        <v>0</v>
+        <v>9009</v>
       </c>
       <c r="P21" s="69">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>15744.18</v>
       </c>
       <c r="Q21" s="244">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R21" s="251"/>
+        <v>-19188.82</v>
+      </c>
+      <c r="R21" s="251">
+        <v>19188.82</v>
+      </c>
       <c r="S21" s="147"/>
     </row>
     <row r="22" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -9454,17 +9484,26 @@
       <c r="B22" s="24">
         <v>44525</v>
       </c>
-      <c r="C22" s="25"/>
-      <c r="D22" s="35"/>
+      <c r="C22" s="25">
+        <f>3851.5+2501.78</f>
+        <v>6353.2800000000007</v>
+      </c>
+      <c r="D22" s="35" t="s">
+        <v>120</v>
+      </c>
       <c r="E22" s="27">
         <v>44525</v>
       </c>
-      <c r="F22" s="28"/>
+      <c r="F22" s="28">
+        <v>56996</v>
+      </c>
       <c r="G22" s="2"/>
       <c r="H22" s="36">
         <v>44525</v>
       </c>
-      <c r="I22" s="30"/>
+      <c r="I22" s="30">
+        <v>0</v>
+      </c>
       <c r="J22" s="37"/>
       <c r="K22" s="31"/>
       <c r="L22" s="49"/>
@@ -9472,17 +9511,19 @@
         <v>0</v>
       </c>
       <c r="N22" s="33">
-        <v>0</v>
+        <v>16995</v>
       </c>
       <c r="P22" s="69">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23348.28</v>
       </c>
       <c r="Q22" s="244">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R22" s="251"/>
+        <v>-33647.72</v>
+      </c>
+      <c r="R22" s="251">
+        <v>33647.72</v>
+      </c>
       <c r="S22" s="147"/>
     </row>
     <row r="23" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -9490,17 +9531,26 @@
       <c r="B23" s="24">
         <v>44526</v>
       </c>
-      <c r="C23" s="25"/>
-      <c r="D23" s="35"/>
+      <c r="C23" s="25">
+        <f>2453+1253.71</f>
+        <v>3706.71</v>
+      </c>
+      <c r="D23" s="35" t="s">
+        <v>121</v>
+      </c>
       <c r="E23" s="27">
         <v>44526</v>
       </c>
-      <c r="F23" s="28"/>
+      <c r="F23" s="28">
+        <v>76926</v>
+      </c>
       <c r="G23" s="2"/>
       <c r="H23" s="36">
         <v>44526</v>
       </c>
-      <c r="I23" s="30"/>
+      <c r="I23" s="30">
+        <v>43</v>
+      </c>
       <c r="J23" s="50"/>
       <c r="K23" s="185"/>
       <c r="L23" s="45"/>
@@ -9508,17 +9558,19 @@
         <v>0</v>
       </c>
       <c r="N23" s="33">
-        <v>0</v>
+        <v>27959</v>
       </c>
       <c r="P23" s="69">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>31708.71</v>
       </c>
       <c r="Q23" s="244">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R23" s="251"/>
+        <v>-45217.29</v>
+      </c>
+      <c r="R23" s="251">
+        <v>45217.29</v>
+      </c>
       <c r="S23" s="147"/>
     </row>
     <row r="24" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -9526,35 +9578,51 @@
       <c r="B24" s="24">
         <v>44527</v>
       </c>
-      <c r="C24" s="25"/>
-      <c r="D24" s="35"/>
+      <c r="C24" s="25">
+        <v>7071</v>
+      </c>
+      <c r="D24" s="35" t="s">
+        <v>108</v>
+      </c>
       <c r="E24" s="27">
         <v>44527</v>
       </c>
-      <c r="F24" s="28"/>
+      <c r="F24" s="28">
+        <v>65252</v>
+      </c>
       <c r="G24" s="2"/>
       <c r="H24" s="36">
         <v>44527</v>
       </c>
-      <c r="I24" s="30"/>
-      <c r="J24" s="51"/>
-      <c r="K24" s="186"/>
-      <c r="L24" s="52"/>
+      <c r="I24" s="30">
+        <v>72</v>
+      </c>
+      <c r="J24" s="51">
+        <v>44527</v>
+      </c>
+      <c r="K24" s="186" t="s">
+        <v>122</v>
+      </c>
+      <c r="L24" s="52">
+        <v>9944.83</v>
+      </c>
       <c r="M24" s="32">
         <v>0</v>
       </c>
       <c r="N24" s="33">
-        <v>0</v>
+        <v>25005</v>
       </c>
       <c r="P24" s="69">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>42092.83</v>
       </c>
       <c r="Q24" s="244">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R24" s="251"/>
+        <v>-23159.17</v>
+      </c>
+      <c r="R24" s="251">
+        <v>23159.17</v>
+      </c>
       <c r="S24" s="147"/>
     </row>
     <row r="25" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -9562,17 +9630,23 @@
       <c r="B25" s="24">
         <v>44528</v>
       </c>
-      <c r="C25" s="25"/>
+      <c r="C25" s="25">
+        <v>0</v>
+      </c>
       <c r="D25" s="35"/>
       <c r="E25" s="27">
         <v>44528</v>
       </c>
-      <c r="F25" s="28"/>
+      <c r="F25" s="28">
+        <v>39533</v>
+      </c>
       <c r="G25" s="2"/>
       <c r="H25" s="36">
         <v>44528</v>
       </c>
-      <c r="I25" s="30"/>
+      <c r="I25" s="30">
+        <v>400</v>
+      </c>
       <c r="J25" s="53"/>
       <c r="K25" s="38"/>
       <c r="L25" s="54"/>
@@ -9580,17 +9654,19 @@
         <v>0</v>
       </c>
       <c r="N25" s="33">
-        <v>0</v>
+        <v>10181</v>
       </c>
       <c r="P25" s="232">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10581</v>
       </c>
       <c r="Q25" s="244">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R25" s="251"/>
+        <v>-28952</v>
+      </c>
+      <c r="R25" s="251">
+        <v>28952</v>
+      </c>
     </row>
     <row r="26" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="23"/>
@@ -10034,21 +10110,21 @@
       <c r="J39" s="60"/>
       <c r="K39" s="190"/>
       <c r="L39" s="61"/>
-      <c r="M39" s="272">
+      <c r="M39" s="261">
         <f>SUM(M5:M38)</f>
         <v>0</v>
       </c>
-      <c r="N39" s="274">
+      <c r="N39" s="263">
         <f>SUM(N5:N38)</f>
-        <v>242637</v>
+        <v>331786</v>
       </c>
       <c r="P39" s="34">
         <f>SUM(P5:P38)</f>
-        <v>364671.12999999995</v>
+        <v>488146.13</v>
       </c>
       <c r="Q39" s="234">
         <f>SUM(Q5:Q38)</f>
-        <v>-450495.87000000005</v>
+        <v>-600660.87000000011</v>
       </c>
     </row>
     <row r="40" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -10064,8 +10140,8 @@
       <c r="J40" s="60"/>
       <c r="K40" s="41"/>
       <c r="L40" s="61"/>
-      <c r="M40" s="273"/>
-      <c r="N40" s="275"/>
+      <c r="M40" s="262"/>
+      <c r="N40" s="264"/>
       <c r="P40" s="34"/>
       <c r="Q40" s="13"/>
     </row>
@@ -10238,7 +10314,7 @@
       </c>
       <c r="C50" s="87">
         <f>SUM(C5:C49)</f>
-        <v>79608.59</v>
+        <v>99502.76</v>
       </c>
       <c r="D50" s="88"/>
       <c r="E50" s="89" t="s">
@@ -10246,7 +10322,7 @@
       </c>
       <c r="F50" s="90">
         <f>SUM(F5:F49)</f>
-        <v>815167</v>
+        <v>1088807</v>
       </c>
       <c r="G50" s="88"/>
       <c r="H50" s="91" t="s">
@@ -10254,7 +10330,7 @@
       </c>
       <c r="I50" s="92">
         <f>SUM(I5:I49)</f>
-        <v>11557.56</v>
+        <v>16044.56</v>
       </c>
       <c r="J50" s="93"/>
       <c r="K50" s="94" t="s">
@@ -10262,7 +10338,7 @@
       </c>
       <c r="L50" s="95">
         <f>SUM(L5:L49)</f>
-        <v>30867.98</v>
+        <v>40812.81</v>
       </c>
       <c r="M50" s="96"/>
       <c r="N50" s="96"/>
@@ -10280,32 +10356,32 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="276" t="s">
+      <c r="H52" s="265" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="277"/>
+      <c r="I52" s="266"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="278">
+      <c r="K52" s="267">
         <f>I50+L50</f>
-        <v>42425.54</v>
-      </c>
-      <c r="L52" s="279"/>
-      <c r="M52" s="280">
+        <v>56857.369999999995</v>
+      </c>
+      <c r="L52" s="268"/>
+      <c r="M52" s="269">
         <f>N39+M39</f>
-        <v>242637</v>
-      </c>
-      <c r="N52" s="281"/>
+        <v>331786</v>
+      </c>
+      <c r="N52" s="270"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D53" s="282" t="s">
+      <c r="D53" s="271" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="282"/>
+      <c r="E53" s="271"/>
       <c r="F53" s="101">
         <f>F50-K52-C50</f>
-        <v>693132.87</v>
+        <v>932446.87</v>
       </c>
       <c r="I53" s="102"/>
       <c r="J53" s="103"/>
@@ -10313,22 +10389,22 @@
       <c r="Q53" s="13"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="282" t="s">
+      <c r="D54" s="271" t="s">
         <v>101</v>
       </c>
-      <c r="E54" s="282"/>
+      <c r="E54" s="271"/>
       <c r="F54" s="96">
         <v>-549976.4</v>
       </c>
-      <c r="I54" s="283" t="s">
+      <c r="I54" s="272" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="284"/>
-      <c r="K54" s="285">
+      <c r="J54" s="273"/>
+      <c r="K54" s="274">
         <f>F56+F57+F58</f>
-        <v>143156.46999999997</v>
-      </c>
-      <c r="L54" s="286"/>
+        <v>382470.47</v>
+      </c>
+      <c r="L54" s="275"/>
       <c r="P54" s="34"/>
       <c r="Q54" s="13"/>
     </row>
@@ -10354,18 +10430,18 @@
       </c>
       <c r="F56" s="96">
         <f>SUM(F53:F55)</f>
-        <v>143156.46999999997</v>
+        <v>382470.47</v>
       </c>
       <c r="H56" s="23"/>
       <c r="I56" s="108" t="s">
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="287">
+      <c r="K56" s="276">
         <f>-C4</f>
         <v>-567389.35</v>
       </c>
-      <c r="L56" s="288"/>
+      <c r="L56" s="277"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -10380,22 +10456,22 @@
     </row>
     <row r="58" spans="1:17" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C58" s="112"/>
-      <c r="D58" s="265" t="s">
+      <c r="D58" s="254" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="266"/>
+      <c r="E58" s="255"/>
       <c r="F58" s="113">
         <v>0</v>
       </c>
-      <c r="I58" s="267" t="s">
+      <c r="I58" s="256" t="s">
         <v>103</v>
       </c>
-      <c r="J58" s="268"/>
-      <c r="K58" s="269">
+      <c r="J58" s="257"/>
+      <c r="K58" s="258">
         <f>K54+K56</f>
-        <v>-424232.88</v>
-      </c>
-      <c r="L58" s="269"/>
+        <v>-184918.88</v>
+      </c>
+      <c r="L58" s="258"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -10539,6 +10615,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="I58:J58"/>
     <mergeCell ref="K58:L58"/>
@@ -10553,12 +10635,6 @@
     <mergeCell ref="I54:J54"/>
     <mergeCell ref="K54:L54"/>
     <mergeCell ref="K56:L56"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -10568,7 +10644,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor rgb="FF002060"/>
   </sheetPr>
@@ -12912,7 +12988,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -12924,7 +13000,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -12936,7 +13012,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor rgb="FF800000"/>
   </sheetPr>

</xml_diff>

<commit_message>
CIERRE DE 6 DE DIC 2021
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 11  NOVIEMBRE 2021/BALANCE    ZAVALETA   NOVIEMBRE    2021.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 11  NOVIEMBRE 2021/BALANCE    ZAVALETA   NOVIEMBRE    2021.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4035" yWindow="0" windowWidth="16335" windowHeight="11070" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="4035" yWindow="0" windowWidth="16335" windowHeight="11070" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="OCTUBRE      2 0 2 1     " sheetId="1" r:id="rId1"/>
@@ -153,7 +153,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="127">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -522,6 +522,18 @@
   </si>
   <si>
     <t>NOMINA # 48</t>
+  </si>
+  <si>
+    <t>POLLO--QUESO-SALCHICHA</t>
+  </si>
+  <si>
+    <t>POLLO-LONGANIZA</t>
+  </si>
+  <si>
+    <t>JAMON-POLLO</t>
+  </si>
+  <si>
+    <t>SANCHICHAS-POLLO-LONGANIZA-LENGUA</t>
   </si>
 </sst>
 </file>
@@ -2280,6 +2292,78 @@
     <xf numFmtId="44" fontId="2" fillId="12" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="6" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="6" borderId="51" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="6" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="50" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2311,78 +2395,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="6" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="6" borderId="51" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="6" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="50" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="43" fillId="6" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3578,23 +3590,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="257"/>
-      <c r="C1" s="259" t="s">
+      <c r="B1" s="281"/>
+      <c r="C1" s="283" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="260"/>
-      <c r="E1" s="260"/>
-      <c r="F1" s="260"/>
-      <c r="G1" s="260"/>
-      <c r="H1" s="260"/>
-      <c r="I1" s="260"/>
-      <c r="J1" s="260"/>
-      <c r="K1" s="260"/>
-      <c r="L1" s="260"/>
-      <c r="M1" s="260"/>
+      <c r="D1" s="284"/>
+      <c r="E1" s="284"/>
+      <c r="F1" s="284"/>
+      <c r="G1" s="284"/>
+      <c r="H1" s="284"/>
+      <c r="I1" s="284"/>
+      <c r="J1" s="284"/>
+      <c r="K1" s="284"/>
+      <c r="L1" s="284"/>
+      <c r="M1" s="284"/>
     </row>
     <row r="2" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="258"/>
+      <c r="B2" s="282"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -3604,17 +3616,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:19" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="261" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="262"/>
+      <c r="B3" s="285" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="286"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="263" t="s">
+      <c r="H3" s="287" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="263"/>
+      <c r="I3" s="287"/>
       <c r="K3" s="178"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
@@ -3628,14 +3640,14 @@
         <v>0</v>
       </c>
       <c r="D4" s="18"/>
-      <c r="E4" s="264" t="s">
+      <c r="E4" s="288" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="265"/>
-      <c r="H4" s="266" t="s">
+      <c r="F4" s="289"/>
+      <c r="H4" s="290" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="267"/>
+      <c r="I4" s="291"/>
       <c r="J4" s="19"/>
       <c r="K4" s="179"/>
       <c r="L4" s="20"/>
@@ -3645,10 +3657,10 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="273" t="s">
+      <c r="P4" s="262" t="s">
         <v>6</v>
       </c>
-      <c r="Q4" s="274"/>
+      <c r="Q4" s="263"/>
     </row>
     <row r="5" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
@@ -5089,11 +5101,11 @@
       <c r="J39" s="60"/>
       <c r="K39" s="190"/>
       <c r="L39" s="61"/>
-      <c r="M39" s="275">
+      <c r="M39" s="264">
         <f>SUM(M5:M38)</f>
         <v>247061</v>
       </c>
-      <c r="N39" s="277">
+      <c r="N39" s="266">
         <f>SUM(N5:N38)</f>
         <v>172863</v>
       </c>
@@ -5119,8 +5131,8 @@
       <c r="J40" s="60"/>
       <c r="K40" s="41"/>
       <c r="L40" s="61"/>
-      <c r="M40" s="276"/>
-      <c r="N40" s="278"/>
+      <c r="M40" s="265"/>
+      <c r="N40" s="267"/>
       <c r="P40" s="34"/>
       <c r="Q40" s="9"/>
     </row>
@@ -5335,29 +5347,29 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="279" t="s">
+      <c r="H52" s="268" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="280"/>
+      <c r="I52" s="269"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="281">
+      <c r="K52" s="270">
         <f>I50+L50</f>
         <v>53873.49</v>
       </c>
-      <c r="L52" s="282"/>
-      <c r="M52" s="283">
+      <c r="L52" s="271"/>
+      <c r="M52" s="272">
         <f>N39+M39</f>
         <v>419924</v>
       </c>
-      <c r="N52" s="284"/>
+      <c r="N52" s="273"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D53" s="285" t="s">
+      <c r="D53" s="274" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="285"/>
+      <c r="E53" s="274"/>
       <c r="F53" s="101">
         <f>F50-K52-C50</f>
         <v>471038.61</v>
@@ -5368,22 +5380,22 @@
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="285" t="s">
+      <c r="D54" s="274" t="s">
         <v>101</v>
       </c>
-      <c r="E54" s="285"/>
+      <c r="E54" s="274"/>
       <c r="F54" s="96">
         <v>-549976.4</v>
       </c>
-      <c r="I54" s="286" t="s">
+      <c r="I54" s="275" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="287"/>
-      <c r="K54" s="288">
+      <c r="J54" s="276"/>
+      <c r="K54" s="277">
         <f>F56+F57+F58</f>
         <v>-24577.400000000023</v>
       </c>
-      <c r="L54" s="289"/>
+      <c r="L54" s="278"/>
       <c r="P54" s="34"/>
       <c r="Q54" s="9"/>
     </row>
@@ -5416,11 +5428,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="290">
+      <c r="K56" s="279">
         <f>-C4</f>
         <v>0</v>
       </c>
-      <c r="L56" s="291"/>
+      <c r="L56" s="280"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -5437,22 +5449,22 @@
       <c r="C58" s="112">
         <v>44507</v>
       </c>
-      <c r="D58" s="268" t="s">
+      <c r="D58" s="257" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="269"/>
+      <c r="E58" s="258"/>
       <c r="F58" s="113">
         <v>567389.35</v>
       </c>
-      <c r="I58" s="270" t="s">
+      <c r="I58" s="259" t="s">
         <v>103</v>
       </c>
-      <c r="J58" s="271"/>
-      <c r="K58" s="272">
+      <c r="J58" s="260"/>
+      <c r="K58" s="261">
         <f>K54+K56</f>
         <v>-24577.400000000023</v>
       </c>
-      <c r="L58" s="272"/>
+      <c r="L58" s="261"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -5596,6 +5608,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="I58:J58"/>
     <mergeCell ref="K58:L58"/>
@@ -5610,12 +5628,6 @@
     <mergeCell ref="I54:J54"/>
     <mergeCell ref="K54:L54"/>
     <mergeCell ref="K56:L56"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.15748031496062992" top="0.35433070866141736" bottom="0.31496062992125984" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="75" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -8559,8 +8571,8 @@
   </sheetPr>
   <dimension ref="A1:U80"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" topLeftCell="C16" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -8585,23 +8597,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="257"/>
-      <c r="C1" s="259" t="s">
+      <c r="B1" s="281"/>
+      <c r="C1" s="283" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="260"/>
-      <c r="E1" s="260"/>
-      <c r="F1" s="260"/>
-      <c r="G1" s="260"/>
-      <c r="H1" s="260"/>
-      <c r="I1" s="260"/>
-      <c r="J1" s="260"/>
-      <c r="K1" s="260"/>
-      <c r="L1" s="260"/>
-      <c r="M1" s="260"/>
+      <c r="D1" s="284"/>
+      <c r="E1" s="284"/>
+      <c r="F1" s="284"/>
+      <c r="G1" s="284"/>
+      <c r="H1" s="284"/>
+      <c r="I1" s="284"/>
+      <c r="J1" s="284"/>
+      <c r="K1" s="284"/>
+      <c r="L1" s="284"/>
+      <c r="M1" s="284"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="258"/>
+      <c r="B2" s="282"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -8611,17 +8623,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="261" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="262"/>
+      <c r="B3" s="285" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="286"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="263" t="s">
+      <c r="H3" s="287" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="263"/>
+      <c r="I3" s="287"/>
       <c r="K3" s="178"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
@@ -8637,14 +8649,14 @@
       <c r="D4" s="18">
         <v>44507</v>
       </c>
-      <c r="E4" s="264" t="s">
+      <c r="E4" s="288" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="265"/>
-      <c r="H4" s="266" t="s">
+      <c r="F4" s="289"/>
+      <c r="H4" s="290" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="267"/>
+      <c r="I4" s="291"/>
       <c r="J4" s="19"/>
       <c r="K4" s="179"/>
       <c r="L4" s="20"/>
@@ -8654,10 +8666,10 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="273" t="s">
+      <c r="P4" s="262" t="s">
         <v>6</v>
       </c>
-      <c r="Q4" s="274"/>
+      <c r="Q4" s="263"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
@@ -9681,52 +9693,70 @@
       <c r="B26" s="24">
         <v>44529</v>
       </c>
-      <c r="C26" s="25"/>
-      <c r="D26" s="35"/>
+      <c r="C26" s="25">
+        <v>5142.5</v>
+      </c>
+      <c r="D26" s="35" t="s">
+        <v>123</v>
+      </c>
       <c r="E26" s="27">
         <v>44529</v>
       </c>
-      <c r="F26" s="28"/>
+      <c r="F26" s="28">
+        <v>51711</v>
+      </c>
       <c r="G26" s="2"/>
       <c r="H26" s="36">
-        <v>44529</v>
-      </c>
-      <c r="I26" s="30"/>
+        <v>1840</v>
+      </c>
+      <c r="I26" s="30">
+        <v>1840</v>
+      </c>
       <c r="J26" s="37"/>
       <c r="K26" s="186"/>
       <c r="L26" s="45"/>
-      <c r="M26" s="32">
-        <v>0</v>
+      <c r="M26" s="195">
+        <v>6336</v>
       </c>
       <c r="N26" s="33">
-        <v>0</v>
+        <v>16621</v>
       </c>
       <c r="P26" s="231">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>29939.5</v>
       </c>
       <c r="Q26" s="244">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R26" s="251"/>
+        <v>-21771.5</v>
+      </c>
+      <c r="R26" s="251">
+        <v>21771.5</v>
+      </c>
     </row>
     <row r="27" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="23"/>
       <c r="B27" s="24">
         <v>44530</v>
       </c>
-      <c r="C27" s="25"/>
-      <c r="D27" s="42"/>
+      <c r="C27" s="25">
+        <v>8184</v>
+      </c>
+      <c r="D27" s="42" t="s">
+        <v>124</v>
+      </c>
       <c r="E27" s="27">
         <v>44530</v>
       </c>
-      <c r="F27" s="28"/>
+      <c r="F27" s="28">
+        <v>31060</v>
+      </c>
       <c r="G27" s="2"/>
       <c r="H27" s="36">
         <v>44530</v>
       </c>
-      <c r="I27" s="30"/>
+      <c r="I27" s="30">
+        <v>660</v>
+      </c>
       <c r="J27" s="55"/>
       <c r="K27" s="187"/>
       <c r="L27" s="54"/>
@@ -9734,34 +9764,44 @@
         <v>0</v>
       </c>
       <c r="N27" s="33">
-        <v>0</v>
+        <v>7579</v>
       </c>
       <c r="P27" s="69">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>16423</v>
       </c>
       <c r="Q27" s="244">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R27" s="251"/>
+        <v>-14637</v>
+      </c>
+      <c r="R27" s="251">
+        <v>14637</v>
+      </c>
     </row>
     <row r="28" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="23"/>
       <c r="B28" s="24">
         <v>44531</v>
       </c>
-      <c r="C28" s="25"/>
-      <c r="D28" s="42"/>
+      <c r="C28" s="25">
+        <v>7763</v>
+      </c>
+      <c r="D28" s="42" t="s">
+        <v>125</v>
+      </c>
       <c r="E28" s="27">
         <v>44531</v>
       </c>
-      <c r="F28" s="28"/>
+      <c r="F28" s="28">
+        <v>53075</v>
+      </c>
       <c r="G28" s="2"/>
       <c r="H28" s="36">
         <v>44531</v>
       </c>
-      <c r="I28" s="30"/>
+      <c r="I28" s="30">
+        <v>2607</v>
+      </c>
       <c r="J28" s="56"/>
       <c r="K28" s="57"/>
       <c r="L28" s="54"/>
@@ -9769,34 +9809,45 @@
         <v>0</v>
       </c>
       <c r="N28" s="33">
-        <v>0</v>
+        <v>16235</v>
       </c>
       <c r="P28" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>26605</v>
       </c>
       <c r="Q28" s="244">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R28" s="251"/>
+        <v>-26470</v>
+      </c>
+      <c r="R28" s="251">
+        <v>26470</v>
+      </c>
     </row>
     <row r="29" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="23"/>
       <c r="B29" s="24">
         <v>44532</v>
       </c>
-      <c r="C29" s="25"/>
-      <c r="D29" s="58"/>
+      <c r="C29" s="25">
+        <v>16193</v>
+      </c>
+      <c r="D29" s="58" t="s">
+        <v>126</v>
+      </c>
       <c r="E29" s="27">
         <v>44532</v>
       </c>
-      <c r="F29" s="28"/>
+      <c r="F29" s="28">
+        <f>61771+112553</f>
+        <v>174324</v>
+      </c>
       <c r="G29" s="2"/>
       <c r="H29" s="36">
         <v>44532</v>
       </c>
-      <c r="I29" s="30"/>
+      <c r="I29" s="30">
+        <v>975</v>
+      </c>
       <c r="J29" s="59"/>
       <c r="K29" s="188"/>
       <c r="L29" s="54"/>
@@ -9806,13 +9857,16 @@
       <c r="N29" s="33">
         <v>0</v>
       </c>
+      <c r="O29">
+        <v>9</v>
+      </c>
       <c r="P29" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>17168</v>
       </c>
       <c r="Q29" s="244">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-157156</v>
       </c>
       <c r="R29" s="251"/>
     </row>
@@ -10118,21 +10172,21 @@
       <c r="J39" s="60"/>
       <c r="K39" s="190"/>
       <c r="L39" s="61"/>
-      <c r="M39" s="275">
+      <c r="M39" s="264">
         <f>SUM(M5:M38)</f>
-        <v>0</v>
-      </c>
-      <c r="N39" s="277">
+        <v>6336</v>
+      </c>
+      <c r="N39" s="266">
         <f>SUM(N5:N38)</f>
-        <v>331786</v>
+        <v>372221</v>
       </c>
       <c r="P39" s="34">
         <f>SUM(P5:P38)</f>
-        <v>488146.13</v>
+        <v>578281.63</v>
       </c>
       <c r="Q39" s="234">
         <f>SUM(Q5:Q38)</f>
-        <v>-600660.87000000011</v>
+        <v>-820695.37000000011</v>
       </c>
     </row>
     <row r="40" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -10148,8 +10202,8 @@
       <c r="J40" s="60"/>
       <c r="K40" s="41"/>
       <c r="L40" s="61"/>
-      <c r="M40" s="276"/>
-      <c r="N40" s="278"/>
+      <c r="M40" s="265"/>
+      <c r="N40" s="267"/>
       <c r="P40" s="34"/>
       <c r="Q40" s="13"/>
     </row>
@@ -10322,7 +10376,7 @@
       </c>
       <c r="C50" s="87">
         <f>SUM(C5:C49)</f>
-        <v>99502.76</v>
+        <v>136785.26</v>
       </c>
       <c r="D50" s="88"/>
       <c r="E50" s="89" t="s">
@@ -10330,7 +10384,7 @@
       </c>
       <c r="F50" s="90">
         <f>SUM(F5:F49)</f>
-        <v>1088807</v>
+        <v>1398977</v>
       </c>
       <c r="G50" s="88"/>
       <c r="H50" s="91" t="s">
@@ -10338,7 +10392,7 @@
       </c>
       <c r="I50" s="92">
         <f>SUM(I5:I49)</f>
-        <v>16044.56</v>
+        <v>22126.559999999998</v>
       </c>
       <c r="J50" s="93"/>
       <c r="K50" s="94" t="s">
@@ -10364,32 +10418,32 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="279" t="s">
+      <c r="H52" s="268" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="280"/>
+      <c r="I52" s="269"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="281">
+      <c r="K52" s="270">
         <f>I50+L50</f>
-        <v>56857.369999999995</v>
-      </c>
-      <c r="L52" s="282"/>
-      <c r="M52" s="283">
+        <v>62939.369999999995</v>
+      </c>
+      <c r="L52" s="271"/>
+      <c r="M52" s="272">
         <f>N39+M39</f>
-        <v>331786</v>
-      </c>
-      <c r="N52" s="284"/>
+        <v>378557</v>
+      </c>
+      <c r="N52" s="273"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D53" s="285" t="s">
+      <c r="D53" s="274" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="285"/>
+      <c r="E53" s="274"/>
       <c r="F53" s="101">
         <f>F50-K52-C50</f>
-        <v>932446.87</v>
+        <v>1199252.3699999999</v>
       </c>
       <c r="I53" s="102"/>
       <c r="J53" s="103"/>
@@ -10397,22 +10451,22 @@
       <c r="Q53" s="13"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="285" t="s">
+      <c r="D54" s="274" t="s">
         <v>101</v>
       </c>
-      <c r="E54" s="285"/>
+      <c r="E54" s="274"/>
       <c r="F54" s="96">
         <v>-549976.4</v>
       </c>
-      <c r="I54" s="286" t="s">
+      <c r="I54" s="275" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="287"/>
-      <c r="K54" s="288">
+      <c r="J54" s="276"/>
+      <c r="K54" s="277">
         <f>F56+F57+F58</f>
-        <v>382470.47</v>
-      </c>
-      <c r="L54" s="289"/>
+        <v>649275.96999999986</v>
+      </c>
+      <c r="L54" s="278"/>
       <c r="P54" s="34"/>
       <c r="Q54" s="13"/>
     </row>
@@ -10438,18 +10492,18 @@
       </c>
       <c r="F56" s="96">
         <f>SUM(F53:F55)</f>
-        <v>382470.47</v>
+        <v>649275.96999999986</v>
       </c>
       <c r="H56" s="23"/>
       <c r="I56" s="108" t="s">
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="290">
+      <c r="K56" s="279">
         <f>-C4</f>
         <v>-567389.35</v>
       </c>
-      <c r="L56" s="291"/>
+      <c r="L56" s="280"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -10464,22 +10518,22 @@
     </row>
     <row r="58" spans="1:17" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C58" s="112"/>
-      <c r="D58" s="268" t="s">
+      <c r="D58" s="257" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="269"/>
+      <c r="E58" s="258"/>
       <c r="F58" s="113">
         <v>0</v>
       </c>
-      <c r="I58" s="270" t="s">
+      <c r="I58" s="259" t="s">
         <v>103</v>
       </c>
-      <c r="J58" s="271"/>
-      <c r="K58" s="272">
+      <c r="J58" s="260"/>
+      <c r="K58" s="261">
         <f>K54+K56</f>
-        <v>-184918.88</v>
-      </c>
-      <c r="L58" s="272"/>
+        <v>81886.619999999879</v>
+      </c>
+      <c r="L58" s="261"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -10623,6 +10677,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="I58:J58"/>
     <mergeCell ref="K58:L58"/>
@@ -10637,12 +10697,6 @@
     <mergeCell ref="I54:J54"/>
     <mergeCell ref="K54:L54"/>
     <mergeCell ref="K56:L56"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -13011,7 +13065,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
CIERRE 10 DIC 2021
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 11  NOVIEMBRE 2021/BALANCE    ZAVALETA   NOVIEMBRE    2021.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 11  NOVIEMBRE 2021/BALANCE    ZAVALETA   NOVIEMBRE    2021.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4035" yWindow="0" windowWidth="16335" windowHeight="11070" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="4035" yWindow="0" windowWidth="16335" windowHeight="11070" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="OCTUBRE      2 0 2 1     " sheetId="1" r:id="rId1"/>
@@ -153,7 +153,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="203">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -759,6 +759,9 @@
   </si>
   <si>
     <t>ADT PRIVATE</t>
+  </si>
+  <si>
+    <t>cancelada</t>
   </si>
 </sst>
 </file>
@@ -2237,7 +2240,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="344">
+  <cellXfs count="350">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -2748,187 +2751,10 @@
     <xf numFmtId="44" fontId="2" fillId="12" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="6" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="6" borderId="51" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="6" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="50" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="43" fillId="6" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="43" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="3" fillId="14" borderId="61" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="3" fillId="14" borderId="63" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="63" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="13" fillId="15" borderId="65" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="15" borderId="66" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="9" borderId="67" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="9" borderId="64" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="33" fillId="13" borderId="68" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="33" fillId="13" borderId="69" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="33" fillId="13" borderId="70" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="33" fillId="13" borderId="71" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="7" fontId="33" fillId="6" borderId="72" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="33" fillId="6" borderId="73" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="6" borderId="74" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="33" fillId="6" borderId="75" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="33" fillId="6" borderId="76" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="6" borderId="77" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="7" fontId="11" fillId="0" borderId="67" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="7" fontId="11" fillId="0" borderId="64" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="7" fontId="11" fillId="0" borderId="68" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="7" fontId="11" fillId="0" borderId="69" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2947,10 +2773,6 @@
     </xf>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="78" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="79" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="79" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2992,6 +2814,199 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="6" borderId="79" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="6" borderId="79" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="6" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="6" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="6" borderId="51" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="6" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="50" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="43" fillId="6" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="43" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="33" fillId="6" borderId="72" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="33" fillId="6" borderId="73" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="33" fillId="6" borderId="75" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="33" fillId="6" borderId="76" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="6" borderId="74" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="6" borderId="77" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="15" borderId="65" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="15" borderId="66" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="9" borderId="67" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="9" borderId="64" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="33" fillId="13" borderId="68" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="33" fillId="13" borderId="69" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="33" fillId="13" borderId="70" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="33" fillId="13" borderId="71" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="11" fillId="0" borderId="67" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="11" fillId="0" borderId="64" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="11" fillId="0" borderId="68" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="11" fillId="0" borderId="69" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="3" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="38" fillId="3" borderId="53" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -4164,23 +4179,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="254"/>
-      <c r="C1" s="256" t="s">
+      <c r="B1" s="287"/>
+      <c r="C1" s="289" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="257"/>
-      <c r="E1" s="257"/>
-      <c r="F1" s="257"/>
-      <c r="G1" s="257"/>
-      <c r="H1" s="257"/>
-      <c r="I1" s="257"/>
-      <c r="J1" s="257"/>
-      <c r="K1" s="257"/>
-      <c r="L1" s="257"/>
-      <c r="M1" s="257"/>
+      <c r="D1" s="290"/>
+      <c r="E1" s="290"/>
+      <c r="F1" s="290"/>
+      <c r="G1" s="290"/>
+      <c r="H1" s="290"/>
+      <c r="I1" s="290"/>
+      <c r="J1" s="290"/>
+      <c r="K1" s="290"/>
+      <c r="L1" s="290"/>
+      <c r="M1" s="290"/>
     </row>
     <row r="2" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="255"/>
+      <c r="B2" s="288"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -4190,17 +4205,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:19" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="258" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="259"/>
+      <c r="B3" s="291" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="292"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="260" t="s">
+      <c r="H3" s="293" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="260"/>
+      <c r="I3" s="293"/>
       <c r="K3" s="178"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
@@ -4214,14 +4229,14 @@
         <v>0</v>
       </c>
       <c r="D4" s="18"/>
-      <c r="E4" s="261" t="s">
+      <c r="E4" s="294" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="262"/>
-      <c r="H4" s="263" t="s">
+      <c r="F4" s="295"/>
+      <c r="H4" s="296" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="264"/>
+      <c r="I4" s="297"/>
       <c r="J4" s="19"/>
       <c r="K4" s="179"/>
       <c r="L4" s="20"/>
@@ -4231,10 +4246,10 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="270" t="s">
+      <c r="P4" s="303" t="s">
         <v>6</v>
       </c>
-      <c r="Q4" s="271"/>
+      <c r="Q4" s="304"/>
     </row>
     <row r="5" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
@@ -5675,11 +5690,11 @@
       <c r="J39" s="60"/>
       <c r="K39" s="190"/>
       <c r="L39" s="61"/>
-      <c r="M39" s="272">
+      <c r="M39" s="305">
         <f>SUM(M5:M38)</f>
         <v>247061</v>
       </c>
-      <c r="N39" s="274">
+      <c r="N39" s="307">
         <f>SUM(N5:N38)</f>
         <v>172863</v>
       </c>
@@ -5705,8 +5720,8 @@
       <c r="J40" s="60"/>
       <c r="K40" s="41"/>
       <c r="L40" s="61"/>
-      <c r="M40" s="273"/>
-      <c r="N40" s="275"/>
+      <c r="M40" s="306"/>
+      <c r="N40" s="308"/>
       <c r="P40" s="34"/>
       <c r="Q40" s="9"/>
     </row>
@@ -5921,29 +5936,29 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="276" t="s">
+      <c r="H52" s="309" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="277"/>
+      <c r="I52" s="310"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="278">
+      <c r="K52" s="311">
         <f>I50+L50</f>
         <v>53873.49</v>
       </c>
-      <c r="L52" s="279"/>
-      <c r="M52" s="280">
+      <c r="L52" s="312"/>
+      <c r="M52" s="313">
         <f>N39+M39</f>
         <v>419924</v>
       </c>
-      <c r="N52" s="281"/>
+      <c r="N52" s="314"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D53" s="282" t="s">
+      <c r="D53" s="315" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="282"/>
+      <c r="E53" s="315"/>
       <c r="F53" s="101">
         <f>F50-K52-C50</f>
         <v>471038.61</v>
@@ -5954,22 +5969,22 @@
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="282" t="s">
+      <c r="D54" s="315" t="s">
         <v>101</v>
       </c>
-      <c r="E54" s="282"/>
+      <c r="E54" s="315"/>
       <c r="F54" s="96">
         <v>-549976.4</v>
       </c>
-      <c r="I54" s="283" t="s">
+      <c r="I54" s="316" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="284"/>
-      <c r="K54" s="285">
+      <c r="J54" s="317"/>
+      <c r="K54" s="318">
         <f>F56+F57+F58</f>
         <v>-24577.400000000023</v>
       </c>
-      <c r="L54" s="286"/>
+      <c r="L54" s="319"/>
       <c r="P54" s="34"/>
       <c r="Q54" s="9"/>
     </row>
@@ -6002,11 +6017,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="287">
+      <c r="K56" s="320">
         <f>-C4</f>
         <v>0</v>
       </c>
-      <c r="L56" s="288"/>
+      <c r="L56" s="321"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -6023,22 +6038,22 @@
       <c r="C58" s="112">
         <v>44507</v>
       </c>
-      <c r="D58" s="265" t="s">
+      <c r="D58" s="298" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="266"/>
+      <c r="E58" s="299"/>
       <c r="F58" s="113">
         <v>567389.35</v>
       </c>
-      <c r="I58" s="267" t="s">
+      <c r="I58" s="300" t="s">
         <v>103</v>
       </c>
-      <c r="J58" s="268"/>
-      <c r="K58" s="269">
+      <c r="J58" s="301"/>
+      <c r="K58" s="302">
         <f>K54+K56</f>
         <v>-24577.400000000023</v>
       </c>
-      <c r="L58" s="269"/>
+      <c r="L58" s="302"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -6217,8 +6232,8 @@
   </sheetPr>
   <dimension ref="A1:N134"/>
   <sheetViews>
-    <sheetView topLeftCell="G37" workbookViewId="0">
-      <selection activeCell="J99" sqref="J99"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D17" sqref="D16:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6233,7 +6248,7 @@
     <col min="9" max="9" width="13.42578125" style="98" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.7109375" style="116" customWidth="1"/>
     <col min="11" max="11" width="16.85546875" style="4" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" style="340" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" style="279" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="19.5703125" style="3" bestFit="1" customWidth="1"/>
   </cols>
@@ -6254,7 +6269,7 @@
       </c>
       <c r="J1" s="207"/>
       <c r="K1" s="202"/>
-      <c r="L1" s="334"/>
+      <c r="L1" s="273"/>
       <c r="M1" s="202"/>
       <c r="N1" s="169" t="s">
         <v>31</v>
@@ -6288,7 +6303,7 @@
       <c r="K2" s="132" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="335" t="s">
+      <c r="L2" s="274" t="s">
         <v>22</v>
       </c>
       <c r="M2" s="132" t="s">
@@ -6323,7 +6338,7 @@
       <c r="K3" s="210">
         <v>19269</v>
       </c>
-      <c r="L3" s="341">
+      <c r="L3" s="280">
         <v>44498</v>
       </c>
       <c r="M3" s="69">
@@ -6360,7 +6375,7 @@
       <c r="K4" s="210">
         <v>25542</v>
       </c>
-      <c r="L4" s="342">
+      <c r="L4" s="281">
         <v>44498</v>
       </c>
       <c r="M4" s="69">
@@ -6396,7 +6411,7 @@
       <c r="K5" s="210">
         <v>10208</v>
       </c>
-      <c r="L5" s="343">
+      <c r="L5" s="282">
         <v>44498</v>
       </c>
       <c r="M5" s="69">
@@ -6744,7 +6759,7 @@
       <c r="E16" s="69">
         <v>145000</v>
       </c>
-      <c r="F16" s="137">
+      <c r="F16" s="349">
         <f t="shared" si="0"/>
         <v>146930.89999999991</v>
       </c>
@@ -6757,7 +6772,7 @@
       <c r="K16" s="210">
         <v>6297</v>
       </c>
-      <c r="L16" s="336"/>
+      <c r="L16" s="275"/>
       <c r="M16" s="69"/>
       <c r="N16" s="137">
         <f t="shared" si="1"/>
@@ -6789,7 +6804,7 @@
       <c r="K17" s="210">
         <v>12350</v>
       </c>
-      <c r="L17" s="336"/>
+      <c r="L17" s="275"/>
       <c r="M17" s="69"/>
       <c r="N17" s="137">
         <f t="shared" si="1"/>
@@ -6821,7 +6836,7 @@
       <c r="K18" s="210">
         <v>5444</v>
       </c>
-      <c r="L18" s="336"/>
+      <c r="L18" s="275"/>
       <c r="M18" s="69"/>
       <c r="N18" s="137">
         <f t="shared" si="1"/>
@@ -6853,7 +6868,7 @@
       <c r="K19" s="210">
         <v>1717</v>
       </c>
-      <c r="L19" s="336"/>
+      <c r="L19" s="275"/>
       <c r="M19" s="69"/>
       <c r="N19" s="137">
         <f t="shared" si="1"/>
@@ -6885,7 +6900,7 @@
       <c r="K20" s="210">
         <v>16136</v>
       </c>
-      <c r="L20" s="336"/>
+      <c r="L20" s="275"/>
       <c r="M20" s="69"/>
       <c r="N20" s="137">
         <f t="shared" si="1"/>
@@ -6917,7 +6932,7 @@
       <c r="K21" s="210">
         <v>9256</v>
       </c>
-      <c r="L21" s="336"/>
+      <c r="L21" s="275"/>
       <c r="M21" s="69"/>
       <c r="N21" s="137">
         <f t="shared" si="1"/>
@@ -6950,7 +6965,7 @@
       <c r="K22" s="210">
         <v>5500</v>
       </c>
-      <c r="L22" s="336"/>
+      <c r="L22" s="275"/>
       <c r="M22" s="69"/>
       <c r="N22" s="137">
         <f t="shared" si="1"/>
@@ -6982,7 +6997,7 @@
       <c r="K23" s="210">
         <v>1331</v>
       </c>
-      <c r="L23" s="336"/>
+      <c r="L23" s="275"/>
       <c r="M23" s="69"/>
       <c r="N23" s="137">
         <f t="shared" si="1"/>
@@ -7014,7 +7029,7 @@
       <c r="K24" s="210">
         <v>420</v>
       </c>
-      <c r="L24" s="336"/>
+      <c r="L24" s="275"/>
       <c r="M24" s="69"/>
       <c r="N24" s="137">
         <f t="shared" si="1"/>
@@ -7046,7 +7061,7 @@
       <c r="K25" s="210">
         <v>770</v>
       </c>
-      <c r="L25" s="336"/>
+      <c r="L25" s="275"/>
       <c r="M25" s="69"/>
       <c r="N25" s="137">
         <f t="shared" si="1"/>
@@ -7078,7 +7093,7 @@
       <c r="K26" s="210">
         <v>2257</v>
       </c>
-      <c r="L26" s="336"/>
+      <c r="L26" s="275"/>
       <c r="M26" s="69"/>
       <c r="N26" s="137">
         <f t="shared" si="1"/>
@@ -7110,7 +7125,7 @@
       <c r="K27" s="210">
         <v>60</v>
       </c>
-      <c r="L27" s="336"/>
+      <c r="L27" s="275"/>
       <c r="M27" s="69"/>
       <c r="N27" s="137">
         <f t="shared" si="1"/>
@@ -7142,7 +7157,7 @@
       <c r="K28" s="210">
         <v>39533</v>
       </c>
-      <c r="L28" s="336"/>
+      <c r="L28" s="275"/>
       <c r="M28" s="69"/>
       <c r="N28" s="137">
         <f t="shared" si="1"/>
@@ -7174,7 +7189,7 @@
       <c r="K29" s="210">
         <v>3727</v>
       </c>
-      <c r="L29" s="336"/>
+      <c r="L29" s="275"/>
       <c r="M29" s="69"/>
       <c r="N29" s="137">
         <f t="shared" si="1"/>
@@ -7207,7 +7222,7 @@
       <c r="K30" s="212">
         <v>3861</v>
       </c>
-      <c r="L30" s="336"/>
+      <c r="L30" s="275"/>
       <c r="M30" s="69"/>
       <c r="N30" s="137">
         <f t="shared" si="1"/>
@@ -7239,7 +7254,7 @@
       <c r="K31" s="210">
         <v>24825</v>
       </c>
-      <c r="L31" s="336"/>
+      <c r="L31" s="275"/>
       <c r="M31" s="69"/>
       <c r="N31" s="137">
         <f t="shared" si="1"/>
@@ -7271,7 +7286,7 @@
       <c r="K32" s="210">
         <v>614</v>
       </c>
-      <c r="L32" s="336"/>
+      <c r="L32" s="275"/>
       <c r="M32" s="69"/>
       <c r="N32" s="137">
         <f t="shared" si="1"/>
@@ -7303,7 +7318,7 @@
       <c r="K33" s="210">
         <v>2901</v>
       </c>
-      <c r="L33" s="336"/>
+      <c r="L33" s="275"/>
       <c r="M33" s="69"/>
       <c r="N33" s="137">
         <f t="shared" si="1"/>
@@ -7335,7 +7350,7 @@
       <c r="K34" s="210">
         <v>2623</v>
       </c>
-      <c r="L34" s="336"/>
+      <c r="L34" s="275"/>
       <c r="M34" s="69"/>
       <c r="N34" s="137">
         <f t="shared" si="1"/>
@@ -7367,7 +7382,7 @@
       <c r="K35" s="210">
         <v>740</v>
       </c>
-      <c r="L35" s="336"/>
+      <c r="L35" s="275"/>
       <c r="M35" s="69"/>
       <c r="N35" s="137">
         <f t="shared" si="1"/>
@@ -7399,7 +7414,7 @@
       <c r="K36" s="212">
         <v>1189</v>
       </c>
-      <c r="L36" s="336"/>
+      <c r="L36" s="275"/>
       <c r="M36" s="69"/>
       <c r="N36" s="137">
         <f t="shared" si="1"/>
@@ -7431,7 +7446,7 @@
       <c r="K37" s="210">
         <v>6711</v>
       </c>
-      <c r="L37" s="336"/>
+      <c r="L37" s="275"/>
       <c r="M37" s="69"/>
       <c r="N37" s="137">
         <f t="shared" si="1"/>
@@ -7463,7 +7478,7 @@
       <c r="K38" s="210">
         <v>71111</v>
       </c>
-      <c r="L38" s="336"/>
+      <c r="L38" s="275"/>
       <c r="M38" s="69"/>
       <c r="N38" s="137">
         <f t="shared" si="1"/>
@@ -7495,7 +7510,7 @@
       <c r="K39" s="210">
         <v>13525</v>
       </c>
-      <c r="L39" s="336"/>
+      <c r="L39" s="275"/>
       <c r="M39" s="69"/>
       <c r="N39" s="137">
         <f t="shared" si="1"/>
@@ -7527,7 +7542,7 @@
       <c r="K40" s="210">
         <v>7227</v>
       </c>
-      <c r="L40" s="336"/>
+      <c r="L40" s="275"/>
       <c r="M40" s="69"/>
       <c r="N40" s="137">
         <f t="shared" si="1"/>
@@ -7538,7 +7553,7 @@
       <c r="A41" s="140">
         <v>44507</v>
       </c>
-      <c r="B41" s="289" t="s">
+      <c r="B41" s="322" t="s">
         <v>98</v>
       </c>
       <c r="C41" s="204">
@@ -7559,7 +7574,7 @@
       <c r="K41" s="210">
         <v>2618</v>
       </c>
-      <c r="L41" s="336"/>
+      <c r="L41" s="275"/>
       <c r="M41" s="69"/>
       <c r="N41" s="137">
         <f t="shared" si="1"/>
@@ -7570,7 +7585,7 @@
       <c r="A42" s="140" t="s">
         <v>99</v>
       </c>
-      <c r="B42" s="290"/>
+      <c r="B42" s="323"/>
       <c r="C42" s="143">
         <v>0</v>
       </c>
@@ -7589,7 +7604,7 @@
       <c r="K42" s="210">
         <v>8371</v>
       </c>
-      <c r="L42" s="336"/>
+      <c r="L42" s="275"/>
       <c r="M42" s="69"/>
       <c r="N42" s="137">
         <f t="shared" si="1"/>
@@ -7615,7 +7630,7 @@
       <c r="K43" s="210">
         <v>753</v>
       </c>
-      <c r="L43" s="336"/>
+      <c r="L43" s="275"/>
       <c r="M43" s="69"/>
       <c r="N43" s="137">
         <f t="shared" si="1"/>
@@ -7641,7 +7656,7 @@
       <c r="K44" s="214">
         <v>0</v>
       </c>
-      <c r="L44" s="336"/>
+      <c r="L44" s="275"/>
       <c r="M44" s="69"/>
       <c r="N44" s="137">
         <f t="shared" si="1"/>
@@ -7667,7 +7682,7 @@
       <c r="K45" s="210">
         <v>5240</v>
       </c>
-      <c r="L45" s="336"/>
+      <c r="L45" s="275"/>
       <c r="M45" s="69"/>
       <c r="N45" s="137">
         <f t="shared" si="1"/>
@@ -7693,7 +7708,7 @@
       <c r="K46" s="210">
         <v>15576</v>
       </c>
-      <c r="L46" s="336"/>
+      <c r="L46" s="275"/>
       <c r="M46" s="69"/>
       <c r="N46" s="137">
         <f t="shared" si="1"/>
@@ -7719,7 +7734,7 @@
       <c r="K47" s="210">
         <v>739</v>
       </c>
-      <c r="L47" s="336"/>
+      <c r="L47" s="275"/>
       <c r="M47" s="69"/>
       <c r="N47" s="137">
         <f t="shared" si="1"/>
@@ -7745,7 +7760,7 @@
       <c r="K48" s="210">
         <v>623</v>
       </c>
-      <c r="L48" s="336"/>
+      <c r="L48" s="275"/>
       <c r="M48" s="69"/>
       <c r="N48" s="137">
         <f t="shared" si="1"/>
@@ -7771,7 +7786,7 @@
       <c r="K49" s="210">
         <v>2636</v>
       </c>
-      <c r="L49" s="336"/>
+      <c r="L49" s="275"/>
       <c r="M49" s="69"/>
       <c r="N49" s="137">
         <f t="shared" si="1"/>
@@ -7797,7 +7812,7 @@
       <c r="K50" s="210">
         <v>120</v>
       </c>
-      <c r="L50" s="336"/>
+      <c r="L50" s="275"/>
       <c r="M50" s="69"/>
       <c r="N50" s="137">
         <f t="shared" si="1"/>
@@ -7823,7 +7838,7 @@
       <c r="K51" s="210">
         <v>14669</v>
       </c>
-      <c r="L51" s="336"/>
+      <c r="L51" s="275"/>
       <c r="M51" s="69"/>
       <c r="N51" s="137">
         <f t="shared" si="1"/>
@@ -7849,7 +7864,7 @@
       <c r="K52" s="210">
         <v>2897</v>
       </c>
-      <c r="L52" s="336"/>
+      <c r="L52" s="275"/>
       <c r="M52" s="69"/>
       <c r="N52" s="137">
         <f t="shared" si="1"/>
@@ -7875,7 +7890,7 @@
       <c r="K53" s="210">
         <v>360</v>
       </c>
-      <c r="L53" s="336"/>
+      <c r="L53" s="275"/>
       <c r="M53" s="69"/>
       <c r="N53" s="137">
         <f t="shared" si="1"/>
@@ -7901,7 +7916,7 @@
       <c r="K54" s="210">
         <v>4820</v>
       </c>
-      <c r="L54" s="336"/>
+      <c r="L54" s="275"/>
       <c r="M54" s="69"/>
       <c r="N54" s="137">
         <f t="shared" si="1"/>
@@ -7927,7 +7942,7 @@
       <c r="K55" s="210">
         <v>4925</v>
       </c>
-      <c r="L55" s="336"/>
+      <c r="L55" s="275"/>
       <c r="M55" s="69"/>
       <c r="N55" s="137">
         <f t="shared" si="1"/>
@@ -7953,7 +7968,7 @@
       <c r="K56" s="210">
         <v>5</v>
       </c>
-      <c r="L56" s="336"/>
+      <c r="L56" s="275"/>
       <c r="M56" s="69"/>
       <c r="N56" s="137">
         <f t="shared" si="1"/>
@@ -7979,7 +7994,7 @@
       <c r="K57" s="210">
         <v>6665</v>
       </c>
-      <c r="L57" s="336"/>
+      <c r="L57" s="275"/>
       <c r="M57" s="69"/>
       <c r="N57" s="137">
         <f t="shared" si="1"/>
@@ -8005,7 +8020,7 @@
       <c r="K58" s="210">
         <v>646</v>
       </c>
-      <c r="L58" s="336"/>
+      <c r="L58" s="275"/>
       <c r="M58" s="69"/>
       <c r="N58" s="137">
         <f t="shared" si="1"/>
@@ -8031,7 +8046,7 @@
       <c r="K59" s="214">
         <v>-34125.46</v>
       </c>
-      <c r="L59" s="336"/>
+      <c r="L59" s="275"/>
       <c r="M59" s="69"/>
       <c r="N59" s="137">
         <f t="shared" si="1"/>
@@ -8051,7 +8066,7 @@
       <c r="I60" s="134"/>
       <c r="J60" s="139"/>
       <c r="K60" s="69"/>
-      <c r="L60" s="336"/>
+      <c r="L60" s="275"/>
       <c r="M60" s="69"/>
       <c r="N60" s="137">
         <f t="shared" si="1"/>
@@ -8071,7 +8086,7 @@
       <c r="I61" s="134"/>
       <c r="J61" s="139"/>
       <c r="K61" s="69"/>
-      <c r="L61" s="336"/>
+      <c r="L61" s="275"/>
       <c r="M61" s="69"/>
       <c r="N61" s="137">
         <f t="shared" si="1"/>
@@ -8091,7 +8106,7 @@
       <c r="I62" s="134"/>
       <c r="J62" s="139"/>
       <c r="K62" s="69"/>
-      <c r="L62" s="336"/>
+      <c r="L62" s="275"/>
       <c r="M62" s="69"/>
       <c r="N62" s="137">
         <f t="shared" si="1"/>
@@ -8111,7 +8126,7 @@
       <c r="I63" s="141"/>
       <c r="J63" s="142"/>
       <c r="K63" s="143"/>
-      <c r="L63" s="336"/>
+      <c r="L63" s="275"/>
       <c r="M63" s="69"/>
       <c r="N63" s="137">
         <f t="shared" si="1"/>
@@ -8131,7 +8146,7 @@
       <c r="I64" s="141"/>
       <c r="J64" s="142"/>
       <c r="K64" s="143"/>
-      <c r="L64" s="336"/>
+      <c r="L64" s="275"/>
       <c r="M64" s="69"/>
       <c r="N64" s="137">
         <f t="shared" si="1"/>
@@ -8151,7 +8166,7 @@
       <c r="I65" s="141"/>
       <c r="J65" s="142"/>
       <c r="K65" s="143"/>
-      <c r="L65" s="336"/>
+      <c r="L65" s="275"/>
       <c r="M65" s="69"/>
       <c r="N65" s="137">
         <f t="shared" si="1"/>
@@ -8171,7 +8186,7 @@
       <c r="I66" s="141"/>
       <c r="J66" s="142"/>
       <c r="K66" s="143"/>
-      <c r="L66" s="336"/>
+      <c r="L66" s="275"/>
       <c r="M66" s="69"/>
       <c r="N66" s="137">
         <f t="shared" si="1"/>
@@ -8191,7 +8206,7 @@
       <c r="I67" s="141"/>
       <c r="J67" s="142"/>
       <c r="K67" s="143"/>
-      <c r="L67" s="336"/>
+      <c r="L67" s="275"/>
       <c r="M67" s="69"/>
       <c r="N67" s="137">
         <f t="shared" si="1"/>
@@ -8211,7 +8226,7 @@
       <c r="I68" s="141"/>
       <c r="J68" s="142"/>
       <c r="K68" s="143"/>
-      <c r="L68" s="336"/>
+      <c r="L68" s="275"/>
       <c r="M68" s="69"/>
       <c r="N68" s="137">
         <f t="shared" si="1"/>
@@ -8231,7 +8246,7 @@
       <c r="I69" s="141"/>
       <c r="J69" s="142"/>
       <c r="K69" s="143"/>
-      <c r="L69" s="336"/>
+      <c r="L69" s="275"/>
       <c r="M69" s="69"/>
       <c r="N69" s="137">
         <f t="shared" ref="N69:N97" si="3">N68+K69-M69</f>
@@ -8251,7 +8266,7 @@
       <c r="I70" s="141"/>
       <c r="J70" s="142"/>
       <c r="K70" s="143"/>
-      <c r="L70" s="336"/>
+      <c r="L70" s="275"/>
       <c r="M70" s="69"/>
       <c r="N70" s="137">
         <f t="shared" si="3"/>
@@ -8271,7 +8286,7 @@
       <c r="I71" s="141"/>
       <c r="J71" s="142"/>
       <c r="K71" s="143"/>
-      <c r="L71" s="336"/>
+      <c r="L71" s="275"/>
       <c r="M71" s="69"/>
       <c r="N71" s="137">
         <f t="shared" si="3"/>
@@ -8291,7 +8306,7 @@
       <c r="I72" s="141"/>
       <c r="J72" s="142"/>
       <c r="K72" s="143"/>
-      <c r="L72" s="336"/>
+      <c r="L72" s="275"/>
       <c r="M72" s="69"/>
       <c r="N72" s="137">
         <f t="shared" si="3"/>
@@ -8311,7 +8326,7 @@
       <c r="I73" s="141"/>
       <c r="J73" s="142"/>
       <c r="K73" s="143"/>
-      <c r="L73" s="336"/>
+      <c r="L73" s="275"/>
       <c r="M73" s="69"/>
       <c r="N73" s="137">
         <f t="shared" si="3"/>
@@ -8331,7 +8346,7 @@
       <c r="I74" s="141"/>
       <c r="J74" s="142"/>
       <c r="K74" s="143"/>
-      <c r="L74" s="336"/>
+      <c r="L74" s="275"/>
       <c r="M74" s="69"/>
       <c r="N74" s="137">
         <f t="shared" si="3"/>
@@ -8351,7 +8366,7 @@
       <c r="I75" s="141"/>
       <c r="J75" s="142"/>
       <c r="K75" s="143"/>
-      <c r="L75" s="336"/>
+      <c r="L75" s="275"/>
       <c r="M75" s="69"/>
       <c r="N75" s="137">
         <f t="shared" si="3"/>
@@ -8371,7 +8386,7 @@
       <c r="I76" s="141"/>
       <c r="J76" s="142"/>
       <c r="K76" s="143"/>
-      <c r="L76" s="336"/>
+      <c r="L76" s="275"/>
       <c r="M76" s="69"/>
       <c r="N76" s="137">
         <f t="shared" si="3"/>
@@ -8391,7 +8406,7 @@
       <c r="I77" s="141"/>
       <c r="J77" s="142"/>
       <c r="K77" s="143"/>
-      <c r="L77" s="336"/>
+      <c r="L77" s="275"/>
       <c r="M77" s="69"/>
       <c r="N77" s="137">
         <f t="shared" si="3"/>
@@ -8411,7 +8426,7 @@
       <c r="I78" s="141"/>
       <c r="J78" s="142"/>
       <c r="K78" s="143"/>
-      <c r="L78" s="336"/>
+      <c r="L78" s="275"/>
       <c r="M78" s="69"/>
       <c r="N78" s="137">
         <f t="shared" si="3"/>
@@ -8431,7 +8446,7 @@
       <c r="I79" s="141"/>
       <c r="J79" s="142"/>
       <c r="K79" s="143"/>
-      <c r="L79" s="336"/>
+      <c r="L79" s="275"/>
       <c r="M79" s="69"/>
       <c r="N79" s="137">
         <f t="shared" si="3"/>
@@ -8451,7 +8466,7 @@
       <c r="I80" s="141"/>
       <c r="J80" s="142"/>
       <c r="K80" s="143"/>
-      <c r="L80" s="336"/>
+      <c r="L80" s="275"/>
       <c r="M80" s="69"/>
       <c r="N80" s="137">
         <f t="shared" si="3"/>
@@ -8591,7 +8606,7 @@
       <c r="I87" s="141"/>
       <c r="J87" s="142"/>
       <c r="K87" s="143"/>
-      <c r="L87" s="337"/>
+      <c r="L87" s="276"/>
       <c r="M87" s="69"/>
       <c r="N87" s="137">
         <f t="shared" si="3"/>
@@ -8611,7 +8626,7 @@
       <c r="I88" s="141"/>
       <c r="J88" s="142"/>
       <c r="K88" s="143"/>
-      <c r="L88" s="337"/>
+      <c r="L88" s="276"/>
       <c r="M88" s="69"/>
       <c r="N88" s="137">
         <f t="shared" si="3"/>
@@ -8631,7 +8646,7 @@
       <c r="I89" s="141"/>
       <c r="J89" s="142"/>
       <c r="K89" s="143"/>
-      <c r="L89" s="337"/>
+      <c r="L89" s="276"/>
       <c r="M89" s="69"/>
       <c r="N89" s="137">
         <f t="shared" si="3"/>
@@ -8651,7 +8666,7 @@
       <c r="I90" s="141"/>
       <c r="J90" s="142"/>
       <c r="K90" s="143"/>
-      <c r="L90" s="337"/>
+      <c r="L90" s="276"/>
       <c r="M90" s="69"/>
       <c r="N90" s="137">
         <f t="shared" si="3"/>
@@ -8671,7 +8686,7 @@
       <c r="I91" s="141"/>
       <c r="J91" s="142"/>
       <c r="K91" s="143"/>
-      <c r="L91" s="337"/>
+      <c r="L91" s="276"/>
       <c r="M91" s="69"/>
       <c r="N91" s="137">
         <f t="shared" si="3"/>
@@ -8691,7 +8706,7 @@
       <c r="I92" s="141"/>
       <c r="J92" s="142"/>
       <c r="K92" s="143"/>
-      <c r="L92" s="337"/>
+      <c r="L92" s="276"/>
       <c r="M92" s="69"/>
       <c r="N92" s="137">
         <f t="shared" si="3"/>
@@ -8711,7 +8726,7 @@
       <c r="I93" s="141"/>
       <c r="J93" s="142"/>
       <c r="K93" s="143"/>
-      <c r="L93" s="337"/>
+      <c r="L93" s="276"/>
       <c r="M93" s="69"/>
       <c r="N93" s="137">
         <f t="shared" si="3"/>
@@ -8731,7 +8746,7 @@
       <c r="I94" s="141"/>
       <c r="J94" s="142"/>
       <c r="K94" s="143"/>
-      <c r="L94" s="337"/>
+      <c r="L94" s="276"/>
       <c r="M94" s="69"/>
       <c r="N94" s="137">
         <f t="shared" si="3"/>
@@ -8751,7 +8766,7 @@
       <c r="I95" s="141"/>
       <c r="J95" s="142"/>
       <c r="K95" s="143"/>
-      <c r="L95" s="337"/>
+      <c r="L95" s="276"/>
       <c r="M95" s="69"/>
       <c r="N95" s="137">
         <f t="shared" si="3"/>
@@ -8771,7 +8786,7 @@
       <c r="I96" s="141"/>
       <c r="J96" s="142"/>
       <c r="K96" s="143"/>
-      <c r="L96" s="337"/>
+      <c r="L96" s="276"/>
       <c r="M96" s="69"/>
       <c r="N96" s="137">
         <f t="shared" si="3"/>
@@ -8795,7 +8810,7 @@
       <c r="K97" s="151">
         <v>0</v>
       </c>
-      <c r="L97" s="338"/>
+      <c r="L97" s="277"/>
       <c r="M97" s="151"/>
       <c r="N97" s="137">
         <f t="shared" si="3"/>
@@ -8821,7 +8836,7 @@
         <f>SUM(K3:K97)</f>
         <v>564370.54</v>
       </c>
-      <c r="L98" s="339"/>
+      <c r="L98" s="278"/>
       <c r="M98" s="1">
         <f>SUM(M3:M97)</f>
         <v>51341.58</v>
@@ -8838,7 +8853,7 @@
       <c r="E99" s="3"/>
       <c r="F99" s="1"/>
       <c r="K99" s="1"/>
-      <c r="L99" s="339"/>
+      <c r="L99" s="278"/>
       <c r="M99" s="3"/>
       <c r="N99" s="1"/>
     </row>
@@ -8849,7 +8864,7 @@
       <c r="E100" s="3"/>
       <c r="F100" s="1"/>
       <c r="K100" s="1"/>
-      <c r="L100" s="339"/>
+      <c r="L100" s="278"/>
       <c r="M100" s="3"/>
       <c r="N100" s="1"/>
     </row>
@@ -9129,7 +9144,7 @@
   </sheetPr>
   <dimension ref="A1:U80"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="J60" sqref="J60"/>
     </sheetView>
   </sheetViews>
@@ -9155,23 +9170,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="254"/>
-      <c r="C1" s="256" t="s">
+      <c r="B1" s="287"/>
+      <c r="C1" s="289" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="257"/>
-      <c r="E1" s="257"/>
-      <c r="F1" s="257"/>
-      <c r="G1" s="257"/>
-      <c r="H1" s="257"/>
-      <c r="I1" s="257"/>
-      <c r="J1" s="257"/>
-      <c r="K1" s="257"/>
-      <c r="L1" s="257"/>
-      <c r="M1" s="257"/>
+      <c r="D1" s="290"/>
+      <c r="E1" s="290"/>
+      <c r="F1" s="290"/>
+      <c r="G1" s="290"/>
+      <c r="H1" s="290"/>
+      <c r="I1" s="290"/>
+      <c r="J1" s="290"/>
+      <c r="K1" s="290"/>
+      <c r="L1" s="290"/>
+      <c r="M1" s="290"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="255"/>
+      <c r="B2" s="288"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -9181,17 +9196,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="258" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="259"/>
+      <c r="B3" s="291" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="292"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="260" t="s">
+      <c r="H3" s="293" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="260"/>
+      <c r="I3" s="293"/>
       <c r="K3" s="178"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
@@ -9207,14 +9222,14 @@
       <c r="D4" s="18">
         <v>44507</v>
       </c>
-      <c r="E4" s="261" t="s">
+      <c r="E4" s="294" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="262"/>
-      <c r="H4" s="263" t="s">
+      <c r="F4" s="295"/>
+      <c r="H4" s="296" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="264"/>
+      <c r="I4" s="297"/>
       <c r="J4" s="19"/>
       <c r="K4" s="179"/>
       <c r="L4" s="20"/>
@@ -9224,10 +9239,10 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="270" t="s">
+      <c r="P4" s="303" t="s">
         <v>6</v>
       </c>
-      <c r="Q4" s="271"/>
+      <c r="Q4" s="304"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
@@ -10585,7 +10600,7 @@
       <c r="J33" s="60" t="s">
         <v>201</v>
       </c>
-      <c r="K33" s="330">
+      <c r="K33" s="269">
         <v>44508</v>
       </c>
       <c r="L33" s="66">
@@ -10627,7 +10642,7 @@
         <v>0</v>
       </c>
       <c r="J34" s="60"/>
-      <c r="K34" s="331">
+      <c r="K34" s="270">
         <v>44509</v>
       </c>
       <c r="L34" s="44">
@@ -10669,7 +10684,7 @@
         <v>0</v>
       </c>
       <c r="J35" s="60"/>
-      <c r="K35" s="332">
+      <c r="K35" s="271">
         <v>44509</v>
       </c>
       <c r="L35" s="66">
@@ -10711,7 +10726,7 @@
         <v>0</v>
       </c>
       <c r="J36" s="60"/>
-      <c r="K36" s="333">
+      <c r="K36" s="272">
         <v>44511</v>
       </c>
       <c r="L36" s="44">
@@ -10749,7 +10764,7 @@
         <v>0</v>
       </c>
       <c r="J37" s="60"/>
-      <c r="K37" s="331">
+      <c r="K37" s="270">
         <v>44523</v>
       </c>
       <c r="L37" s="44">
@@ -10805,11 +10820,11 @@
       <c r="J39" s="60"/>
       <c r="K39" s="190"/>
       <c r="L39" s="61"/>
-      <c r="M39" s="272">
+      <c r="M39" s="305">
         <f>SUM(M5:M38)</f>
         <v>321168.83</v>
       </c>
-      <c r="N39" s="274">
+      <c r="N39" s="307">
         <f>SUM(N5:N38)</f>
         <v>467016</v>
       </c>
@@ -10835,8 +10850,8 @@
       <c r="J40" s="60"/>
       <c r="K40" s="41"/>
       <c r="L40" s="61"/>
-      <c r="M40" s="273"/>
-      <c r="N40" s="275"/>
+      <c r="M40" s="306"/>
+      <c r="N40" s="308"/>
       <c r="P40" s="34"/>
       <c r="Q40" s="13"/>
     </row>
@@ -11051,29 +11066,29 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="276" t="s">
+      <c r="H52" s="309" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="277"/>
+      <c r="I52" s="310"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="278">
+      <c r="K52" s="311">
         <f>I50+L50</f>
         <v>65231.97</v>
       </c>
-      <c r="L52" s="279"/>
-      <c r="M52" s="280">
+      <c r="L52" s="312"/>
+      <c r="M52" s="313">
         <f>N39+M39</f>
         <v>788184.83000000007</v>
       </c>
-      <c r="N52" s="281"/>
+      <c r="N52" s="314"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="D53" s="282" t="s">
+      <c r="D53" s="315" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="282"/>
+      <c r="E53" s="315"/>
       <c r="F53" s="101">
         <f>F50-K52-C50</f>
         <v>-17892.929999999935</v>
@@ -11084,27 +11099,27 @@
       <c r="Q53" s="13"/>
     </row>
     <row r="54" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D54" s="282" t="s">
+      <c r="D54" s="315" t="s">
         <v>101</v>
       </c>
-      <c r="E54" s="282"/>
+      <c r="E54" s="315"/>
       <c r="F54" s="96">
         <v>-706888.38</v>
       </c>
-      <c r="I54" s="283" t="s">
+      <c r="I54" s="316" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="284"/>
-      <c r="K54" s="285">
+      <c r="J54" s="317"/>
+      <c r="K54" s="318">
         <f>F56+F57+F58</f>
         <v>1417526.31</v>
       </c>
-      <c r="L54" s="286"/>
-      <c r="P54" s="294" t="s">
+      <c r="L54" s="319"/>
+      <c r="P54" s="324" t="s">
         <v>130</v>
       </c>
-      <c r="Q54" s="294"/>
-      <c r="R54" s="295"/>
+      <c r="Q54" s="324"/>
+      <c r="R54" s="254"/>
     </row>
     <row r="55" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D55" s="203" t="s">
@@ -11118,10 +11133,10 @@
       <c r="J55" s="106"/>
       <c r="K55" s="191"/>
       <c r="L55" s="107"/>
-      <c r="P55" s="296">
+      <c r="P55" s="255">
         <v>50000</v>
       </c>
-      <c r="Q55" s="317">
+      <c r="Q55" s="258">
         <v>44505</v>
       </c>
       <c r="R55" s="13"/>
@@ -11142,15 +11157,15 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="287">
+      <c r="K56" s="320">
         <f>-C4</f>
         <v>-567389.35</v>
       </c>
-      <c r="L56" s="288"/>
-      <c r="P56" s="296">
+      <c r="L56" s="321"/>
+      <c r="P56" s="255">
         <v>50000</v>
       </c>
-      <c r="Q56" s="317">
+      <c r="Q56" s="258">
         <v>44505</v>
       </c>
       <c r="R56" s="13"/>
@@ -11165,10 +11180,10 @@
       <c r="F57" s="111">
         <v>0</v>
       </c>
-      <c r="P57" s="296">
+      <c r="P57" s="255">
         <v>50000</v>
       </c>
-      <c r="Q57" s="317">
+      <c r="Q57" s="258">
         <v>44505</v>
       </c>
       <c r="R57" s="13"/>
@@ -11177,26 +11192,26 @@
       <c r="C58" s="112">
         <v>44535</v>
       </c>
-      <c r="D58" s="265" t="s">
+      <c r="D58" s="298" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="266"/>
+      <c r="E58" s="299"/>
       <c r="F58" s="113">
         <v>2142307.62</v>
       </c>
-      <c r="I58" s="267" t="s">
+      <c r="I58" s="300" t="s">
         <v>103</v>
       </c>
-      <c r="J58" s="268"/>
-      <c r="K58" s="269">
+      <c r="J58" s="301"/>
+      <c r="K58" s="302">
         <f>K54+K56</f>
         <v>850136.96000000008</v>
       </c>
-      <c r="L58" s="269"/>
-      <c r="P58" s="296">
+      <c r="L58" s="302"/>
+      <c r="P58" s="255">
         <v>100000</v>
       </c>
-      <c r="Q58" s="318">
+      <c r="Q58" s="259">
         <v>44509</v>
       </c>
       <c r="R58" s="13"/>
@@ -11207,10 +11222,10 @@
       <c r="E59" s="116"/>
       <c r="F59" s="117"/>
       <c r="J59" s="118"/>
-      <c r="P59" s="296">
+      <c r="P59" s="255">
         <v>215000</v>
       </c>
-      <c r="Q59" s="318">
+      <c r="Q59" s="259">
         <v>44510</v>
       </c>
       <c r="R59" s="13"/>
@@ -11220,10 +11235,10 @@
       <c r="J60" s="119"/>
       <c r="K60" s="192"/>
       <c r="L60" s="120"/>
-      <c r="P60" s="296">
+      <c r="P60" s="255">
         <v>200500</v>
       </c>
-      <c r="Q60" s="317">
+      <c r="Q60" s="258">
         <v>44517</v>
       </c>
       <c r="R60" s="13"/>
@@ -11239,10 +11254,10 @@
       <c r="L61" s="120"/>
       <c r="M61" s="124"/>
       <c r="N61" s="98"/>
-      <c r="P61" s="296">
+      <c r="P61" s="255">
         <v>260000</v>
       </c>
-      <c r="Q61" s="317">
+      <c r="Q61" s="258">
         <v>44523</v>
       </c>
       <c r="R61" s="13"/>
@@ -11253,10 +11268,10 @@
       <c r="E62" s="34"/>
       <c r="M62" s="124"/>
       <c r="N62" s="98"/>
-      <c r="P62" s="296">
+      <c r="P62" s="255">
         <v>9636</v>
       </c>
-      <c r="Q62" s="317">
+      <c r="Q62" s="258">
         <v>44533</v>
       </c>
       <c r="R62" s="13"/>
@@ -11268,10 +11283,10 @@
       <c r="F63" s="126"/>
       <c r="L63" s="127"/>
       <c r="M63" s="1"/>
-      <c r="P63" s="296">
-        <v>0</v>
-      </c>
-      <c r="Q63" s="317"/>
+      <c r="P63" s="255">
+        <v>0</v>
+      </c>
+      <c r="Q63" s="258"/>
       <c r="R63" s="13"/>
     </row>
     <row r="64" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -11279,10 +11294,10 @@
       <c r="C64" s="125"/>
       <c r="E64" s="34"/>
       <c r="M64" s="1"/>
-      <c r="P64" s="296">
-        <v>0</v>
-      </c>
-      <c r="Q64" s="317"/>
+      <c r="P64" s="255">
+        <v>0</v>
+      </c>
+      <c r="Q64" s="258"/>
       <c r="R64" s="13"/>
     </row>
     <row r="65" spans="2:18" x14ac:dyDescent="0.25">
@@ -11292,65 +11307,65 @@
       <c r="E65" s="34"/>
       <c r="F65" s="129"/>
       <c r="M65" s="1"/>
-      <c r="P65" s="296">
-        <v>0</v>
-      </c>
-      <c r="Q65" s="319"/>
-      <c r="R65" s="295"/>
+      <c r="P65" s="255">
+        <v>0</v>
+      </c>
+      <c r="Q65" s="260"/>
+      <c r="R65" s="254"/>
     </row>
     <row r="66" spans="2:18" x14ac:dyDescent="0.25">
       <c r="D66" s="128"/>
       <c r="E66" s="130"/>
       <c r="F66" s="34"/>
       <c r="M66" s="1"/>
-      <c r="P66" s="297">
-        <v>0</v>
-      </c>
-      <c r="Q66" s="317"/>
-      <c r="R66" s="295"/>
+      <c r="P66" s="256">
+        <v>0</v>
+      </c>
+      <c r="Q66" s="258"/>
+      <c r="R66" s="254"/>
     </row>
     <row r="67" spans="2:18" x14ac:dyDescent="0.25">
       <c r="D67" s="128"/>
       <c r="E67" s="130"/>
       <c r="F67" s="34"/>
       <c r="M67" s="1"/>
-      <c r="P67" s="298">
-        <v>0</v>
-      </c>
-      <c r="Q67" s="320"/>
-      <c r="R67" s="295"/>
+      <c r="P67" s="257">
+        <v>0</v>
+      </c>
+      <c r="Q67" s="261"/>
+      <c r="R67" s="254"/>
     </row>
     <row r="68" spans="2:18" x14ac:dyDescent="0.25">
       <c r="D68" s="128"/>
       <c r="E68" s="130"/>
       <c r="F68" s="34"/>
       <c r="M68" s="1"/>
-      <c r="P68" s="299">
+      <c r="P68" s="331">
         <f t="shared" ref="P68" si="3">SUM(P55:P67)</f>
         <v>935136</v>
       </c>
-      <c r="Q68" s="320"/>
-      <c r="R68" s="295"/>
+      <c r="Q68" s="261"/>
+      <c r="R68" s="254"/>
     </row>
     <row r="69" spans="2:18" x14ac:dyDescent="0.25">
       <c r="D69" s="128"/>
       <c r="E69" s="130"/>
       <c r="F69" s="34"/>
       <c r="M69" s="1"/>
-      <c r="P69" s="300"/>
+      <c r="P69" s="332"/>
       <c r="Q69" s="33"/>
-      <c r="R69" s="295"/>
+      <c r="R69" s="254"/>
     </row>
     <row r="70" spans="2:18" ht="17.25" x14ac:dyDescent="0.3">
       <c r="D70" s="128"/>
       <c r="E70" s="130"/>
       <c r="F70" s="34"/>
       <c r="M70" s="1"/>
-      <c r="P70" s="301" t="s">
+      <c r="P70" s="333" t="s">
         <v>131</v>
       </c>
-      <c r="Q70" s="302"/>
-      <c r="R70" s="295"/>
+      <c r="Q70" s="334"/>
+      <c r="R70" s="254"/>
     </row>
     <row r="71" spans="2:18" x14ac:dyDescent="0.25">
       <c r="D71" s="128"/>
@@ -11359,69 +11374,69 @@
       <c r="M71" s="1"/>
       <c r="P71" s="85"/>
       <c r="Q71" s="33"/>
-      <c r="R71" s="295"/>
+      <c r="R71" s="254"/>
     </row>
     <row r="72" spans="2:18" x14ac:dyDescent="0.25">
       <c r="D72" s="128"/>
       <c r="E72" s="130"/>
       <c r="F72" s="34"/>
       <c r="M72" s="1"/>
-      <c r="P72" s="303">
+      <c r="P72" s="335">
         <v>-53663.11</v>
       </c>
-      <c r="Q72" s="304"/>
-      <c r="R72" s="295"/>
+      <c r="Q72" s="336"/>
+      <c r="R72" s="254"/>
     </row>
     <row r="73" spans="2:18" x14ac:dyDescent="0.25">
       <c r="D73" s="128"/>
       <c r="E73" s="130"/>
       <c r="F73" s="34"/>
       <c r="M73" s="1"/>
-      <c r="P73" s="305"/>
-      <c r="Q73" s="306"/>
-      <c r="R73" s="295"/>
+      <c r="P73" s="337"/>
+      <c r="Q73" s="338"/>
+      <c r="R73" s="254"/>
     </row>
     <row r="74" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D74" s="128"/>
       <c r="E74" s="130"/>
       <c r="F74" s="34"/>
       <c r="M74" s="1"/>
-      <c r="P74" s="313">
-        <v>0</v>
-      </c>
-      <c r="Q74" s="314"/>
-      <c r="R74" s="295"/>
+      <c r="P74" s="339">
+        <v>0</v>
+      </c>
+      <c r="Q74" s="340"/>
+      <c r="R74" s="254"/>
     </row>
     <row r="75" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D75" s="128"/>
       <c r="E75" s="130"/>
       <c r="F75" s="34"/>
       <c r="M75" s="1"/>
-      <c r="P75" s="315">
-        <v>0</v>
-      </c>
-      <c r="Q75" s="316"/>
-      <c r="R75" s="295"/>
+      <c r="P75" s="341">
+        <v>0</v>
+      </c>
+      <c r="Q75" s="342"/>
+      <c r="R75" s="254"/>
     </row>
     <row r="76" spans="2:18" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D76" s="128"/>
       <c r="E76" s="130"/>
       <c r="F76" s="34"/>
       <c r="M76" s="1"/>
-      <c r="P76" s="307">
+      <c r="P76" s="325">
         <f>SUM(P75+P74+P72)</f>
         <v>-53663.11</v>
       </c>
-      <c r="Q76" s="308"/>
-      <c r="R76" s="309"/>
+      <c r="Q76" s="326"/>
+      <c r="R76" s="329"/>
     </row>
     <row r="77" spans="2:18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D77" s="128"/>
       <c r="E77" s="130"/>
       <c r="F77" s="34"/>
-      <c r="P77" s="310"/>
-      <c r="Q77" s="311"/>
-      <c r="R77" s="312"/>
+      <c r="P77" s="327"/>
+      <c r="Q77" s="328"/>
+      <c r="R77" s="330"/>
     </row>
     <row r="78" spans="2:18" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D78" s="128"/>
@@ -11483,8 +11498,8 @@
   </sheetPr>
   <dimension ref="A1:N134"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11565,13 +11580,13 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="324" t="s">
+      <c r="A3" s="265" t="s">
         <v>132</v>
       </c>
-      <c r="B3" s="325" t="s">
+      <c r="B3" s="283" t="s">
         <v>133</v>
       </c>
-      <c r="C3" s="326">
+      <c r="C3" s="284">
         <v>15652.4</v>
       </c>
       <c r="D3" s="136"/>
@@ -11591,13 +11606,13 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="328" t="s">
+      <c r="A4" s="267" t="s">
         <v>132</v>
       </c>
-      <c r="B4" s="329" t="s">
+      <c r="B4" s="285" t="s">
         <v>134</v>
       </c>
-      <c r="C4" s="111">
+      <c r="C4" s="286">
         <v>6679.8</v>
       </c>
       <c r="D4" s="136"/>
@@ -11618,13 +11633,13 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="328" t="s">
+      <c r="A5" s="267" t="s">
         <v>135</v>
       </c>
-      <c r="B5" s="329" t="s">
+      <c r="B5" s="285" t="s">
         <v>136</v>
       </c>
-      <c r="C5" s="111">
+      <c r="C5" s="286">
         <v>18704.419999999998</v>
       </c>
       <c r="D5" s="136"/>
@@ -11644,13 +11659,13 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="328" t="s">
+      <c r="A6" s="267" t="s">
         <v>135</v>
       </c>
-      <c r="B6" s="329" t="s">
+      <c r="B6" s="285" t="s">
         <v>137</v>
       </c>
-      <c r="C6" s="111">
+      <c r="C6" s="286">
         <v>840</v>
       </c>
       <c r="D6" s="136"/>
@@ -11670,10 +11685,10 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="328" t="s">
+      <c r="A7" s="267" t="s">
         <v>138</v>
       </c>
-      <c r="B7" s="329" t="s">
+      <c r="B7" s="268" t="s">
         <v>139</v>
       </c>
       <c r="C7" s="111">
@@ -11696,10 +11711,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="328" t="s">
+      <c r="A8" s="267" t="s">
         <v>138</v>
       </c>
-      <c r="B8" s="329" t="s">
+      <c r="B8" s="268" t="s">
         <v>140</v>
       </c>
       <c r="C8" s="111">
@@ -11722,10 +11737,10 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="328" t="s">
+      <c r="A9" s="267" t="s">
         <v>141</v>
       </c>
-      <c r="B9" s="329" t="s">
+      <c r="B9" s="268" t="s">
         <v>142</v>
       </c>
       <c r="C9" s="111">
@@ -11748,10 +11763,10 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="328" t="s">
+      <c r="A10" s="267" t="s">
         <v>141</v>
       </c>
-      <c r="B10" s="329" t="s">
+      <c r="B10" s="268" t="s">
         <v>143</v>
       </c>
       <c r="C10" s="111">
@@ -11775,10 +11790,10 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="328" t="s">
+      <c r="A11" s="267" t="s">
         <v>144</v>
       </c>
-      <c r="B11" s="329" t="s">
+      <c r="B11" s="268" t="s">
         <v>145</v>
       </c>
       <c r="C11" s="111">
@@ -11801,10 +11816,10 @@
       </c>
     </row>
     <row r="12" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="328" t="s">
+      <c r="A12" s="267" t="s">
         <v>146</v>
       </c>
-      <c r="B12" s="329" t="s">
+      <c r="B12" s="268" t="s">
         <v>147</v>
       </c>
       <c r="C12" s="111">
@@ -11827,10 +11842,10 @@
       </c>
     </row>
     <row r="13" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="328" t="s">
+      <c r="A13" s="267" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="329" t="s">
+      <c r="B13" s="268" t="s">
         <v>148</v>
       </c>
       <c r="C13" s="111">
@@ -11853,10 +11868,10 @@
       </c>
     </row>
     <row r="14" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="328" t="s">
+      <c r="A14" s="267" t="s">
         <v>149</v>
       </c>
-      <c r="B14" s="329" t="s">
+      <c r="B14" s="268" t="s">
         <v>150</v>
       </c>
       <c r="C14" s="111">
@@ -11879,10 +11894,10 @@
       </c>
     </row>
     <row r="15" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="328" t="s">
+      <c r="A15" s="267" t="s">
         <v>151</v>
       </c>
-      <c r="B15" s="329" t="s">
+      <c r="B15" s="268" t="s">
         <v>152</v>
       </c>
       <c r="C15" s="111">
@@ -11905,10 +11920,10 @@
       </c>
     </row>
     <row r="16" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="328" t="s">
+      <c r="A16" s="267" t="s">
         <v>151</v>
       </c>
-      <c r="B16" s="329" t="s">
+      <c r="B16" s="268" t="s">
         <v>153</v>
       </c>
       <c r="C16" s="111">
@@ -11931,10 +11946,10 @@
       </c>
     </row>
     <row r="17" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="328" t="s">
+      <c r="A17" s="267" t="s">
         <v>154</v>
       </c>
-      <c r="B17" s="329" t="s">
+      <c r="B17" s="268" t="s">
         <v>155</v>
       </c>
       <c r="C17" s="111">
@@ -11957,10 +11972,10 @@
       </c>
     </row>
     <row r="18" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="328" t="s">
+      <c r="A18" s="267" t="s">
         <v>154</v>
       </c>
-      <c r="B18" s="329" t="s">
+      <c r="B18" s="268" t="s">
         <v>156</v>
       </c>
       <c r="C18" s="111">
@@ -11983,10 +11998,10 @@
       </c>
     </row>
     <row r="19" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="328" t="s">
+      <c r="A19" s="267" t="s">
         <v>154</v>
       </c>
-      <c r="B19" s="329" t="s">
+      <c r="B19" s="268" t="s">
         <v>157</v>
       </c>
       <c r="C19" s="111">
@@ -12009,10 +12024,10 @@
       </c>
     </row>
     <row r="20" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="328" t="s">
+      <c r="A20" s="267" t="s">
         <v>158</v>
       </c>
-      <c r="B20" s="329" t="s">
+      <c r="B20" s="268" t="s">
         <v>159</v>
       </c>
       <c r="C20" s="111">
@@ -12035,10 +12050,10 @@
       </c>
     </row>
     <row r="21" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="328" t="s">
+      <c r="A21" s="267" t="s">
         <v>158</v>
       </c>
-      <c r="B21" s="329" t="s">
+      <c r="B21" s="268" t="s">
         <v>160</v>
       </c>
       <c r="C21" s="111">
@@ -12061,10 +12076,10 @@
       </c>
     </row>
     <row r="22" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A22" s="328" t="s">
+      <c r="A22" s="267" t="s">
         <v>161</v>
       </c>
-      <c r="B22" s="329" t="s">
+      <c r="B22" s="268" t="s">
         <v>162</v>
       </c>
       <c r="C22" s="111">
@@ -12088,10 +12103,10 @@
       </c>
     </row>
     <row r="23" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="328" t="s">
+      <c r="A23" s="267" t="s">
         <v>161</v>
       </c>
-      <c r="B23" s="329" t="s">
+      <c r="B23" s="268" t="s">
         <v>163</v>
       </c>
       <c r="C23" s="111">
@@ -12114,10 +12129,10 @@
       </c>
     </row>
     <row r="24" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="328" t="s">
+      <c r="A24" s="267" t="s">
         <v>164</v>
       </c>
-      <c r="B24" s="329" t="s">
+      <c r="B24" s="268" t="s">
         <v>165</v>
       </c>
       <c r="C24" s="111">
@@ -12140,10 +12155,10 @@
       </c>
     </row>
     <row r="25" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="328" t="s">
+      <c r="A25" s="267" t="s">
         <v>164</v>
       </c>
-      <c r="B25" s="329" t="s">
+      <c r="B25" s="268" t="s">
         <v>166</v>
       </c>
       <c r="C25" s="111">
@@ -12166,16 +12181,18 @@
       </c>
     </row>
     <row r="26" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="328" t="s">
+      <c r="A26" s="267" t="s">
         <v>164</v>
       </c>
-      <c r="B26" s="329" t="s">
+      <c r="B26" s="268" t="s">
         <v>167</v>
       </c>
       <c r="C26" s="111">
         <v>34909.9</v>
       </c>
-      <c r="D26" s="140"/>
+      <c r="D26" s="140" t="s">
+        <v>202</v>
+      </c>
       <c r="E26" s="69"/>
       <c r="F26" s="137">
         <f t="shared" si="0"/>
@@ -12192,10 +12209,10 @@
       </c>
     </row>
     <row r="27" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="328" t="s">
+      <c r="A27" s="267" t="s">
         <v>164</v>
       </c>
-      <c r="B27" s="329" t="s">
+      <c r="B27" s="268" t="s">
         <v>168</v>
       </c>
       <c r="C27" s="111">
@@ -12218,10 +12235,10 @@
       </c>
     </row>
     <row r="28" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="328" t="s">
+      <c r="A28" s="267" t="s">
         <v>169</v>
       </c>
-      <c r="B28" s="329" t="s">
+      <c r="B28" s="268" t="s">
         <v>170</v>
       </c>
       <c r="C28" s="111">
@@ -12244,10 +12261,10 @@
       </c>
     </row>
     <row r="29" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="328" t="s">
+      <c r="A29" s="267" t="s">
         <v>169</v>
       </c>
-      <c r="B29" s="329" t="s">
+      <c r="B29" s="268" t="s">
         <v>171</v>
       </c>
       <c r="C29" s="111">
@@ -12270,10 +12287,10 @@
       </c>
     </row>
     <row r="30" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A30" s="328" t="s">
+      <c r="A30" s="267" t="s">
         <v>172</v>
       </c>
-      <c r="B30" s="329" t="s">
+      <c r="B30" s="268" t="s">
         <v>173</v>
       </c>
       <c r="C30" s="111">
@@ -12297,10 +12314,10 @@
       </c>
     </row>
     <row r="31" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="328" t="s">
+      <c r="A31" s="267" t="s">
         <v>174</v>
       </c>
-      <c r="B31" s="329" t="s">
+      <c r="B31" s="268" t="s">
         <v>175</v>
       </c>
       <c r="C31" s="111">
@@ -12323,10 +12340,10 @@
       </c>
     </row>
     <row r="32" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="328" t="s">
+      <c r="A32" s="267" t="s">
         <v>174</v>
       </c>
-      <c r="B32" s="329" t="s">
+      <c r="B32" s="268" t="s">
         <v>176</v>
       </c>
       <c r="C32" s="111">
@@ -12349,10 +12366,10 @@
       </c>
     </row>
     <row r="33" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="328" t="s">
+      <c r="A33" s="267" t="s">
         <v>177</v>
       </c>
-      <c r="B33" s="329" t="s">
+      <c r="B33" s="268" t="s">
         <v>178</v>
       </c>
       <c r="C33" s="111">
@@ -12375,10 +12392,10 @@
       </c>
     </row>
     <row r="34" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="328" t="s">
+      <c r="A34" s="267" t="s">
         <v>177</v>
       </c>
-      <c r="B34" s="329" t="s">
+      <c r="B34" s="268" t="s">
         <v>179</v>
       </c>
       <c r="C34" s="111">
@@ -12401,16 +12418,16 @@
       </c>
     </row>
     <row r="35" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="328" t="s">
+      <c r="A35" s="267" t="s">
         <v>180</v>
       </c>
-      <c r="B35" s="329" t="s">
+      <c r="B35" s="346" t="s">
         <v>181</v>
       </c>
-      <c r="C35" s="111">
+      <c r="C35" s="347">
         <v>9701.98</v>
       </c>
-      <c r="D35" s="140"/>
+      <c r="D35" s="348"/>
       <c r="E35" s="69"/>
       <c r="F35" s="137">
         <f t="shared" si="0"/>
@@ -12427,10 +12444,10 @@
       </c>
     </row>
     <row r="36" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="328" t="s">
+      <c r="A36" s="267" t="s">
         <v>180</v>
       </c>
-      <c r="B36" s="329" t="s">
+      <c r="B36" s="268" t="s">
         <v>182</v>
       </c>
       <c r="C36" s="111">
@@ -12453,10 +12470,10 @@
       </c>
     </row>
     <row r="37" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="328" t="s">
+      <c r="A37" s="267" t="s">
         <v>183</v>
       </c>
-      <c r="B37" s="329" t="s">
+      <c r="B37" s="268" t="s">
         <v>184</v>
       </c>
       <c r="C37" s="111">
@@ -12479,10 +12496,10 @@
       </c>
     </row>
     <row r="38" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="328" t="s">
+      <c r="A38" s="267" t="s">
         <v>183</v>
       </c>
-      <c r="B38" s="329" t="s">
+      <c r="B38" s="268" t="s">
         <v>185</v>
       </c>
       <c r="C38" s="111">
@@ -12505,10 +12522,10 @@
       </c>
     </row>
     <row r="39" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="328" t="s">
+      <c r="A39" s="267" t="s">
         <v>186</v>
       </c>
-      <c r="B39" s="329" t="s">
+      <c r="B39" s="268" t="s">
         <v>187</v>
       </c>
       <c r="C39" s="111">
@@ -12531,10 +12548,10 @@
       </c>
     </row>
     <row r="40" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="328" t="s">
+      <c r="A40" s="267" t="s">
         <v>188</v>
       </c>
-      <c r="B40" s="329" t="s">
+      <c r="B40" s="268" t="s">
         <v>189</v>
       </c>
       <c r="C40" s="111">
@@ -12557,10 +12574,10 @@
       </c>
     </row>
     <row r="41" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="328" t="s">
+      <c r="A41" s="267" t="s">
         <v>188</v>
       </c>
-      <c r="B41" s="329" t="s">
+      <c r="B41" s="268" t="s">
         <v>190</v>
       </c>
       <c r="C41" s="111">
@@ -12583,10 +12600,10 @@
       </c>
     </row>
     <row r="42" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="328" t="s">
+      <c r="A42" s="267" t="s">
         <v>191</v>
       </c>
-      <c r="B42" s="329" t="s">
+      <c r="B42" s="268" t="s">
         <v>192</v>
       </c>
       <c r="C42" s="111">
@@ -12609,10 +12626,10 @@
       </c>
     </row>
     <row r="43" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="328" t="s">
+      <c r="A43" s="267" t="s">
         <v>193</v>
       </c>
-      <c r="B43" s="329" t="s">
+      <c r="B43" s="268" t="s">
         <v>194</v>
       </c>
       <c r="C43" s="111">
@@ -12635,10 +12652,10 @@
       </c>
     </row>
     <row r="44" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="328" t="s">
+      <c r="A44" s="267" t="s">
         <v>193</v>
       </c>
-      <c r="B44" s="329" t="s">
+      <c r="B44" s="268" t="s">
         <v>195</v>
       </c>
       <c r="C44" s="111">
@@ -12661,7 +12678,7 @@
       </c>
     </row>
     <row r="45" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="328" t="s">
+      <c r="A45" s="267" t="s">
         <v>196</v>
       </c>
       <c r="B45" s="57" t="s">
@@ -12687,13 +12704,13 @@
       </c>
     </row>
     <row r="46" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="328" t="s">
+      <c r="A46" s="267" t="s">
         <v>196</v>
       </c>
       <c r="B46" s="57" t="s">
         <v>198</v>
       </c>
-      <c r="C46" s="323">
+      <c r="C46" s="264">
         <v>104.4</v>
       </c>
       <c r="D46" s="140"/>
@@ -12713,13 +12730,13 @@
       </c>
     </row>
     <row r="47" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="328" t="s">
+      <c r="A47" s="267" t="s">
         <v>196</v>
       </c>
       <c r="B47" s="57" t="s">
         <v>199</v>
       </c>
-      <c r="C47" s="323">
+      <c r="C47" s="264">
         <v>702</v>
       </c>
       <c r="D47" s="140"/>
@@ -12739,13 +12756,13 @@
       </c>
     </row>
     <row r="48" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="322">
+      <c r="A48" s="263">
         <v>44534</v>
       </c>
-      <c r="B48" s="321" t="s">
+      <c r="B48" s="262" t="s">
         <v>200</v>
       </c>
-      <c r="C48" s="327">
+      <c r="C48" s="266">
         <v>73956.800000000003</v>
       </c>
       <c r="D48" s="140"/>
@@ -14152,12 +14169,12 @@
     <row r="42" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="43" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="155"/>
-      <c r="B43" s="291" t="s">
+      <c r="B43" s="343" t="s">
         <v>25</v>
       </c>
-      <c r="C43" s="292"/>
-      <c r="D43" s="292"/>
-      <c r="E43" s="293"/>
+      <c r="C43" s="344"/>
+      <c r="D43" s="344"/>
+      <c r="E43" s="345"/>
       <c r="F43" s="1"/>
     </row>
     <row r="44" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
cierre 14 Dic 2021
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 11  NOVIEMBRE 2021/BALANCE    ZAVALETA   NOVIEMBRE    2021.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 11  NOVIEMBRE 2021/BALANCE    ZAVALETA   NOVIEMBRE    2021.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4035" yWindow="0" windowWidth="16335" windowHeight="11070" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="4035" yWindow="0" windowWidth="16335" windowHeight="11070" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="OCTUBRE      2 0 2 1     " sheetId="1" r:id="rId1"/>
@@ -2240,7 +2240,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="350">
+  <cellXfs count="353">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -2822,183 +2822,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="3" fillId="6" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="6" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="6" borderId="51" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="6" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="50" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="43" fillId="6" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="43" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="7" fontId="33" fillId="6" borderId="72" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="33" fillId="6" borderId="73" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="33" fillId="6" borderId="75" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="33" fillId="6" borderId="76" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="6" borderId="74" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="6" borderId="77" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="15" borderId="65" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="15" borderId="66" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="9" borderId="67" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="9" borderId="64" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="33" fillId="13" borderId="68" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="33" fillId="13" borderId="69" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="33" fillId="13" borderId="70" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="33" fillId="13" borderId="71" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="7" fontId="11" fillId="0" borderId="67" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="7" fontId="11" fillId="0" borderId="64" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="7" fontId="11" fillId="0" borderId="68" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="7" fontId="11" fillId="0" borderId="69" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3007,6 +2830,186 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="38" fillId="3" borderId="53" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="6" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="6" borderId="51" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="6" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="50" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="43" fillId="6" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="43" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="7" fontId="33" fillId="6" borderId="72" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="33" fillId="6" borderId="73" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="33" fillId="6" borderId="75" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="33" fillId="6" borderId="76" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="6" borderId="74" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="6" borderId="77" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="15" borderId="65" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="15" borderId="66" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="9" borderId="67" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="9" borderId="64" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="33" fillId="13" borderId="68" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="33" fillId="13" borderId="69" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="33" fillId="13" borderId="70" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="33" fillId="13" borderId="71" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="11" fillId="0" borderId="67" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="11" fillId="0" borderId="64" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="11" fillId="0" borderId="68" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="11" fillId="0" borderId="69" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="16" fillId="3" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="2" fillId="3" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -4179,23 +4182,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="287"/>
-      <c r="C1" s="289" t="s">
+      <c r="B1" s="315"/>
+      <c r="C1" s="317" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="290"/>
-      <c r="E1" s="290"/>
-      <c r="F1" s="290"/>
-      <c r="G1" s="290"/>
-      <c r="H1" s="290"/>
-      <c r="I1" s="290"/>
-      <c r="J1" s="290"/>
-      <c r="K1" s="290"/>
-      <c r="L1" s="290"/>
-      <c r="M1" s="290"/>
+      <c r="D1" s="318"/>
+      <c r="E1" s="318"/>
+      <c r="F1" s="318"/>
+      <c r="G1" s="318"/>
+      <c r="H1" s="318"/>
+      <c r="I1" s="318"/>
+      <c r="J1" s="318"/>
+      <c r="K1" s="318"/>
+      <c r="L1" s="318"/>
+      <c r="M1" s="318"/>
     </row>
     <row r="2" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="288"/>
+      <c r="B2" s="316"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -4205,17 +4208,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:19" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="291" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="292"/>
+      <c r="B3" s="319" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="320"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="293" t="s">
+      <c r="H3" s="321" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="293"/>
+      <c r="I3" s="321"/>
       <c r="K3" s="178"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
@@ -4229,14 +4232,14 @@
         <v>0</v>
       </c>
       <c r="D4" s="18"/>
-      <c r="E4" s="294" t="s">
+      <c r="E4" s="322" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="295"/>
-      <c r="H4" s="296" t="s">
+      <c r="F4" s="323"/>
+      <c r="H4" s="324" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="297"/>
+      <c r="I4" s="325"/>
       <c r="J4" s="19"/>
       <c r="K4" s="179"/>
       <c r="L4" s="20"/>
@@ -4246,10 +4249,10 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="303" t="s">
+      <c r="P4" s="296" t="s">
         <v>6</v>
       </c>
-      <c r="Q4" s="304"/>
+      <c r="Q4" s="297"/>
     </row>
     <row r="5" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
@@ -5690,11 +5693,11 @@
       <c r="J39" s="60"/>
       <c r="K39" s="190"/>
       <c r="L39" s="61"/>
-      <c r="M39" s="305">
+      <c r="M39" s="298">
         <f>SUM(M5:M38)</f>
         <v>247061</v>
       </c>
-      <c r="N39" s="307">
+      <c r="N39" s="300">
         <f>SUM(N5:N38)</f>
         <v>172863</v>
       </c>
@@ -5720,8 +5723,8 @@
       <c r="J40" s="60"/>
       <c r="K40" s="41"/>
       <c r="L40" s="61"/>
-      <c r="M40" s="306"/>
-      <c r="N40" s="308"/>
+      <c r="M40" s="299"/>
+      <c r="N40" s="301"/>
       <c r="P40" s="34"/>
       <c r="Q40" s="9"/>
     </row>
@@ -5936,29 +5939,29 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="309" t="s">
+      <c r="H52" s="302" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="310"/>
+      <c r="I52" s="303"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="311">
+      <c r="K52" s="304">
         <f>I50+L50</f>
         <v>53873.49</v>
       </c>
-      <c r="L52" s="312"/>
-      <c r="M52" s="313">
+      <c r="L52" s="305"/>
+      <c r="M52" s="306">
         <f>N39+M39</f>
         <v>419924</v>
       </c>
-      <c r="N52" s="314"/>
+      <c r="N52" s="307"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D53" s="315" t="s">
+      <c r="D53" s="308" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="315"/>
+      <c r="E53" s="308"/>
       <c r="F53" s="101">
         <f>F50-K52-C50</f>
         <v>471038.61</v>
@@ -5969,22 +5972,22 @@
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="315" t="s">
+      <c r="D54" s="308" t="s">
         <v>101</v>
       </c>
-      <c r="E54" s="315"/>
+      <c r="E54" s="308"/>
       <c r="F54" s="96">
         <v>-549976.4</v>
       </c>
-      <c r="I54" s="316" t="s">
+      <c r="I54" s="309" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="317"/>
-      <c r="K54" s="318">
+      <c r="J54" s="310"/>
+      <c r="K54" s="311">
         <f>F56+F57+F58</f>
         <v>-24577.400000000023</v>
       </c>
-      <c r="L54" s="319"/>
+      <c r="L54" s="312"/>
       <c r="P54" s="34"/>
       <c r="Q54" s="9"/>
     </row>
@@ -6017,11 +6020,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="320">
+      <c r="K56" s="313">
         <f>-C4</f>
         <v>0</v>
       </c>
-      <c r="L56" s="321"/>
+      <c r="L56" s="314"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -6038,22 +6041,22 @@
       <c r="C58" s="112">
         <v>44507</v>
       </c>
-      <c r="D58" s="298" t="s">
+      <c r="D58" s="291" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="299"/>
+      <c r="E58" s="292"/>
       <c r="F58" s="113">
         <v>567389.35</v>
       </c>
-      <c r="I58" s="300" t="s">
+      <c r="I58" s="293" t="s">
         <v>103</v>
       </c>
-      <c r="J58" s="301"/>
-      <c r="K58" s="302">
+      <c r="J58" s="294"/>
+      <c r="K58" s="295">
         <f>K54+K56</f>
         <v>-24577.400000000023</v>
       </c>
-      <c r="L58" s="302"/>
+      <c r="L58" s="295"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -6197,6 +6200,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="I58:J58"/>
     <mergeCell ref="K58:L58"/>
@@ -6211,12 +6220,6 @@
     <mergeCell ref="I54:J54"/>
     <mergeCell ref="K54:L54"/>
     <mergeCell ref="K56:L56"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.15748031496062992" top="0.35433070866141736" bottom="0.31496062992125984" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="75" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -6759,7 +6762,7 @@
       <c r="E16" s="69">
         <v>145000</v>
       </c>
-      <c r="F16" s="349">
+      <c r="F16" s="290">
         <f t="shared" si="0"/>
         <v>146930.89999999991</v>
       </c>
@@ -7553,7 +7556,7 @@
       <c r="A41" s="140">
         <v>44507</v>
       </c>
-      <c r="B41" s="322" t="s">
+      <c r="B41" s="326" t="s">
         <v>98</v>
       </c>
       <c r="C41" s="204">
@@ -7585,7 +7588,7 @@
       <c r="A42" s="140" t="s">
         <v>99</v>
       </c>
-      <c r="B42" s="323"/>
+      <c r="B42" s="327"/>
       <c r="C42" s="143">
         <v>0</v>
       </c>
@@ -9144,8 +9147,8 @@
   </sheetPr>
   <dimension ref="A1:U80"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="J60" sqref="J60"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -9170,23 +9173,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="287"/>
-      <c r="C1" s="289" t="s">
+      <c r="B1" s="315"/>
+      <c r="C1" s="317" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="290"/>
-      <c r="E1" s="290"/>
-      <c r="F1" s="290"/>
-      <c r="G1" s="290"/>
-      <c r="H1" s="290"/>
-      <c r="I1" s="290"/>
-      <c r="J1" s="290"/>
-      <c r="K1" s="290"/>
-      <c r="L1" s="290"/>
-      <c r="M1" s="290"/>
+      <c r="D1" s="318"/>
+      <c r="E1" s="318"/>
+      <c r="F1" s="318"/>
+      <c r="G1" s="318"/>
+      <c r="H1" s="318"/>
+      <c r="I1" s="318"/>
+      <c r="J1" s="318"/>
+      <c r="K1" s="318"/>
+      <c r="L1" s="318"/>
+      <c r="M1" s="318"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="288"/>
+      <c r="B2" s="316"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -9196,17 +9199,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="291" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="292"/>
+      <c r="B3" s="319" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="320"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="293" t="s">
+      <c r="H3" s="321" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="293"/>
+      <c r="I3" s="321"/>
       <c r="K3" s="178"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
@@ -9222,14 +9225,14 @@
       <c r="D4" s="18">
         <v>44507</v>
       </c>
-      <c r="E4" s="294" t="s">
+      <c r="E4" s="322" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="295"/>
-      <c r="H4" s="296" t="s">
+      <c r="F4" s="323"/>
+      <c r="H4" s="324" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="297"/>
+      <c r="I4" s="325"/>
       <c r="J4" s="19"/>
       <c r="K4" s="179"/>
       <c r="L4" s="20"/>
@@ -9239,10 +9242,10 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="303" t="s">
+      <c r="P4" s="296" t="s">
         <v>6</v>
       </c>
-      <c r="Q4" s="304"/>
+      <c r="Q4" s="297"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
@@ -9672,13 +9675,13 @@
       <c r="J13" s="37"/>
       <c r="K13" s="38"/>
       <c r="L13" s="39"/>
-      <c r="M13" s="32">
-        <v>0</v>
-      </c>
-      <c r="N13" s="33">
+      <c r="M13" s="350">
+        <v>0</v>
+      </c>
+      <c r="N13" s="351">
         <v>21106</v>
       </c>
-      <c r="O13" s="2"/>
+      <c r="O13" s="352"/>
       <c r="P13" s="69">
         <f t="shared" si="2"/>
         <v>23882.36</v>
@@ -10820,11 +10823,11 @@
       <c r="J39" s="60"/>
       <c r="K39" s="190"/>
       <c r="L39" s="61"/>
-      <c r="M39" s="305">
+      <c r="M39" s="298">
         <f>SUM(M5:M38)</f>
         <v>321168.83</v>
       </c>
-      <c r="N39" s="307">
+      <c r="N39" s="300">
         <f>SUM(N5:N38)</f>
         <v>467016</v>
       </c>
@@ -10850,8 +10853,8 @@
       <c r="J40" s="60"/>
       <c r="K40" s="41"/>
       <c r="L40" s="61"/>
-      <c r="M40" s="306"/>
-      <c r="N40" s="308"/>
+      <c r="M40" s="299"/>
+      <c r="N40" s="301"/>
       <c r="P40" s="34"/>
       <c r="Q40" s="13"/>
     </row>
@@ -11066,29 +11069,29 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="309" t="s">
+      <c r="H52" s="302" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="310"/>
+      <c r="I52" s="303"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="311">
+      <c r="K52" s="304">
         <f>I50+L50</f>
         <v>65231.97</v>
       </c>
-      <c r="L52" s="312"/>
-      <c r="M52" s="313">
+      <c r="L52" s="305"/>
+      <c r="M52" s="306">
         <f>N39+M39</f>
         <v>788184.83000000007</v>
       </c>
-      <c r="N52" s="314"/>
+      <c r="N52" s="307"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="D53" s="315" t="s">
+      <c r="D53" s="308" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="315"/>
+      <c r="E53" s="308"/>
       <c r="F53" s="101">
         <f>F50-K52-C50</f>
         <v>-17892.929999999935</v>
@@ -11099,26 +11102,26 @@
       <c r="Q53" s="13"/>
     </row>
     <row r="54" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D54" s="315" t="s">
+      <c r="D54" s="308" t="s">
         <v>101</v>
       </c>
-      <c r="E54" s="315"/>
+      <c r="E54" s="308"/>
       <c r="F54" s="96">
         <v>-706888.38</v>
       </c>
-      <c r="I54" s="316" t="s">
+      <c r="I54" s="309" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="317"/>
-      <c r="K54" s="318">
+      <c r="J54" s="310"/>
+      <c r="K54" s="311">
         <f>F56+F57+F58</f>
         <v>1417526.31</v>
       </c>
-      <c r="L54" s="319"/>
-      <c r="P54" s="324" t="s">
+      <c r="L54" s="312"/>
+      <c r="P54" s="346" t="s">
         <v>130</v>
       </c>
-      <c r="Q54" s="324"/>
+      <c r="Q54" s="346"/>
       <c r="R54" s="254"/>
     </row>
     <row r="55" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -11157,11 +11160,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="320">
+      <c r="K56" s="313">
         <f>-C4</f>
         <v>-567389.35</v>
       </c>
-      <c r="L56" s="321"/>
+      <c r="L56" s="314"/>
       <c r="P56" s="255">
         <v>50000</v>
       </c>
@@ -11192,22 +11195,22 @@
       <c r="C58" s="112">
         <v>44535</v>
       </c>
-      <c r="D58" s="298" t="s">
+      <c r="D58" s="291" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="299"/>
+      <c r="E58" s="292"/>
       <c r="F58" s="113">
         <v>2142307.62</v>
       </c>
-      <c r="I58" s="300" t="s">
+      <c r="I58" s="293" t="s">
         <v>103</v>
       </c>
-      <c r="J58" s="301"/>
-      <c r="K58" s="302">
+      <c r="J58" s="294"/>
+      <c r="K58" s="295">
         <f>K54+K56</f>
         <v>850136.96000000008</v>
       </c>
-      <c r="L58" s="302"/>
+      <c r="L58" s="295"/>
       <c r="P58" s="255">
         <v>100000</v>
       </c>
@@ -11340,7 +11343,7 @@
       <c r="E68" s="130"/>
       <c r="F68" s="34"/>
       <c r="M68" s="1"/>
-      <c r="P68" s="331">
+      <c r="P68" s="334">
         <f t="shared" ref="P68" si="3">SUM(P55:P67)</f>
         <v>935136</v>
       </c>
@@ -11352,7 +11355,7 @@
       <c r="E69" s="130"/>
       <c r="F69" s="34"/>
       <c r="M69" s="1"/>
-      <c r="P69" s="332"/>
+      <c r="P69" s="335"/>
       <c r="Q69" s="33"/>
       <c r="R69" s="254"/>
     </row>
@@ -11361,10 +11364,10 @@
       <c r="E70" s="130"/>
       <c r="F70" s="34"/>
       <c r="M70" s="1"/>
-      <c r="P70" s="333" t="s">
+      <c r="P70" s="336" t="s">
         <v>131</v>
       </c>
-      <c r="Q70" s="334"/>
+      <c r="Q70" s="337"/>
       <c r="R70" s="254"/>
     </row>
     <row r="71" spans="2:18" x14ac:dyDescent="0.25">
@@ -11381,10 +11384,10 @@
       <c r="E72" s="130"/>
       <c r="F72" s="34"/>
       <c r="M72" s="1"/>
-      <c r="P72" s="335">
+      <c r="P72" s="338">
         <v>-53663.11</v>
       </c>
-      <c r="Q72" s="336"/>
+      <c r="Q72" s="339"/>
       <c r="R72" s="254"/>
     </row>
     <row r="73" spans="2:18" x14ac:dyDescent="0.25">
@@ -11392,8 +11395,8 @@
       <c r="E73" s="130"/>
       <c r="F73" s="34"/>
       <c r="M73" s="1"/>
-      <c r="P73" s="337"/>
-      <c r="Q73" s="338"/>
+      <c r="P73" s="340"/>
+      <c r="Q73" s="341"/>
       <c r="R73" s="254"/>
     </row>
     <row r="74" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
@@ -11401,10 +11404,10 @@
       <c r="E74" s="130"/>
       <c r="F74" s="34"/>
       <c r="M74" s="1"/>
-      <c r="P74" s="339">
-        <v>0</v>
-      </c>
-      <c r="Q74" s="340"/>
+      <c r="P74" s="342">
+        <v>0</v>
+      </c>
+      <c r="Q74" s="343"/>
       <c r="R74" s="254"/>
     </row>
     <row r="75" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -11412,10 +11415,10 @@
       <c r="E75" s="130"/>
       <c r="F75" s="34"/>
       <c r="M75" s="1"/>
-      <c r="P75" s="341">
-        <v>0</v>
-      </c>
-      <c r="Q75" s="342"/>
+      <c r="P75" s="344">
+        <v>0</v>
+      </c>
+      <c r="Q75" s="345"/>
       <c r="R75" s="254"/>
     </row>
     <row r="76" spans="2:18" thickTop="1" x14ac:dyDescent="0.25">
@@ -11423,20 +11426,20 @@
       <c r="E76" s="130"/>
       <c r="F76" s="34"/>
       <c r="M76" s="1"/>
-      <c r="P76" s="325">
+      <c r="P76" s="328">
         <f>SUM(P75+P74+P72)</f>
         <v>-53663.11</v>
       </c>
-      <c r="Q76" s="326"/>
-      <c r="R76" s="329"/>
+      <c r="Q76" s="329"/>
+      <c r="R76" s="332"/>
     </row>
     <row r="77" spans="2:18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D77" s="128"/>
       <c r="E77" s="130"/>
       <c r="F77" s="34"/>
-      <c r="P77" s="327"/>
-      <c r="Q77" s="328"/>
-      <c r="R77" s="330"/>
+      <c r="P77" s="330"/>
+      <c r="Q77" s="331"/>
+      <c r="R77" s="333"/>
     </row>
     <row r="78" spans="2:18" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D78" s="128"/>
@@ -11455,13 +11458,12 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="P76:Q77"/>
-    <mergeCell ref="R76:R77"/>
-    <mergeCell ref="P68:P69"/>
-    <mergeCell ref="P70:Q70"/>
-    <mergeCell ref="P72:Q73"/>
-    <mergeCell ref="P74:Q74"/>
-    <mergeCell ref="P75:Q75"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="I58:J58"/>
     <mergeCell ref="K58:L58"/>
@@ -11477,12 +11479,13 @@
     <mergeCell ref="K54:L54"/>
     <mergeCell ref="K56:L56"/>
     <mergeCell ref="P54:Q54"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="P76:Q77"/>
+    <mergeCell ref="R76:R77"/>
+    <mergeCell ref="P68:P69"/>
+    <mergeCell ref="P70:Q70"/>
+    <mergeCell ref="P72:Q73"/>
+    <mergeCell ref="P74:Q74"/>
+    <mergeCell ref="P75:Q75"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -11498,7 +11501,7 @@
   </sheetPr>
   <dimension ref="A1:N134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
@@ -12421,13 +12424,13 @@
       <c r="A35" s="267" t="s">
         <v>180</v>
       </c>
-      <c r="B35" s="346" t="s">
+      <c r="B35" s="287" t="s">
         <v>181</v>
       </c>
-      <c r="C35" s="347">
+      <c r="C35" s="288">
         <v>9701.98</v>
       </c>
-      <c r="D35" s="348"/>
+      <c r="D35" s="289"/>
       <c r="E35" s="69"/>
       <c r="F35" s="137">
         <f t="shared" si="0"/>
@@ -14169,12 +14172,12 @@
     <row r="42" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="43" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="155"/>
-      <c r="B43" s="343" t="s">
+      <c r="B43" s="347" t="s">
         <v>25</v>
       </c>
-      <c r="C43" s="344"/>
-      <c r="D43" s="344"/>
-      <c r="E43" s="345"/>
+      <c r="C43" s="348"/>
+      <c r="D43" s="348"/>
+      <c r="E43" s="349"/>
       <c r="F43" s="1"/>
     </row>
     <row r="44" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>